<commit_message>
Update LDI data 11/30/22
</commit_message>
<xml_diff>
--- a/data/index_data.xlsx
+++ b/data/index_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maddi\Documents\UPS_MV\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RRQ1FYQ\Documents\UPS_MV\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8D4A0A-2977-4886-9FE7-3C4B0D444E70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{496E9707-9DB4-4F91-9EC0-BB3E616D6FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3630" yWindow="920" windowWidth="15670" windowHeight="10170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="615" windowWidth="19200" windowHeight="7230" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bbg" sheetId="1" r:id="rId1"/>
@@ -33,8 +33,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -204,99 +202,147 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|15391177109235035820</stp>
-        <tr r="H7" s="1"/>
+        <stp>BDH|13143508141758957083</stp>
+        <tr r="V7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|14309177196172688359</stp>
-        <tr r="R7" s="1"/>
+        <stp>BDH|12976415469799243355</stp>
+        <tr r="T7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|16841319149829204575</stp>
+        <stp>BDH|12846913110700018020</stp>
+        <tr r="N7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|10605591940029431696</stp>
         <tr r="A7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|16559791485255285162</stp>
-        <tr r="K7" s="1"/>
+        <stp>BDH|13864980239984823277</stp>
+        <tr r="S7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|16010634124229847813</stp>
-        <tr r="U7" s="1"/>
+        <stp>BDH|12483361804497120478</stp>
+        <tr r="X7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|16466284545796995026</stp>
-        <tr r="F7" s="1"/>
+        <stp>BDH|17110321863039016946</stp>
+        <tr r="M7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|15018518179361754759</stp>
+        <tr r="L7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|12209347536670989485</stp>
+        <tr r="G7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|13669283076037410617</stp>
+        <tr r="I7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|13794444742221657585</stp>
+        <tr r="D7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|15611286639032243202</stp>
+        <tr r="E7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|15881097696519860133</stp>
+        <tr r="C7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|14484735279352247394</stp>
+        <tr r="U7" s="1"/>
       </tp>
     </main>
     <main first="bloomberg.rtd">
-      <tp t="s">
-        <v>Last Price</v>
+      <tp t="e">
+        <v>#N/A</v>
         <stp/>
         <stp>##V3_BFIELDINFOV12</stp>
         <stp>[index_data.xlsx]bbg!R5C9</stp>
         <stp>PX_LAST</stp>
         <tr r="I5" s="1"/>
       </tp>
-      <tp t="s">
-        <v>Last Price</v>
+      <tp t="e">
+        <v>#N/A</v>
         <stp/>
         <stp>##V3_BFIELDINFOV12</stp>
         <stp>[index_data.xlsx]bbg!R5C8</stp>
         <stp>PX_LAST</stp>
         <tr r="H5" s="1"/>
       </tp>
-      <tp t="s">
-        <v>Last Price</v>
+      <tp t="e">
+        <v>#N/A</v>
         <stp/>
         <stp>##V3_BFIELDINFOV12</stp>
         <stp>[index_data.xlsx]bbg!R5C7</stp>
         <stp>PX_LAST</stp>
         <tr r="G5" s="1"/>
       </tp>
-      <tp t="s">
-        <v>Last Price</v>
+      <tp t="e">
+        <v>#N/A</v>
         <stp/>
         <stp>##V3_BFIELDINFOV12</stp>
         <stp>[index_data.xlsx]bbg!R5C6</stp>
         <stp>PX_LAST</stp>
         <tr r="F5" s="1"/>
       </tp>
-      <tp t="s">
-        <v>Last Price</v>
+      <tp t="e">
+        <v>#N/A</v>
         <stp/>
         <stp>##V3_BFIELDINFOV12</stp>
         <stp>[index_data.xlsx]bbg!R5C5</stp>
         <stp>PX_LAST</stp>
         <tr r="E5" s="1"/>
       </tp>
-      <tp t="s">
-        <v>Last Price</v>
+      <tp t="e">
+        <v>#N/A</v>
         <stp/>
         <stp>##V3_BFIELDINFOV12</stp>
         <stp>[index_data.xlsx]bbg!R5C4</stp>
         <stp>PX_LAST</stp>
         <tr r="D5" s="1"/>
       </tp>
-      <tp t="s">
-        <v>Last Price</v>
+      <tp t="e">
+        <v>#N/A</v>
         <stp/>
         <stp>##V3_BFIELDINFOV12</stp>
         <stp>[index_data.xlsx]bbg!R5C3</stp>
         <stp>PX_LAST</stp>
         <tr r="C5" s="1"/>
       </tp>
-      <tp t="s">
-        <v>Last Price</v>
+      <tp t="e">
+        <v>#N/A</v>
         <stp/>
         <stp>##V3_BFIELDINFOV12</stp>
         <stp>[index_data.xlsx]bbg!R5C2</stp>
@@ -308,20 +354,8 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|1876933372882949014</stp>
+        <stp>BDH|8505007945428267990</stp>
         <tr r="W7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|6678966189993658993</stp>
-        <tr r="I7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|5914862928754717559</stp>
-        <tr r="C7" s="1"/>
       </tp>
     </main>
     <main first="bloomberg.rtd">
@@ -365,56 +399,56 @@
         <stp>PX_LAST</stp>
         <tr r="X5" s="1"/>
       </tp>
-      <tp t="s">
-        <v>Last Price</v>
+      <tp t="e">
+        <v>#N/A</v>
         <stp/>
         <stp>##V3_BFIELDINFOV12</stp>
         <stp>[index_data.xlsx]bbg!R5C10</stp>
         <stp>PX_LAST</stp>
         <tr r="J5" s="1"/>
       </tp>
-      <tp t="s">
-        <v>Last Price</v>
+      <tp t="e">
+        <v>#N/A</v>
         <stp/>
         <stp>##V3_BFIELDINFOV12</stp>
         <stp>[index_data.xlsx]bbg!R5C11</stp>
         <stp>PX_LAST</stp>
         <tr r="K5" s="1"/>
       </tp>
-      <tp t="s">
-        <v>Last Price</v>
+      <tp t="e">
+        <v>#N/A</v>
         <stp/>
         <stp>##V3_BFIELDINFOV12</stp>
         <stp>[index_data.xlsx]bbg!R5C12</stp>
         <stp>PX_LAST</stp>
         <tr r="L5" s="1"/>
       </tp>
-      <tp t="s">
-        <v>Last Price</v>
+      <tp t="e">
+        <v>#N/A</v>
         <stp/>
         <stp>##V3_BFIELDINFOV12</stp>
         <stp>[index_data.xlsx]bbg!R5C13</stp>
         <stp>PX_LAST</stp>
         <tr r="M5" s="1"/>
       </tp>
-      <tp t="s">
-        <v>Last Price</v>
+      <tp t="e">
+        <v>#N/A</v>
         <stp/>
         <stp>##V3_BFIELDINFOV12</stp>
         <stp>[index_data.xlsx]bbg!R5C14</stp>
         <stp>PX_LAST</stp>
         <tr r="N5" s="1"/>
       </tp>
-      <tp t="s">
-        <v>Last Price</v>
+      <tp t="e">
+        <v>#N/A</v>
         <stp/>
         <stp>##V3_BFIELDINFOV12</stp>
         <stp>[index_data.xlsx]bbg!R5C15</stp>
         <stp>PX_LAST</stp>
         <tr r="O5" s="1"/>
       </tp>
-      <tp t="s">
-        <v>Last Price</v>
+      <tp t="e">
+        <v>#N/A</v>
         <stp/>
         <stp>##V3_BFIELDINFOV12</stp>
         <stp>[index_data.xlsx]bbg!R5C16</stp>
@@ -450,90 +484,50 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|9477214532556026147</stp>
-        <tr r="L7" s="1"/>
+        <stp>BDH|43685579364898016</stp>
+        <tr r="H7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|36292386659241103</stp>
-        <tr r="V7" s="1"/>
+        <stp>BDH|6182457108729376244</stp>
+        <tr r="O7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|9896719964680467082</stp>
-        <tr r="P7" s="1"/>
+        <stp>BDH|9500202451907111299</stp>
+        <tr r="K7" s="1"/>
       </tp>
-    </main>
-    <main first="bofaddin.rtdserver">
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|8623315304807624694</stp>
+        <stp>BDH|4000643446125238843</stp>
+        <tr r="R7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|4898401300431124594</stp>
+        <tr r="J7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|7399313637984075741</stp>
         <tr r="Q7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|1008198799575830707</stp>
-        <tr r="O7" s="1"/>
+        <stp>BDH|1585218511057172461</stp>
+        <tr r="P7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|7035392656159871322</stp>
-        <tr r="E7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|9722384114934577972</stp>
-        <tr r="D7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|3584399528085967195</stp>
-        <tr r="X7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|6737116125103358117</stp>
-        <tr r="M7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|6311698408087231725</stp>
-        <tr r="G7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|6295339182207942854</stp>
-        <tr r="N7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|7767777114126087591</stp>
-        <tr r="T7" s="1"/>
-      </tp>
-    </main>
-    <main first="bofaddin.rtdserver">
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|159754737960912633</stp>
-        <tr r="J7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|207830744321886275</stp>
-        <tr r="S7" s="1"/>
+        <stp>BDH|7717146989234872807</stp>
+        <tr r="F7" s="1"/>
       </tp>
     </main>
   </volType>
@@ -837,15 +831,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X185"/>
+  <dimension ref="A1:X186"/>
   <sheetViews>
-    <sheetView topLeftCell="C161" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A185" sqref="A185:X185"/>
+    <sheetView topLeftCell="A138" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A186" sqref="A186:X186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
@@ -874,7 +868,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>44865</v>
+        <v>44895</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
@@ -1118,98 +1112,98 @@
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <f>_xll.BDH(B$4,B$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=S","cols=2;rows=179")</f>
+        <f>_xll.BDH(B$4,B$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=S","cols=2;rows=180")</f>
         <v>39447</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
       </c>
       <c r="C7">
-        <f>_xll.BDH(C$4,C$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=179")</f>
+        <f>_xll.BDH(C$4,C$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
         <v>1902.17</v>
       </c>
       <c r="D7" t="str">
-        <f>_xll.BDH(D$4,D$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=179")</f>
+        <f>_xll.BDH(D$4,D$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
         <v>#N/A N/A</v>
       </c>
       <c r="E7">
-        <f>_xll.BDH(E$4,E$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=179")</f>
+        <f>_xll.BDH(E$4,E$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
         <v>1468.36</v>
       </c>
       <c r="F7">
-        <f>_xll.BDH(F$4,F$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=179")</f>
+        <f>_xll.BDH(F$4,F$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
         <v>403.25</v>
       </c>
       <c r="G7">
-        <f>_xll.BDH(G$4,G$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=179")</f>
+        <f>_xll.BDH(G$4,G$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
         <v>766.03700000000003</v>
       </c>
       <c r="H7">
-        <f>_xll.BDH(H$4,H$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=179")</f>
+        <f>_xll.BDH(H$4,H$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
         <v>2253.36</v>
       </c>
       <c r="I7">
-        <f>_xll.BDH(I$4,I$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=179")</f>
+        <f>_xll.BDH(I$4,I$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
         <v>1245.5899999999999</v>
       </c>
       <c r="J7">
-        <f>_xll.BDH(J$4,J$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=179")</f>
+        <f>_xll.BDH(J$4,J$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
         <v>270.02620000000002</v>
       </c>
       <c r="K7">
-        <f>_xll.BDH(K$4,K$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=179")</f>
+        <f>_xll.BDH(K$4,K$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
         <v>590.78</v>
       </c>
       <c r="L7">
-        <f>_xll.BDH(L$4,L$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=179")</f>
+        <f>_xll.BDH(L$4,L$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
         <v>1294.82</v>
       </c>
       <c r="M7">
-        <f>_xll.BDH(M$4,M$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=179")</f>
+        <f>_xll.BDH(M$4,M$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
         <v>12335.221</v>
       </c>
       <c r="N7">
-        <f>_xll.BDH(N$4,N$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=179")</f>
+        <f>_xll.BDH(N$4,N$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
         <v>1915.1320000000001</v>
       </c>
       <c r="O7">
-        <f>_xll.BDH(O$4,O$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=179")</f>
+        <f>_xll.BDH(O$4,O$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
         <v>1389.21</v>
       </c>
       <c r="P7">
-        <f>_xll.BDH(P$4,P$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=179")</f>
+        <f>_xll.BDH(P$4,P$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
         <v>255.67</v>
       </c>
       <c r="Q7">
-        <f>_xll.BDH(Q$4,Q$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=179")</f>
+        <f>_xll.BDH(Q$4,Q$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
         <v>141.76349999999999</v>
       </c>
       <c r="R7">
-        <f>_xll.BDH(R$4,R$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=179")</f>
+        <f>_xll.BDH(R$4,R$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
         <v>3.1589900000000002</v>
       </c>
       <c r="S7">
-        <f>_xll.BDH(S$4,S$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=179")</f>
+        <f>_xll.BDH(S$4,S$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
         <v>3.33792826</v>
       </c>
       <c r="T7">
-        <f>_xll.BDH(T$4,T$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=179")</f>
+        <f>_xll.BDH(T$4,T$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
         <v>1412.28</v>
       </c>
       <c r="U7">
-        <f>_xll.BDH(U$4,U$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=179")</f>
+        <f>_xll.BDH(U$4,U$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
         <v>996.96</v>
       </c>
       <c r="V7">
-        <f>_xll.BDH(V$4,V$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=179")</f>
+        <f>_xll.BDH(V$4,V$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
         <v>849.221</v>
       </c>
       <c r="W7" t="str">
-        <f>_xll.BDH(W$4,W$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=179")</f>
+        <f>_xll.BDH(W$4,W$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
         <v>#N/A N/A</v>
       </c>
       <c r="X7">
-        <f>_xll.BDH(X$4,X$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=179")</f>
+        <f>_xll.BDH(X$4,X$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
         <v>221.59</v>
       </c>
     </row>
@@ -14296,7 +14290,7 @@
         <v>3.2972545599999998</v>
       </c>
       <c r="T184">
-        <v>4887.8999999999996</v>
+        <v>4976.87</v>
       </c>
       <c r="U184">
         <v>1403.68</v>
@@ -14349,7 +14343,7 @@
         <v>1297.27</v>
       </c>
       <c r="M185">
-        <v>19349.467000000001</v>
+        <v>19286.981</v>
       </c>
       <c r="N185">
         <v>4128.7719999999999</v>
@@ -14370,7 +14364,7 @@
         <v>4.11230765</v>
       </c>
       <c r="T185">
-        <v>4887.8999999999996</v>
+        <v>4976.87</v>
       </c>
       <c r="U185">
         <v>1489.05</v>
@@ -14383,6 +14377,80 @@
       </c>
       <c r="X185">
         <v>350.53</v>
+      </c>
+    </row>
+    <row r="186" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A186" s="1">
+        <v>44895</v>
+      </c>
+      <c r="B186">
+        <v>136.32</v>
+      </c>
+      <c r="C186">
+        <v>3938.05</v>
+      </c>
+      <c r="D186">
+        <v>171.22319999999999</v>
+      </c>
+      <c r="E186">
+        <v>4080.11</v>
+      </c>
+      <c r="F186">
+        <v>630.91999999999996</v>
+      </c>
+      <c r="G186">
+        <v>1886.577</v>
+      </c>
+      <c r="H186">
+        <v>1944.03</v>
+      </c>
+      <c r="I186">
+        <v>972.29</v>
+      </c>
+      <c r="J186">
+        <v>493.30450000000002</v>
+      </c>
+      <c r="K186">
+        <v>1412.32</v>
+      </c>
+      <c r="L186">
+        <v>1266.26</v>
+      </c>
+      <c r="M186">
+        <v>18959.576000000001</v>
+      </c>
+      <c r="N186">
+        <v>3879.6979999999999</v>
+      </c>
+      <c r="O186">
+        <v>1718.69</v>
+      </c>
+      <c r="P186">
+        <v>392.34</v>
+      </c>
+      <c r="Q186">
+        <v>162.4709</v>
+      </c>
+      <c r="R186">
+        <v>4.1383099999999997</v>
+      </c>
+      <c r="S186">
+        <v>4.3319210000000004</v>
+      </c>
+      <c r="T186">
+        <v>4976.87</v>
+      </c>
+      <c r="U186">
+        <v>1600.06</v>
+      </c>
+      <c r="V186">
+        <v>2358.4470000000001</v>
+      </c>
+      <c r="W186">
+        <v>135.875</v>
+      </c>
+      <c r="X186">
+        <v>371.08</v>
       </c>
     </row>
   </sheetData>
@@ -14392,10 +14460,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:X180"/>
+  <dimension ref="A1:X181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A181" sqref="A181:X181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27734,6 +27802,80 @@
       </c>
       <c r="X180">
         <v>350.53</v>
+      </c>
+    </row>
+    <row r="181" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A181" s="1">
+        <v>44895</v>
+      </c>
+      <c r="B181">
+        <v>136.32</v>
+      </c>
+      <c r="C181">
+        <v>3938.05</v>
+      </c>
+      <c r="D181">
+        <v>171.22319999999999</v>
+      </c>
+      <c r="E181">
+        <v>4080.11</v>
+      </c>
+      <c r="F181">
+        <v>630.91999999999996</v>
+      </c>
+      <c r="G181">
+        <v>1886.577</v>
+      </c>
+      <c r="H181">
+        <v>1944.03</v>
+      </c>
+      <c r="I181">
+        <v>972.29</v>
+      </c>
+      <c r="J181">
+        <v>493.30450000000002</v>
+      </c>
+      <c r="K181">
+        <v>1412.32</v>
+      </c>
+      <c r="L181">
+        <v>1266.26</v>
+      </c>
+      <c r="M181">
+        <v>18959.576000000001</v>
+      </c>
+      <c r="N181">
+        <v>3879.6979999999999</v>
+      </c>
+      <c r="O181">
+        <v>1718.69</v>
+      </c>
+      <c r="P181">
+        <v>392.34</v>
+      </c>
+      <c r="Q181">
+        <v>162.4709</v>
+      </c>
+      <c r="R181">
+        <v>4.1383099999999997</v>
+      </c>
+      <c r="S181">
+        <v>4.3319210000000004</v>
+      </c>
+      <c r="T181">
+        <v>4976.87</v>
+      </c>
+      <c r="U181">
+        <v>1600.06</v>
+      </c>
+      <c r="V181">
+        <v>2358.4470000000001</v>
+      </c>
+      <c r="W181">
+        <v>135.875</v>
+      </c>
+      <c r="X181">
+        <v>371.08</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update index data 12/31/2022
</commit_message>
<xml_diff>
--- a/data/index_data.xlsx
+++ b/data/index_data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RRQ1FYQ\Documents\UPS_MV\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bloomberg\Documents\GitHub\UPS_MV\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{496E9707-9DB4-4F91-9EC0-BB3E616D6FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="615" windowWidth="19200" windowHeight="7230" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="615" windowWidth="19200" windowHeight="7230" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="bbg" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
     <definedName name="SpreadsheetBuilder_1" localSheetId="1" hidden="1">data!$A$1:$P$3</definedName>
     <definedName name="SpreadsheetBuilder_8" hidden="1">bbg!$A$1:$P$7</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="29">
   <si>
     <t>Start Date</t>
   </si>
@@ -125,11 +124,15 @@
   <si>
     <t>SPUSTBTR Index</t>
   </si>
+  <si>
+    <t>12/31
+/2022</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000%"/>
   </numFmts>
@@ -170,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -178,6 +181,9 @@
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -202,86 +208,74 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|13143508141758957083</stp>
+        <stp>BDH|16260322941572045888</stp>
+        <tr r="S7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|15186403787347702677</stp>
+        <tr r="D7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|17715390876150307109</stp>
+        <tr r="G7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|14406751109895676413</stp>
+        <tr r="R7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|17616552325801162125</stp>
+        <tr r="T7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|10209224655710149712</stp>
+        <tr r="U7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|17591541156537809071</stp>
+        <tr r="P7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|14289313393759269664</stp>
+        <tr r="I7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|10354867160237036826</stp>
         <tr r="V7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|12976415469799243355</stp>
-        <tr r="T7" s="1"/>
+        <stp>BDH|17339952999957269647</stp>
+        <tr r="W7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|12846913110700018020</stp>
-        <tr r="N7" s="1"/>
+        <stp>BDH|12836079640644446547</stp>
+        <tr r="Q7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|10605591940029431696</stp>
-        <tr r="A7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|13864980239984823277</stp>
-        <tr r="S7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|12483361804497120478</stp>
-        <tr r="X7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|17110321863039016946</stp>
-        <tr r="M7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|15018518179361754759</stp>
-        <tr r="L7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|12209347536670989485</stp>
-        <tr r="G7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|13669283076037410617</stp>
-        <tr r="I7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|13794444742221657585</stp>
-        <tr r="D7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|15611286639032243202</stp>
-        <tr r="E7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|15881097696519860133</stp>
+        <stp>BDH|13340564228128127892</stp>
         <tr r="C7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|14484735279352247394</stp>
-        <tr r="U7" s="1"/>
       </tp>
     </main>
     <main first="bloomberg.rtd">
@@ -354,8 +348,8 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|8505007945428267990</stp>
-        <tr r="W7" s="1"/>
+        <stp>BDH|2583946357844558468</stp>
+        <tr r="F7" s="1"/>
       </tp>
     </main>
     <main first="bloomberg.rtd">
@@ -484,50 +478,62 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|43685579364898016</stp>
+        <stp>BDH|8715571147982884261</stp>
+        <tr r="A7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|5337857811456651135</stp>
+        <tr r="M7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|1937304033633197694</stp>
         <tr r="H7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|6182457108729376244</stp>
+        <stp>BDH|5148256585428118167</stp>
+        <tr r="L7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|1536785358873787645</stp>
+        <tr r="N7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|2449917877528190397</stp>
+        <tr r="X7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|1570140149985888625</stp>
+        <tr r="E7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|3329653219596187212</stp>
         <tr r="O7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|9500202451907111299</stp>
-        <tr r="K7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|4000643446125238843</stp>
-        <tr r="R7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|4898401300431124594</stp>
+        <stp>BDH|9930674116049078781</stp>
         <tr r="J7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|7399313637984075741</stp>
-        <tr r="Q7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|1585218511057172461</stp>
-        <tr r="P7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|7717146989234872807</stp>
-        <tr r="F7" s="1"/>
+        <stp>BDH|2079352188799857328</stp>
+        <tr r="K7" s="1"/>
       </tp>
     </main>
   </volType>
@@ -830,17 +836,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X186"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X187"/>
   <sheetViews>
-    <sheetView topLeftCell="A138" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A186" sqref="A186:X186"/>
+    <sheetView topLeftCell="A133" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A187" sqref="A187:X187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
@@ -863,12 +869,12 @@
         <v>39447</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
-        <v>44895</v>
+      <c r="B2" s="7" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
@@ -1112,98 +1118,98 @@
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <f>_xll.BDH(B$4,B$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=S","cols=2;rows=180")</f>
+        <f>_xll.BDH(B$4,B$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=S","cols=2;rows=181")</f>
         <v>39447</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
       </c>
       <c r="C7">
-        <f>_xll.BDH(C$4,C$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
+        <f>_xll.BDH(C$4,C$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
         <v>1902.17</v>
       </c>
       <c r="D7" t="str">
-        <f>_xll.BDH(D$4,D$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
+        <f>_xll.BDH(D$4,D$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
         <v>#N/A N/A</v>
       </c>
       <c r="E7">
-        <f>_xll.BDH(E$4,E$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
+        <f>_xll.BDH(E$4,E$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
         <v>1468.36</v>
       </c>
       <c r="F7">
-        <f>_xll.BDH(F$4,F$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
+        <f>_xll.BDH(F$4,F$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
         <v>403.25</v>
       </c>
       <c r="G7">
-        <f>_xll.BDH(G$4,G$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
+        <f>_xll.BDH(G$4,G$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
         <v>766.03700000000003</v>
       </c>
       <c r="H7">
-        <f>_xll.BDH(H$4,H$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
+        <f>_xll.BDH(H$4,H$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
         <v>2253.36</v>
       </c>
       <c r="I7">
-        <f>_xll.BDH(I$4,I$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
+        <f>_xll.BDH(I$4,I$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
         <v>1245.5899999999999</v>
       </c>
       <c r="J7">
-        <f>_xll.BDH(J$4,J$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
+        <f>_xll.BDH(J$4,J$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
         <v>270.02620000000002</v>
       </c>
       <c r="K7">
-        <f>_xll.BDH(K$4,K$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
+        <f>_xll.BDH(K$4,K$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
         <v>590.78</v>
       </c>
       <c r="L7">
-        <f>_xll.BDH(L$4,L$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
+        <f>_xll.BDH(L$4,L$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
         <v>1294.82</v>
       </c>
       <c r="M7">
-        <f>_xll.BDH(M$4,M$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
+        <f>_xll.BDH(M$4,M$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
         <v>12335.221</v>
       </c>
       <c r="N7">
-        <f>_xll.BDH(N$4,N$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
+        <f>_xll.BDH(N$4,N$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
         <v>1915.1320000000001</v>
       </c>
       <c r="O7">
-        <f>_xll.BDH(O$4,O$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
+        <f>_xll.BDH(O$4,O$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
         <v>1389.21</v>
       </c>
       <c r="P7">
-        <f>_xll.BDH(P$4,P$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
+        <f>_xll.BDH(P$4,P$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
         <v>255.67</v>
       </c>
       <c r="Q7">
-        <f>_xll.BDH(Q$4,Q$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
+        <f>_xll.BDH(Q$4,Q$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
         <v>141.76349999999999</v>
       </c>
       <c r="R7">
-        <f>_xll.BDH(R$4,R$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
+        <f>_xll.BDH(R$4,R$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
         <v>3.1589900000000002</v>
       </c>
       <c r="S7">
-        <f>_xll.BDH(S$4,S$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
+        <f>_xll.BDH(S$4,S$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
         <v>3.33792826</v>
       </c>
       <c r="T7">
-        <f>_xll.BDH(T$4,T$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
+        <f>_xll.BDH(T$4,T$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
         <v>1412.28</v>
       </c>
       <c r="U7">
-        <f>_xll.BDH(U$4,U$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
+        <f>_xll.BDH(U$4,U$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
         <v>996.96</v>
       </c>
       <c r="V7">
-        <f>_xll.BDH(V$4,V$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
+        <f>_xll.BDH(V$4,V$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
         <v>849.221</v>
       </c>
       <c r="W7" t="str">
-        <f>_xll.BDH(W$4,W$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
+        <f>_xll.BDH(W$4,W$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
         <v>#N/A N/A</v>
       </c>
       <c r="X7">
-        <f>_xll.BDH(X$4,X$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=180")</f>
+        <f>_xll.BDH(X$4,X$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
         <v>221.59</v>
       </c>
     </row>
@@ -14417,7 +14423,7 @@
         <v>1266.26</v>
       </c>
       <c r="M186">
-        <v>18959.576000000001</v>
+        <v>18880.728999999999</v>
       </c>
       <c r="N186">
         <v>3879.6979999999999</v>
@@ -14451,6 +14457,80 @@
       </c>
       <c r="X186">
         <v>371.08</v>
+      </c>
+    </row>
+    <row r="187" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A187" s="1">
+        <v>44925</v>
+      </c>
+      <c r="B187">
+        <v>133.24</v>
+      </c>
+      <c r="C187">
+        <v>3892.91</v>
+      </c>
+      <c r="D187">
+        <v>168.74969999999999</v>
+      </c>
+      <c r="E187">
+        <v>3839.5</v>
+      </c>
+      <c r="F187">
+        <v>605.38</v>
+      </c>
+      <c r="G187">
+        <v>1761.2460000000001</v>
+      </c>
+      <c r="H187">
+        <v>1943.93</v>
+      </c>
+      <c r="I187">
+        <v>956.38</v>
+      </c>
+      <c r="J187">
+        <v>495.06270000000001</v>
+      </c>
+      <c r="K187">
+        <v>1401.68</v>
+      </c>
+      <c r="L187">
+        <v>1266.8900000000001</v>
+      </c>
+      <c r="M187">
+        <v>18968.453000000001</v>
+      </c>
+      <c r="N187">
+        <v>3870.6570000000002</v>
+      </c>
+      <c r="O187">
+        <v>1718.69</v>
+      </c>
+      <c r="P187">
+        <v>370.27</v>
+      </c>
+      <c r="Q187">
+        <v>162.4709</v>
+      </c>
+      <c r="R187">
+        <v>4.3072400000000002</v>
+      </c>
+      <c r="S187">
+        <v>4.3983636739999996</v>
+      </c>
+      <c r="T187">
+        <v>4976.87</v>
+      </c>
+      <c r="U187">
+        <v>1536.73</v>
+      </c>
+      <c r="V187">
+        <v>2217.145</v>
+      </c>
+      <c r="W187">
+        <v>134.3125</v>
+      </c>
+      <c r="X187">
+        <v>367.56</v>
       </c>
     </row>
   </sheetData>
@@ -14459,11 +14539,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:X181"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X182"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A181" sqref="A181:X181"/>
+    <sheetView tabSelected="1" topLeftCell="A153" workbookViewId="0">
+      <selection activeCell="A182" sqref="A182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27878,13 +27958,87 @@
         <v>371.08</v>
       </c>
     </row>
+    <row r="182" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A182" s="1">
+        <v>44925</v>
+      </c>
+      <c r="B182">
+        <v>133.24</v>
+      </c>
+      <c r="C182">
+        <v>3892.91</v>
+      </c>
+      <c r="D182">
+        <v>168.74969999999999</v>
+      </c>
+      <c r="E182">
+        <v>3839.5</v>
+      </c>
+      <c r="F182">
+        <v>605.38</v>
+      </c>
+      <c r="G182">
+        <v>1761.2460000000001</v>
+      </c>
+      <c r="H182">
+        <v>1943.93</v>
+      </c>
+      <c r="I182">
+        <v>956.38</v>
+      </c>
+      <c r="J182">
+        <v>495.06270000000001</v>
+      </c>
+      <c r="K182">
+        <v>1401.68</v>
+      </c>
+      <c r="L182">
+        <v>1266.8900000000001</v>
+      </c>
+      <c r="M182">
+        <v>18968.453000000001</v>
+      </c>
+      <c r="N182">
+        <v>3870.6570000000002</v>
+      </c>
+      <c r="O182">
+        <v>1718.69</v>
+      </c>
+      <c r="P182">
+        <v>370.27</v>
+      </c>
+      <c r="Q182">
+        <v>162.4709</v>
+      </c>
+      <c r="R182">
+        <v>4.3072400000000002</v>
+      </c>
+      <c r="S182">
+        <v>4.3983636739999996</v>
+      </c>
+      <c r="T182">
+        <v>4976.87</v>
+      </c>
+      <c r="U182">
+        <v>1536.73</v>
+      </c>
+      <c r="V182">
+        <v>2217.145</v>
+      </c>
+      <c r="W182">
+        <v>134.3125</v>
+      </c>
+      <c r="X182">
+        <v>367.56</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X179"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Update ldi data 2/2023
</commit_message>
<xml_diff>
--- a/data/index_data.xlsx
+++ b/data/index_data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bloomberg\Documents\GitHub\UPS_MV\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RRQ1FYQ\Documents\UPS_MV\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4291288E-3FAE-450C-9D1A-4E136433DE6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="615" windowWidth="19200" windowHeight="7230" activeTab="1"/>
+    <workbookView xWindow="450" yWindow="1800" windowWidth="21600" windowHeight="11325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bbg" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
     <definedName name="SpreadsheetBuilder_1" localSheetId="1" hidden="1">data!$A$1:$P$3</definedName>
     <definedName name="SpreadsheetBuilder_8" hidden="1">bbg!$A$1:$P$7</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,6 +33,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="28">
   <si>
     <t>Start Date</t>
   </si>
@@ -124,15 +127,11 @@
   <si>
     <t>SPUSTBTR Index</t>
   </si>
-  <si>
-    <t>12/31
-/2022</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000%"/>
   </numFmts>
@@ -208,74 +207,50 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|16260322941572045888</stp>
-        <tr r="S7" s="1"/>
+        <stp>BDH|18237526495139166654</stp>
+        <tr r="N7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|15186403787347702677</stp>
+        <stp>BDH|11716787340289124001</stp>
+        <tr r="A7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|17984493393030080389</stp>
+        <tr r="E7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|14269559167394485133</stp>
+        <tr r="H7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|13254190218125375505</stp>
         <tr r="D7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|17715390876150307109</stp>
+        <stp>BDH|10613056508164008773</stp>
+        <tr r="I7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|12542054832835615290</stp>
         <tr r="G7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|14406751109895676413</stp>
-        <tr r="R7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|17616552325801162125</stp>
-        <tr r="T7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|10209224655710149712</stp>
-        <tr r="U7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|17591541156537809071</stp>
-        <tr r="P7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|14289313393759269664</stp>
-        <tr r="I7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|10354867160237036826</stp>
-        <tr r="V7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|17339952999957269647</stp>
-        <tr r="W7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|12836079640644446547</stp>
-        <tr r="Q7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|13340564228128127892</stp>
-        <tr r="C7" s="1"/>
+        <stp>BDH|17289885426543044979</stp>
+        <tr r="X7" s="1"/>
       </tp>
     </main>
     <main first="bloomberg.rtd">
@@ -348,8 +323,8 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|2583946357844558468</stp>
-        <tr r="F7" s="1"/>
+        <stp>BDH|4423416296506656375</stp>
+        <tr r="Q7" s="1"/>
       </tp>
     </main>
     <main first="bloomberg.rtd">
@@ -478,62 +453,86 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|8715571147982884261</stp>
-        <tr r="A7" s="1"/>
+        <stp>BDH|3732344933689158519</stp>
+        <tr r="K7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|5337857811456651135</stp>
+        <stp>BDH|4628544335325102838</stp>
+        <tr r="V7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|4883981393634241990</stp>
+        <tr r="L7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|3207824271537345139</stp>
+        <tr r="C7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|8319283653537681335</stp>
+        <tr r="R7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|1645143108382074725</stp>
+        <tr r="S7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|5355938979259842728</stp>
+        <tr r="J7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|1471632021310053023</stp>
+        <tr r="O7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|7951969993591120147</stp>
+        <tr r="F7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|2079819245496186834</stp>
+        <tr r="W7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|6680358376653754164</stp>
+        <tr r="P7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|3634296683179203156</stp>
+        <tr r="T7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|5923488071320113518</stp>
         <tr r="M7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|1937304033633197694</stp>
-        <tr r="H7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|5148256585428118167</stp>
-        <tr r="L7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|1536785358873787645</stp>
-        <tr r="N7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|2449917877528190397</stp>
-        <tr r="X7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|1570140149985888625</stp>
-        <tr r="E7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|3329653219596187212</stp>
-        <tr r="O7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|9930674116049078781</stp>
-        <tr r="J7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|2079352188799857328</stp>
-        <tr r="K7" s="1"/>
+        <stp>BDH|590095370470294085</stp>
+        <tr r="U7" s="1"/>
       </tp>
     </main>
   </volType>
@@ -836,11 +835,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X187"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:X189"/>
   <sheetViews>
-    <sheetView topLeftCell="A133" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A187" sqref="A187:X187"/>
+    <sheetView topLeftCell="A140" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A189" sqref="A187:X189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -869,12 +868,12 @@
         <v>39447</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>28</v>
+      <c r="B2" s="7">
+        <v>44985</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
@@ -949,65 +948,65 @@
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B5" t="str">
+      <c r="B5" t="e">
         <f>_xll.BFieldInfo(B$6)</f>
-        <v>Last Price</v>
-      </c>
-      <c r="C5" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="C5" t="e">
         <f>_xll.BFieldInfo(C$6)</f>
-        <v>Last Price</v>
-      </c>
-      <c r="D5" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="D5" t="e">
         <f>_xll.BFieldInfo(D$6)</f>
-        <v>Last Price</v>
-      </c>
-      <c r="E5" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="E5" t="e">
         <f>_xll.BFieldInfo(E$6)</f>
-        <v>Last Price</v>
-      </c>
-      <c r="F5" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="F5" t="e">
         <f>_xll.BFieldInfo(F$6)</f>
-        <v>Last Price</v>
-      </c>
-      <c r="G5" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="G5" t="e">
         <f>_xll.BFieldInfo(G$6)</f>
-        <v>Last Price</v>
-      </c>
-      <c r="H5" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="H5" t="e">
         <f>_xll.BFieldInfo(H$6)</f>
-        <v>Last Price</v>
-      </c>
-      <c r="I5" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="I5" t="e">
         <f>_xll.BFieldInfo(I$6)</f>
-        <v>Last Price</v>
-      </c>
-      <c r="J5" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="J5" t="e">
         <f>_xll.BFieldInfo(J$6)</f>
-        <v>Last Price</v>
-      </c>
-      <c r="K5" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="K5" t="e">
         <f>_xll.BFieldInfo(K$6)</f>
-        <v>Last Price</v>
-      </c>
-      <c r="L5" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="L5" t="e">
         <f>_xll.BFieldInfo(L$6)</f>
-        <v>Last Price</v>
-      </c>
-      <c r="M5" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="M5" t="e">
         <f>_xll.BFieldInfo(M$6)</f>
-        <v>Last Price</v>
-      </c>
-      <c r="N5" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="N5" t="e">
         <f>_xll.BFieldInfo(N$6)</f>
-        <v>Last Price</v>
-      </c>
-      <c r="O5" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="O5" t="e">
         <f>_xll.BFieldInfo(O$6)</f>
-        <v>Last Price</v>
-      </c>
-      <c r="P5" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="P5" t="e">
         <f>_xll.BFieldInfo(P$6)</f>
-        <v>Last Price</v>
+        <v>#N/A</v>
       </c>
       <c r="Q5" t="e">
         <f>_xll.BFieldInfo(Q$6)</f>
@@ -1118,98 +1117,98 @@
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <f>_xll.BDH(B$4,B$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=S","cols=2;rows=181")</f>
+        <f>_xll.BDH(B$4,B$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=S","cols=2;rows=183")</f>
         <v>39447</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
       </c>
       <c r="C7">
-        <f>_xll.BDH(C$4,C$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(C$4,C$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
         <v>1902.17</v>
       </c>
       <c r="D7" t="str">
-        <f>_xll.BDH(D$4,D$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(D$4,D$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
         <v>#N/A N/A</v>
       </c>
       <c r="E7">
-        <f>_xll.BDH(E$4,E$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(E$4,E$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
         <v>1468.36</v>
       </c>
       <c r="F7">
-        <f>_xll.BDH(F$4,F$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(F$4,F$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
         <v>403.25</v>
       </c>
       <c r="G7">
-        <f>_xll.BDH(G$4,G$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(G$4,G$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
         <v>766.03700000000003</v>
       </c>
       <c r="H7">
-        <f>_xll.BDH(H$4,H$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(H$4,H$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
         <v>2253.36</v>
       </c>
       <c r="I7">
-        <f>_xll.BDH(I$4,I$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(I$4,I$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
         <v>1245.5899999999999</v>
       </c>
       <c r="J7">
-        <f>_xll.BDH(J$4,J$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(J$4,J$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
         <v>270.02620000000002</v>
       </c>
       <c r="K7">
-        <f>_xll.BDH(K$4,K$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(K$4,K$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
         <v>590.78</v>
       </c>
       <c r="L7">
-        <f>_xll.BDH(L$4,L$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(L$4,L$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
         <v>1294.82</v>
       </c>
       <c r="M7">
-        <f>_xll.BDH(M$4,M$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(M$4,M$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
         <v>12335.221</v>
       </c>
       <c r="N7">
-        <f>_xll.BDH(N$4,N$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(N$4,N$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
         <v>1915.1320000000001</v>
       </c>
       <c r="O7">
-        <f>_xll.BDH(O$4,O$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(O$4,O$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
         <v>1389.21</v>
       </c>
       <c r="P7">
-        <f>_xll.BDH(P$4,P$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(P$4,P$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
         <v>255.67</v>
       </c>
       <c r="Q7">
-        <f>_xll.BDH(Q$4,Q$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(Q$4,Q$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
         <v>141.76349999999999</v>
       </c>
       <c r="R7">
-        <f>_xll.BDH(R$4,R$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(R$4,R$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
         <v>3.1589900000000002</v>
       </c>
       <c r="S7">
-        <f>_xll.BDH(S$4,S$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(S$4,S$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
         <v>3.33792826</v>
       </c>
       <c r="T7">
-        <f>_xll.BDH(T$4,T$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(T$4,T$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
         <v>1412.28</v>
       </c>
       <c r="U7">
-        <f>_xll.BDH(U$4,U$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(U$4,U$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
         <v>996.96</v>
       </c>
       <c r="V7">
-        <f>_xll.BDH(V$4,V$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(V$4,V$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
         <v>849.221</v>
       </c>
       <c r="W7" t="str">
-        <f>_xll.BDH(W$4,W$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(W$4,W$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
         <v>#N/A N/A</v>
       </c>
       <c r="X7">
-        <f>_xll.BDH(X$4,X$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(X$4,X$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
         <v>221.59</v>
       </c>
     </row>
@@ -14497,7 +14496,7 @@
         <v>1266.8900000000001</v>
       </c>
       <c r="M187">
-        <v>18968.453000000001</v>
+        <v>18910.451000000001</v>
       </c>
       <c r="N187">
         <v>3870.6570000000002</v>
@@ -14531,6 +14530,154 @@
       </c>
       <c r="X187">
         <v>367.56</v>
+      </c>
+    </row>
+    <row r="188" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A188" s="1">
+        <v>44957</v>
+      </c>
+      <c r="B188">
+        <v>145.46</v>
+      </c>
+      <c r="C188">
+        <v>4161.7</v>
+      </c>
+      <c r="D188">
+        <v>178.0941</v>
+      </c>
+      <c r="E188">
+        <v>4076.6</v>
+      </c>
+      <c r="F188">
+        <v>648.37</v>
+      </c>
+      <c r="G188">
+        <v>1931.9449999999999</v>
+      </c>
+      <c r="H188">
+        <v>2100.44</v>
+      </c>
+      <c r="I188">
+        <v>1031.5</v>
+      </c>
+      <c r="J188">
+        <v>507.7645</v>
+      </c>
+      <c r="K188">
+        <v>1456.48</v>
+      </c>
+      <c r="L188">
+        <v>1267.28</v>
+      </c>
+      <c r="M188">
+        <v>18975.955000000002</v>
+      </c>
+      <c r="N188">
+        <v>3817.4569999999999</v>
+      </c>
+      <c r="O188">
+        <v>1718.69</v>
+      </c>
+      <c r="P188">
+        <v>407.11</v>
+      </c>
+      <c r="Q188">
+        <v>162.4709</v>
+      </c>
+      <c r="R188">
+        <v>4.5090300000000001</v>
+      </c>
+      <c r="S188">
+        <v>4.6489987660000001</v>
+      </c>
+      <c r="T188">
+        <v>4976.87</v>
+      </c>
+      <c r="U188">
+        <v>1648.91</v>
+      </c>
+      <c r="V188">
+        <v>2367.614</v>
+      </c>
+      <c r="W188">
+        <v>141.75</v>
+      </c>
+      <c r="X188">
+        <v>382.39</v>
+      </c>
+    </row>
+    <row r="189" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A189" s="1">
+        <v>44985</v>
+      </c>
+      <c r="B189">
+        <v>136.36000000000001</v>
+      </c>
+      <c r="C189">
+        <v>3934.93</v>
+      </c>
+      <c r="D189">
+        <v>168.9444</v>
+      </c>
+      <c r="E189">
+        <v>3970.15</v>
+      </c>
+      <c r="F189">
+        <v>629.02</v>
+      </c>
+      <c r="G189">
+        <v>1896.991</v>
+      </c>
+      <c r="H189">
+        <v>2053.69</v>
+      </c>
+      <c r="I189">
+        <v>964.01</v>
+      </c>
+      <c r="J189">
+        <v>510.96210000000002</v>
+      </c>
+      <c r="K189">
+        <v>1437.64</v>
+      </c>
+      <c r="L189">
+        <v>1273.56</v>
+      </c>
+      <c r="M189">
+        <v>18991.472000000002</v>
+      </c>
+      <c r="N189">
+        <v>3888.33</v>
+      </c>
+      <c r="O189">
+        <v>1718.69</v>
+      </c>
+      <c r="P189">
+        <v>382.53</v>
+      </c>
+      <c r="Q189">
+        <v>162.4709</v>
+      </c>
+      <c r="R189">
+        <v>4.67272</v>
+      </c>
+      <c r="S189">
+        <v>4.8077261</v>
+      </c>
+      <c r="T189">
+        <v>4976.87</v>
+      </c>
+      <c r="U189">
+        <v>1601.19</v>
+      </c>
+      <c r="V189">
+        <v>2308.3960000000002</v>
+      </c>
+      <c r="W189">
+        <v>134.5625</v>
+      </c>
+      <c r="X189">
+        <v>366.54</v>
       </c>
     </row>
   </sheetData>
@@ -14539,11 +14686,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X182"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:X184"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A153" workbookViewId="0">
-      <selection activeCell="A182" sqref="A182"/>
+      <selection activeCell="C177" sqref="C177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27996,7 +28143,7 @@
         <v>1266.8900000000001</v>
       </c>
       <c r="M182">
-        <v>18968.453000000001</v>
+        <v>18910.451000000001</v>
       </c>
       <c r="N182">
         <v>3870.6570000000002</v>
@@ -28030,6 +28177,154 @@
       </c>
       <c r="X182">
         <v>367.56</v>
+      </c>
+    </row>
+    <row r="183" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A183" s="1">
+        <v>44957</v>
+      </c>
+      <c r="B183">
+        <v>145.46</v>
+      </c>
+      <c r="C183">
+        <v>4161.7</v>
+      </c>
+      <c r="D183">
+        <v>178.0941</v>
+      </c>
+      <c r="E183">
+        <v>4076.6</v>
+      </c>
+      <c r="F183">
+        <v>648.37</v>
+      </c>
+      <c r="G183">
+        <v>1931.9449999999999</v>
+      </c>
+      <c r="H183">
+        <v>2100.44</v>
+      </c>
+      <c r="I183">
+        <v>1031.5</v>
+      </c>
+      <c r="J183">
+        <v>507.7645</v>
+      </c>
+      <c r="K183">
+        <v>1456.48</v>
+      </c>
+      <c r="L183">
+        <v>1267.28</v>
+      </c>
+      <c r="M183">
+        <v>18975.955000000002</v>
+      </c>
+      <c r="N183">
+        <v>3817.4569999999999</v>
+      </c>
+      <c r="O183">
+        <v>1718.69</v>
+      </c>
+      <c r="P183">
+        <v>407.11</v>
+      </c>
+      <c r="Q183">
+        <v>162.4709</v>
+      </c>
+      <c r="R183">
+        <v>4.5090300000000001</v>
+      </c>
+      <c r="S183">
+        <v>4.6489987660000001</v>
+      </c>
+      <c r="T183">
+        <v>4976.87</v>
+      </c>
+      <c r="U183">
+        <v>1648.91</v>
+      </c>
+      <c r="V183">
+        <v>2367.614</v>
+      </c>
+      <c r="W183">
+        <v>141.75</v>
+      </c>
+      <c r="X183">
+        <v>382.39</v>
+      </c>
+    </row>
+    <row r="184" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A184" s="1">
+        <v>44985</v>
+      </c>
+      <c r="B184">
+        <v>136.36000000000001</v>
+      </c>
+      <c r="C184">
+        <v>3934.93</v>
+      </c>
+      <c r="D184">
+        <v>168.9444</v>
+      </c>
+      <c r="E184">
+        <v>3970.15</v>
+      </c>
+      <c r="F184">
+        <v>629.02</v>
+      </c>
+      <c r="G184">
+        <v>1896.991</v>
+      </c>
+      <c r="H184">
+        <v>2053.69</v>
+      </c>
+      <c r="I184">
+        <v>964.01</v>
+      </c>
+      <c r="J184">
+        <v>510.96210000000002</v>
+      </c>
+      <c r="K184">
+        <v>1437.64</v>
+      </c>
+      <c r="L184">
+        <v>1273.56</v>
+      </c>
+      <c r="M184">
+        <v>18991.472000000002</v>
+      </c>
+      <c r="N184">
+        <v>3888.33</v>
+      </c>
+      <c r="O184">
+        <v>1718.69</v>
+      </c>
+      <c r="P184">
+        <v>382.53</v>
+      </c>
+      <c r="Q184">
+        <v>162.4709</v>
+      </c>
+      <c r="R184">
+        <v>4.67272</v>
+      </c>
+      <c r="S184">
+        <v>4.8077261</v>
+      </c>
+      <c r="T184">
+        <v>4976.87</v>
+      </c>
+      <c r="U184">
+        <v>1601.19</v>
+      </c>
+      <c r="V184">
+        <v>2308.3960000000002</v>
+      </c>
+      <c r="W184">
+        <v>134.5625</v>
+      </c>
+      <c r="X184">
+        <v>366.54</v>
       </c>
     </row>
   </sheetData>
@@ -28038,7 +28333,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X179"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
update index data 3/2023
</commit_message>
<xml_diff>
--- a/data/index_data.xlsx
+++ b/data/index_data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RRQ1FYQ\Documents\UPS_MV\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bloomberg\Documents\GitHub\UPS_MV\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4291288E-3FAE-450C-9D1A-4E136433DE6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="450" yWindow="1800" windowWidth="21600" windowHeight="11325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="450" yWindow="1800" windowWidth="21600" windowHeight="11325" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="bbg" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
     <definedName name="SpreadsheetBuilder_1" localSheetId="1" hidden="1">data!$A$1:$P$3</definedName>
     <definedName name="SpreadsheetBuilder_8" hidden="1">bbg!$A$1:$P$7</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -131,7 +130,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000%"/>
   </numFmts>
@@ -207,50 +206,86 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|18237526495139166654</stp>
-        <tr r="N7" s="1"/>
+        <stp>BDH|17994530590059944802</stp>
+        <tr r="L7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|11716787340289124001</stp>
+        <stp>BDH|14614064144859221328</stp>
+        <tr r="M7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|10066041057338964529</stp>
+        <tr r="P7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|13360348291630870662</stp>
+        <tr r="K7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|17379281609409995372</stp>
+        <tr r="Q7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|11973208686543130484</stp>
+        <tr r="J7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|17939252844589858576</stp>
+        <tr r="U7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|11476140918418459444</stp>
+        <tr r="T7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|15714601384368367308</stp>
+        <tr r="S7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|13721467209285278229</stp>
+        <tr r="I7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|13196198711444073682</stp>
+        <tr r="W7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|18101862802616111717</stp>
+        <tr r="O7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|16316854339659422288</stp>
         <tr r="A7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|17984493393030080389</stp>
-        <tr r="E7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|14269559167394485133</stp>
-        <tr r="H7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|13254190218125375505</stp>
+        <stp>BDH|14749983102850481914</stp>
         <tr r="D7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|10613056508164008773</stp>
-        <tr r="I7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|12542054832835615290</stp>
-        <tr r="G7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|17289885426543044979</stp>
-        <tr r="X7" s="1"/>
       </tp>
     </main>
     <main first="bloomberg.rtd">
@@ -323,8 +358,20 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|4423416296506656375</stp>
-        <tr r="Q7" s="1"/>
+        <stp>BDH|4417616153489887246</stp>
+        <tr r="N7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|6701200194435068502</stp>
+        <tr r="V7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|6305991446764064282</stp>
+        <tr r="R7" s="1"/>
       </tp>
     </main>
     <main first="bloomberg.rtd">
@@ -453,86 +500,38 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|3732344933689158519</stp>
-        <tr r="K7" s="1"/>
+        <stp>BDH|1371833314462199579</stp>
+        <tr r="X7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|4628544335325102838</stp>
-        <tr r="V7" s="1"/>
+        <stp>BDH|7124408260957279820</stp>
+        <tr r="H7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|4883981393634241990</stp>
-        <tr r="L7" s="1"/>
+        <stp>BDH|1894109681251107234</stp>
+        <tr r="G7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|3207824271537345139</stp>
+        <stp>BDH|3187446125722133222</stp>
         <tr r="C7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|8319283653537681335</stp>
-        <tr r="R7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|1645143108382074725</stp>
-        <tr r="S7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|5355938979259842728</stp>
-        <tr r="J7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|1471632021310053023</stp>
-        <tr r="O7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|7951969993591120147</stp>
+        <stp>BDH|7865134027932032142</stp>
         <tr r="F7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|2079819245496186834</stp>
-        <tr r="W7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|6680358376653754164</stp>
-        <tr r="P7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|3634296683179203156</stp>
-        <tr r="T7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|5923488071320113518</stp>
-        <tr r="M7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|590095370470294085</stp>
-        <tr r="U7" s="1"/>
+        <stp>BDH|4084044015421773736</stp>
+        <tr r="E7" s="1"/>
       </tp>
     </main>
   </volType>
@@ -835,11 +834,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X189"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X190"/>
   <sheetViews>
-    <sheetView topLeftCell="A140" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A189" sqref="A187:X189"/>
+    <sheetView topLeftCell="A143" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A190" sqref="A189:X190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,7 +872,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7">
-        <v>44985</v>
+        <v>45016</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
@@ -1117,98 +1116,98 @@
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <f>_xll.BDH(B$4,B$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=S","cols=2;rows=183")</f>
+        <f>_xll.BDH(B$4,B$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=S","cols=2;rows=184")</f>
         <v>39447</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
       </c>
       <c r="C7">
-        <f>_xll.BDH(C$4,C$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
+        <f>_xll.BDH(C$4,C$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=184")</f>
         <v>1902.17</v>
       </c>
       <c r="D7" t="str">
-        <f>_xll.BDH(D$4,D$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
+        <f>_xll.BDH(D$4,D$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=184")</f>
         <v>#N/A N/A</v>
       </c>
       <c r="E7">
-        <f>_xll.BDH(E$4,E$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
+        <f>_xll.BDH(E$4,E$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=184")</f>
         <v>1468.36</v>
       </c>
       <c r="F7">
-        <f>_xll.BDH(F$4,F$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
+        <f>_xll.BDH(F$4,F$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=184")</f>
         <v>403.25</v>
       </c>
       <c r="G7">
-        <f>_xll.BDH(G$4,G$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
+        <f>_xll.BDH(G$4,G$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=184")</f>
         <v>766.03700000000003</v>
       </c>
       <c r="H7">
-        <f>_xll.BDH(H$4,H$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
+        <f>_xll.BDH(H$4,H$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=184")</f>
         <v>2253.36</v>
       </c>
       <c r="I7">
-        <f>_xll.BDH(I$4,I$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
+        <f>_xll.BDH(I$4,I$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=184")</f>
         <v>1245.5899999999999</v>
       </c>
       <c r="J7">
-        <f>_xll.BDH(J$4,J$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
+        <f>_xll.BDH(J$4,J$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=184")</f>
         <v>270.02620000000002</v>
       </c>
       <c r="K7">
-        <f>_xll.BDH(K$4,K$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
+        <f>_xll.BDH(K$4,K$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=184")</f>
         <v>590.78</v>
       </c>
       <c r="L7">
-        <f>_xll.BDH(L$4,L$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
+        <f>_xll.BDH(L$4,L$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=184")</f>
         <v>1294.82</v>
       </c>
       <c r="M7">
-        <f>_xll.BDH(M$4,M$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
+        <f>_xll.BDH(M$4,M$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=184")</f>
         <v>12335.221</v>
       </c>
       <c r="N7">
-        <f>_xll.BDH(N$4,N$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
+        <f>_xll.BDH(N$4,N$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=184")</f>
         <v>1915.1320000000001</v>
       </c>
       <c r="O7">
-        <f>_xll.BDH(O$4,O$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
+        <f>_xll.BDH(O$4,O$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=184")</f>
         <v>1389.21</v>
       </c>
       <c r="P7">
-        <f>_xll.BDH(P$4,P$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
+        <f>_xll.BDH(P$4,P$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=184")</f>
         <v>255.67</v>
       </c>
       <c r="Q7">
-        <f>_xll.BDH(Q$4,Q$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
+        <f>_xll.BDH(Q$4,Q$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=184")</f>
         <v>141.76349999999999</v>
       </c>
       <c r="R7">
-        <f>_xll.BDH(R$4,R$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
+        <f>_xll.BDH(R$4,R$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=184")</f>
         <v>3.1589900000000002</v>
       </c>
       <c r="S7">
-        <f>_xll.BDH(S$4,S$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
+        <f>_xll.BDH(S$4,S$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=184")</f>
         <v>3.33792826</v>
       </c>
       <c r="T7">
-        <f>_xll.BDH(T$4,T$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
+        <f>_xll.BDH(T$4,T$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=184")</f>
         <v>1412.28</v>
       </c>
       <c r="U7">
-        <f>_xll.BDH(U$4,U$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
+        <f>_xll.BDH(U$4,U$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=184")</f>
         <v>996.96</v>
       </c>
       <c r="V7">
-        <f>_xll.BDH(V$4,V$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
+        <f>_xll.BDH(V$4,V$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=184")</f>
         <v>849.221</v>
       </c>
       <c r="W7" t="str">
-        <f>_xll.BDH(W$4,W$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
+        <f>_xll.BDH(W$4,W$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=184")</f>
         <v>#N/A N/A</v>
       </c>
       <c r="X7">
-        <f>_xll.BDH(X$4,X$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=183")</f>
+        <f>_xll.BDH(X$4,X$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=184")</f>
         <v>221.59</v>
       </c>
     </row>
@@ -14517,7 +14516,7 @@
         <v>4.3983636739999996</v>
       </c>
       <c r="T187">
-        <v>4976.87</v>
+        <v>5079.05</v>
       </c>
       <c r="U187">
         <v>1536.73</v>
@@ -14591,7 +14590,7 @@
         <v>4.6489987660000001</v>
       </c>
       <c r="T188">
-        <v>4976.87</v>
+        <v>5079.05</v>
       </c>
       <c r="U188">
         <v>1648.91</v>
@@ -14644,7 +14643,7 @@
         <v>1273.56</v>
       </c>
       <c r="M189">
-        <v>18991.472000000002</v>
+        <v>18958.985000000001</v>
       </c>
       <c r="N189">
         <v>3888.33</v>
@@ -14665,7 +14664,7 @@
         <v>4.8077261</v>
       </c>
       <c r="T189">
-        <v>4976.87</v>
+        <v>5079.05</v>
       </c>
       <c r="U189">
         <v>1601.19</v>
@@ -14678,6 +14677,80 @@
       </c>
       <c r="X189">
         <v>366.54</v>
+      </c>
+    </row>
+    <row r="190" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A190" s="1">
+        <v>45016</v>
+      </c>
+      <c r="B190">
+        <v>143.85</v>
+      </c>
+      <c r="C190">
+        <v>4104.91</v>
+      </c>
+      <c r="D190">
+        <v>176.52780000000001</v>
+      </c>
+      <c r="E190">
+        <v>4109.3100000000004</v>
+      </c>
+      <c r="F190">
+        <v>646.76</v>
+      </c>
+      <c r="G190">
+        <v>1802.4839999999999</v>
+      </c>
+      <c r="H190">
+        <v>2092.6</v>
+      </c>
+      <c r="I190">
+        <v>990.28</v>
+      </c>
+      <c r="J190">
+        <v>510.464</v>
+      </c>
+      <c r="K190">
+        <v>1453.82</v>
+      </c>
+      <c r="L190">
+        <v>1235.1600000000001</v>
+      </c>
+      <c r="M190">
+        <v>18958.985000000001</v>
+      </c>
+      <c r="N190">
+        <v>3589.37</v>
+      </c>
+      <c r="O190">
+        <v>1718.69</v>
+      </c>
+      <c r="P190">
+        <v>373.22</v>
+      </c>
+      <c r="Q190">
+        <v>162.4709</v>
+      </c>
+      <c r="R190">
+        <v>4.6408199999999997</v>
+      </c>
+      <c r="S190">
+        <v>4.7309068339999998</v>
+      </c>
+      <c r="T190">
+        <v>5079.05</v>
+      </c>
+      <c r="U190">
+        <v>1636.36</v>
+      </c>
+      <c r="V190">
+        <v>2366.27</v>
+      </c>
+      <c r="W190">
+        <v>141.125</v>
+      </c>
+      <c r="X190">
+        <v>385.5</v>
       </c>
     </row>
   </sheetData>
@@ -14686,11 +14759,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:X184"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X185"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A153" workbookViewId="0">
-      <selection activeCell="C177" sqref="C177"/>
+      <selection activeCell="C170" sqref="C170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28291,7 +28364,7 @@
         <v>1273.56</v>
       </c>
       <c r="M184">
-        <v>18991.472000000002</v>
+        <v>18958.985000000001</v>
       </c>
       <c r="N184">
         <v>3888.33</v>
@@ -28312,7 +28385,7 @@
         <v>4.8077261</v>
       </c>
       <c r="T184">
-        <v>4976.87</v>
+        <v>5079.05</v>
       </c>
       <c r="U184">
         <v>1601.19</v>
@@ -28325,6 +28398,80 @@
       </c>
       <c r="X184">
         <v>366.54</v>
+      </c>
+    </row>
+    <row r="185" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A185" s="1">
+        <v>45016</v>
+      </c>
+      <c r="B185">
+        <v>143.85</v>
+      </c>
+      <c r="C185">
+        <v>4104.91</v>
+      </c>
+      <c r="D185">
+        <v>176.52780000000001</v>
+      </c>
+      <c r="E185">
+        <v>4109.3100000000004</v>
+      </c>
+      <c r="F185">
+        <v>646.76</v>
+      </c>
+      <c r="G185">
+        <v>1802.4839999999999</v>
+      </c>
+      <c r="H185">
+        <v>2092.6</v>
+      </c>
+      <c r="I185">
+        <v>990.28</v>
+      </c>
+      <c r="J185">
+        <v>510.464</v>
+      </c>
+      <c r="K185">
+        <v>1453.82</v>
+      </c>
+      <c r="L185">
+        <v>1235.1600000000001</v>
+      </c>
+      <c r="M185">
+        <v>18958.985000000001</v>
+      </c>
+      <c r="N185">
+        <v>3589.37</v>
+      </c>
+      <c r="O185">
+        <v>1718.69</v>
+      </c>
+      <c r="P185">
+        <v>373.22</v>
+      </c>
+      <c r="Q185">
+        <v>162.4709</v>
+      </c>
+      <c r="R185">
+        <v>4.6408199999999997</v>
+      </c>
+      <c r="S185">
+        <v>4.7309068339999998</v>
+      </c>
+      <c r="T185">
+        <v>5079.05</v>
+      </c>
+      <c r="U185">
+        <v>1636.36</v>
+      </c>
+      <c r="V185">
+        <v>2366.27</v>
+      </c>
+      <c r="W185">
+        <v>141.125</v>
+      </c>
+      <c r="X185">
+        <v>385.5</v>
       </c>
     </row>
   </sheetData>
@@ -28333,7 +28480,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X179"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
update index data and equity hedge data 6/30/2023
</commit_message>
<xml_diff>
--- a/data/index_data.xlsx
+++ b/data/index_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RRQ1FYQ\Documents\UPS_MV\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4271A7AE-15EA-4827-8CF5-FA9312CF18EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A279FF94-4A3D-49D6-AE26-7DD8E22FF5D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28690" yWindow="-50" windowWidth="29020" windowHeight="15820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bbg" sheetId="1" r:id="rId1"/>
@@ -207,62 +207,68 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|16292177803839189059</stp>
-        <tr r="N7" s="1"/>
+        <stp>BDH|14430508253105431889</stp>
+        <tr r="J7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|17988952705723847269</stp>
+        <stp>BDH|13300111439778905093</stp>
+        <tr r="R7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|17054979179049051922</stp>
         <tr r="X7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|12067926999587948708</stp>
+        <stp>BDH|14573662733917990494</stp>
+        <tr r="E7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|15264966013319547236</stp>
+        <tr r="V7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|14138442034706631236</stp>
+        <tr r="W7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|16750789879671825027</stp>
+        <tr r="O7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|17684609975043374173</stp>
+        <tr r="C7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|17232476322746686222</stp>
         <tr r="K7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|14540102340774316643</stp>
-        <tr r="V7" s="1"/>
+        <stp>BDH|18424911560534582667</stp>
+        <tr r="U7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|11570793133451546734</stp>
-        <tr r="E7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|12460200030597930777</stp>
-        <tr r="D7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|15996052102095826030</stp>
-        <tr r="S7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|18105468774372977826</stp>
+        <stp>BDH|14798026118925185568</stp>
         <tr r="T7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|10066179351251429322</stp>
-        <tr r="W7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|11139072104960448668</stp>
-        <tr r="O7" s="1"/>
       </tp>
     </main>
     <main first="bloomberg.rtd">
@@ -335,32 +341,20 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|2787984733547940391</stp>
-        <tr r="L7" s="1"/>
+        <stp>BDH|9475382885488797639</stp>
+        <tr r="A7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|9456689022549277953</stp>
-        <tr r="C7" s="1"/>
+        <stp>BDH|1759676734358192016</stp>
+        <tr r="N7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|4490232062748490543</stp>
-        <tr r="Q7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|40761258190329259</stp>
+        <stp>BDH|2680171383107945154</stp>
         <tr r="I7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|97018755010856558</stp>
-        <tr r="R7" s="1"/>
       </tp>
     </main>
     <main first="bloomberg.rtd">
@@ -489,50 +483,56 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|8673555013017436415</stp>
-        <tr r="M7" s="1"/>
+        <stp>BDH|9091616480626840958</stp>
+        <tr r="S7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|3177733186871178420</stp>
-        <tr r="J7" s="1"/>
+        <stp>BDH|6648897089413683196</stp>
+        <tr r="H7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|8847738042261444031</stp>
-        <tr r="U7" s="1"/>
+        <stp>BDH|4671485203977821397</stp>
+        <tr r="L7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|2444586119726993522</stp>
+        <stp>BDH|7774624745716708612</stp>
+        <tr r="G7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|2509090463804255763</stp>
+        <tr r="F7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|2414594225336140364</stp>
+        <tr r="D7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|4665116362116927401</stp>
         <tr r="P7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|1706159518261063577</stp>
-        <tr r="G7" s="1"/>
+        <stp>BDH|2589533274723677268</stp>
+        <tr r="Q7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|4521756224046205239</stp>
-        <tr r="F7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|6319051472520387107</stp>
-        <tr r="H7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|1956056447826009014</stp>
-        <tr r="A7" s="1"/>
+        <stp>BDH|327312568533046778</stp>
+        <tr r="M7" s="1"/>
       </tp>
     </main>
   </volType>
@@ -836,10 +836,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X192"/>
+  <dimension ref="A1:X193"/>
   <sheetViews>
-    <sheetView topLeftCell="C171" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A192" sqref="A192:X192"/>
+    <sheetView topLeftCell="A145" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A193" sqref="A193:X193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -873,7 +873,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7">
-        <v>45077</v>
+        <v>45107</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.35">
@@ -1117,98 +1117,98 @@
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
-        <f>_xll.BDH(B$4,B$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=S","cols=2;rows=186")</f>
+        <f>_xll.BDH(B$4,B$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=S","cols=2;rows=187")</f>
         <v>39447</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
       </c>
       <c r="C7">
-        <f>_xll.BDH(C$4,C$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=186")</f>
+        <f>_xll.BDH(C$4,C$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=187")</f>
         <v>1902.17</v>
       </c>
       <c r="D7" t="str">
-        <f>_xll.BDH(D$4,D$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=186")</f>
+        <f>_xll.BDH(D$4,D$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=187")</f>
         <v>#N/A N/A</v>
       </c>
       <c r="E7">
-        <f>_xll.BDH(E$4,E$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=186")</f>
+        <f>_xll.BDH(E$4,E$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=187")</f>
         <v>1468.36</v>
       </c>
       <c r="F7">
-        <f>_xll.BDH(F$4,F$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=186")</f>
+        <f>_xll.BDH(F$4,F$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=187")</f>
         <v>403.25</v>
       </c>
       <c r="G7">
-        <f>_xll.BDH(G$4,G$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=186")</f>
+        <f>_xll.BDH(G$4,G$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=187")</f>
         <v>766.03700000000003</v>
       </c>
       <c r="H7">
-        <f>_xll.BDH(H$4,H$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=186")</f>
+        <f>_xll.BDH(H$4,H$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=187")</f>
         <v>2253.36</v>
       </c>
       <c r="I7">
-        <f>_xll.BDH(I$4,I$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=186")</f>
+        <f>_xll.BDH(I$4,I$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=187")</f>
         <v>1245.5899999999999</v>
       </c>
       <c r="J7">
-        <f>_xll.BDH(J$4,J$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=186")</f>
+        <f>_xll.BDH(J$4,J$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=187")</f>
         <v>270.02620000000002</v>
       </c>
       <c r="K7">
-        <f>_xll.BDH(K$4,K$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=186")</f>
+        <f>_xll.BDH(K$4,K$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=187")</f>
         <v>590.78</v>
       </c>
       <c r="L7">
-        <f>_xll.BDH(L$4,L$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=186")</f>
+        <f>_xll.BDH(L$4,L$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=187")</f>
         <v>1294.82</v>
       </c>
       <c r="M7">
-        <f>_xll.BDH(M$4,M$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=186")</f>
+        <f>_xll.BDH(M$4,M$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=187")</f>
         <v>12335.221</v>
       </c>
       <c r="N7">
-        <f>_xll.BDH(N$4,N$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=186")</f>
+        <f>_xll.BDH(N$4,N$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=187")</f>
         <v>1915.1320000000001</v>
       </c>
       <c r="O7">
-        <f>_xll.BDH(O$4,O$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=186")</f>
+        <f>_xll.BDH(O$4,O$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=187")</f>
         <v>1389.21</v>
       </c>
       <c r="P7">
-        <f>_xll.BDH(P$4,P$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=186")</f>
+        <f>_xll.BDH(P$4,P$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=187")</f>
         <v>255.67</v>
       </c>
       <c r="Q7">
-        <f>_xll.BDH(Q$4,Q$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=186")</f>
+        <f>_xll.BDH(Q$4,Q$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=187")</f>
         <v>141.76349999999999</v>
       </c>
       <c r="R7">
-        <f>_xll.BDH(R$4,R$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=186")</f>
+        <f>_xll.BDH(R$4,R$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=187")</f>
         <v>3.1589900000000002</v>
       </c>
       <c r="S7">
-        <f>_xll.BDH(S$4,S$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=186")</f>
+        <f>_xll.BDH(S$4,S$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=187")</f>
         <v>3.33792826</v>
       </c>
       <c r="T7">
-        <f>_xll.BDH(T$4,T$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=186")</f>
+        <f>_xll.BDH(T$4,T$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=187")</f>
         <v>1412.28</v>
       </c>
       <c r="U7">
-        <f>_xll.BDH(U$4,U$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=186")</f>
+        <f>_xll.BDH(U$4,U$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=187")</f>
         <v>996.96</v>
       </c>
       <c r="V7">
-        <f>_xll.BDH(V$4,V$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=186")</f>
+        <f>_xll.BDH(V$4,V$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=187")</f>
         <v>849.221</v>
       </c>
       <c r="W7" t="str">
-        <f>_xll.BDH(W$4,W$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=186")</f>
+        <f>_xll.BDH(W$4,W$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=187")</f>
         <v>#N/A N/A</v>
       </c>
       <c r="X7">
-        <f>_xll.BDH(X$4,X$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=186")</f>
+        <f>_xll.BDH(X$4,X$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=187")</f>
         <v>221.59</v>
       </c>
     </row>
@@ -14866,10 +14866,10 @@
         <v>1263.18</v>
       </c>
       <c r="M192">
-        <v>18571.196</v>
+        <v>18548.652999999998</v>
       </c>
       <c r="N192">
-        <v>3801.7919999999999</v>
+        <v>3798.5059999999999</v>
       </c>
       <c r="O192">
         <v>1718.69</v>
@@ -14900,6 +14900,80 @@
       </c>
       <c r="X192">
         <v>379.55</v>
+      </c>
+    </row>
+    <row r="193" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A193" s="1">
+        <v>45107</v>
+      </c>
+      <c r="B193">
+        <v>139.72999999999999</v>
+      </c>
+      <c r="C193">
+        <v>4082.76</v>
+      </c>
+      <c r="D193">
+        <v>169.756</v>
+      </c>
+      <c r="E193">
+        <v>4450.38</v>
+      </c>
+      <c r="F193">
+        <v>682.84</v>
+      </c>
+      <c r="G193">
+        <v>1888.7339999999999</v>
+      </c>
+      <c r="H193">
+        <v>2131.7199999999998</v>
+      </c>
+      <c r="I193">
+        <v>989.48</v>
+      </c>
+      <c r="J193">
+        <v>526.38220000000001</v>
+      </c>
+      <c r="K193">
+        <v>1477.58</v>
+      </c>
+      <c r="L193">
+        <v>1270.1099999999999</v>
+      </c>
+      <c r="M193">
+        <v>18821.123</v>
+      </c>
+      <c r="N193">
+        <v>3875.848</v>
+      </c>
+      <c r="O193">
+        <v>1718.69</v>
+      </c>
+      <c r="P193">
+        <v>373.51</v>
+      </c>
+      <c r="Q193">
+        <v>162.4709</v>
+      </c>
+      <c r="R193">
+        <v>5.2157900000000001</v>
+      </c>
+      <c r="S193">
+        <v>5.2487262379999997</v>
+      </c>
+      <c r="T193">
+        <v>5215.8100000000004</v>
+      </c>
+      <c r="U193">
+        <v>1722.87</v>
+      </c>
+      <c r="V193">
+        <v>2554.4879999999998</v>
+      </c>
+      <c r="W193">
+        <v>136.21875</v>
+      </c>
+      <c r="X193">
+        <v>376.94</v>
       </c>
     </row>
   </sheetData>
@@ -14909,10 +14983,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:X187"/>
+  <dimension ref="A1:X188"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
+      <selection activeCell="D182" sqref="D182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -28771,6 +28845,80 @@
         <v>379.55</v>
       </c>
     </row>
+    <row r="188" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A188" s="1">
+        <v>45107</v>
+      </c>
+      <c r="B188">
+        <v>139.72999999999999</v>
+      </c>
+      <c r="C188">
+        <v>4082.76</v>
+      </c>
+      <c r="D188">
+        <v>169.756</v>
+      </c>
+      <c r="E188">
+        <v>4450.38</v>
+      </c>
+      <c r="F188">
+        <v>682.84</v>
+      </c>
+      <c r="G188">
+        <v>1888.7339999999999</v>
+      </c>
+      <c r="H188">
+        <v>2131.7199999999998</v>
+      </c>
+      <c r="I188">
+        <v>989.48</v>
+      </c>
+      <c r="J188">
+        <v>526.38220000000001</v>
+      </c>
+      <c r="K188">
+        <v>1477.58</v>
+      </c>
+      <c r="L188">
+        <v>1270.1099999999999</v>
+      </c>
+      <c r="M188">
+        <v>18821.123</v>
+      </c>
+      <c r="N188">
+        <v>3875.848</v>
+      </c>
+      <c r="O188">
+        <v>1718.69</v>
+      </c>
+      <c r="P188">
+        <v>373.51</v>
+      </c>
+      <c r="Q188">
+        <v>162.4709</v>
+      </c>
+      <c r="R188">
+        <v>5.2157900000000001</v>
+      </c>
+      <c r="S188">
+        <v>5.2487262379999997</v>
+      </c>
+      <c r="T188">
+        <v>5215.8100000000004</v>
+      </c>
+      <c r="U188">
+        <v>1722.87</v>
+      </c>
+      <c r="V188">
+        <v>2554.4879999999998</v>
+      </c>
+      <c r="W188">
+        <v>136.21875</v>
+      </c>
+      <c r="X188">
+        <v>376.94</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -28781,8 +28929,8 @@
   <dimension ref="A1:X179"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A169" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11:A179"/>
+      <pane ySplit="1" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A179" sqref="A176:R179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
update equity hedge data and index data 8/31/2023
</commit_message>
<xml_diff>
--- a/data/index_data.xlsx
+++ b/data/index_data.xlsx
@@ -205,80 +205,68 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|15704611409131547986</stp>
+        <stp>BDH|17236690565707920910</stp>
+        <tr r="R7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|13297851655590193145</stp>
         <tr r="W7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|12578794970191210854</stp>
-        <tr r="K7" s="1"/>
+        <stp>BDH|12926881264240898362</stp>
+        <tr r="Y7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|16751372766569035577</stp>
+        <stp>BDH|14913224394640073269</stp>
+        <tr r="D7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|14837846873736313046</stp>
+        <tr r="L7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|11971190572452601512</stp>
         <tr r="M7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|10019762198386025471</stp>
-        <tr r="T7" s="1"/>
+        <stp>BDH|12055499512048169900</stp>
+        <tr r="F7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|16802085578070638315</stp>
-        <tr r="Q7" s="1"/>
+        <stp>BDH|17448202811811406212</stp>
+        <tr r="P7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|13803598231190848635</stp>
+        <stp>BDH|18075417015289167059</stp>
         <tr r="G7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|14119084901273067715</stp>
-        <tr r="P7" s="1"/>
+        <stp>BDH|15548123227067243483</stp>
+        <tr r="A7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|14575500529786634551</stp>
-        <tr r="L7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|10401488906425032711</stp>
-        <tr r="Y7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|17207570018174916070</stp>
-        <tr r="E7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|11199792137282520392</stp>
-        <tr r="D7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|10996652712136526520</stp>
-        <tr r="I7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|14353583720632358535</stp>
-        <tr r="F7" s="1"/>
+        <stp>BDH|12058450981862031989</stp>
+        <tr r="S7" s="1"/>
       </tp>
     </main>
     <main first="bloomberg.rtd">
@@ -351,8 +339,32 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|7660588928386380857</stp>
-        <tr r="S7" s="1"/>
+        <stp>BDH|6547989470101314558</stp>
+        <tr r="J7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|7925042130241954952</stp>
+        <tr r="T7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|7802926848347401096</stp>
+        <tr r="I7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|3942950741802448155</stp>
+        <tr r="N7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|4823383110640400848</stp>
+        <tr r="C7" s="1"/>
       </tp>
     </main>
     <main first="bloomberg.rtd">
@@ -489,62 +501,50 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|3066111060899481677</stp>
+        <stp>BDH|8933502120889095924</stp>
+        <tr r="Q7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|2503271317151895933</stp>
+        <tr r="E7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|2997792379889335131</stp>
         <tr r="H7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|8623347243285480159</stp>
-        <tr r="R7" s="1"/>
+        <stp>BDH|5345391822715725709</stp>
+        <tr r="V7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|5978705900445174175</stp>
-        <tr r="J7" s="1"/>
+        <stp>BDH|5902682273164826096</stp>
+        <tr r="X7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|9115383278289275591</stp>
-        <tr r="N7" s="1"/>
+        <stp>BDH|5406525454397911320</stp>
+        <tr r="K7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|8088141795562237353</stp>
+        <stp>BDH|3235266235923597252</stp>
         <tr r="O7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|7873303195008770764</stp>
+        <stp>BDH|539207429269322929</stp>
         <tr r="U7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|6127367128415885171</stp>
-        <tr r="C7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|6413629914772277044</stp>
-        <tr r="A7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|425472714690785074</stp>
-        <tr r="X7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|613858023814496423</stp>
-        <tr r="V7" s="1"/>
       </tp>
     </main>
   </volType>
@@ -848,10 +848,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y188"/>
+  <dimension ref="A1:Y195"/>
   <sheetViews>
-    <sheetView topLeftCell="A143" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A186" sqref="A186:Y188"/>
+    <sheetView topLeftCell="A163" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A188" sqref="A188:Y195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,7 +885,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>44957</v>
+        <v>45169</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -1139,102 +1139,102 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <f>_xll.BDH(B$4,B$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=S","cols=2;rows=182")</f>
+        <f>_xll.BDH(B$4,B$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=S","cols=2;rows=189")</f>
         <v>39447</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
       </c>
       <c r="C7">
-        <f>_xll.BDH(C$4,C$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
+        <f>_xll.BDH(C$4,C$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=189")</f>
         <v>1902.17</v>
       </c>
       <c r="D7" t="str">
-        <f>_xll.BDH(D$4,D$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
+        <f>_xll.BDH(D$4,D$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=189")</f>
         <v>#N/A N/A</v>
       </c>
       <c r="E7">
-        <f>_xll.BDH(E$4,E$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
+        <f>_xll.BDH(E$4,E$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=189")</f>
         <v>1468.36</v>
       </c>
       <c r="F7">
-        <f>_xll.BDH(F$4,F$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
+        <f>_xll.BDH(F$4,F$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=189")</f>
         <v>403.25</v>
       </c>
       <c r="G7">
-        <f>_xll.BDH(G$4,G$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
+        <f>_xll.BDH(G$4,G$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=189")</f>
         <v>766.03700000000003</v>
       </c>
       <c r="H7">
-        <f>_xll.BDH(H$4,H$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
+        <f>_xll.BDH(H$4,H$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=189")</f>
         <v>2253.36</v>
       </c>
       <c r="I7">
-        <f>_xll.BDH(I$4,I$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
+        <f>_xll.BDH(I$4,I$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=189")</f>
         <v>1245.5899999999999</v>
       </c>
       <c r="J7">
-        <f>_xll.BDH(J$4,J$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
+        <f>_xll.BDH(J$4,J$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=189")</f>
         <v>270.02620000000002</v>
       </c>
       <c r="K7">
-        <f>_xll.BDH(K$4,K$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
+        <f>_xll.BDH(K$4,K$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=189")</f>
         <v>590.78</v>
       </c>
       <c r="L7">
-        <f>_xll.BDH(L$4,L$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
-        <v>1294.82</v>
+        <f>_xll.BDH(L$4,L$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=189")</f>
+        <v>1294.818</v>
       </c>
       <c r="M7">
-        <f>_xll.BDH(M$4,M$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
+        <f>_xll.BDH(M$4,M$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=189")</f>
         <v>12335.221</v>
       </c>
       <c r="N7">
-        <f>_xll.BDH(N$4,N$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
+        <f>_xll.BDH(N$4,N$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=189")</f>
         <v>1915.1320000000001</v>
       </c>
       <c r="O7">
-        <f>_xll.BDH(O$4,O$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
+        <f>_xll.BDH(O$4,O$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=189")</f>
         <v>1389.21</v>
       </c>
       <c r="P7">
-        <f>_xll.BDH(P$4,P$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
+        <f>_xll.BDH(P$4,P$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=189")</f>
         <v>255.67</v>
       </c>
       <c r="Q7">
-        <f>_xll.BDH(Q$4,Q$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
+        <f>_xll.BDH(Q$4,Q$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=189")</f>
         <v>141.76349999999999</v>
       </c>
       <c r="R7">
-        <f>_xll.BDH(R$4,R$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
+        <f>_xll.BDH(R$4,R$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=189")</f>
         <v>3.1589900000000002</v>
       </c>
       <c r="S7">
-        <f>_xll.BDH(S$4,S$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
+        <f>_xll.BDH(S$4,S$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=189")</f>
         <v>3.33792826</v>
       </c>
       <c r="T7">
-        <f>_xll.BDH(T$4,T$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
+        <f>_xll.BDH(T$4,T$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=189")</f>
         <v>1412.28</v>
       </c>
       <c r="U7">
-        <f>_xll.BDH(U$4,U$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
+        <f>_xll.BDH(U$4,U$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=189")</f>
         <v>996.96</v>
       </c>
       <c r="V7">
-        <f>_xll.BDH(V$4,V$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
+        <f>_xll.BDH(V$4,V$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=189")</f>
         <v>849.221</v>
       </c>
       <c r="W7" t="str">
-        <f>_xll.BDH(W$4,W$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
+        <f>_xll.BDH(W$4,W$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=189")</f>
         <v>#N/A N/A</v>
       </c>
       <c r="X7">
-        <f>_xll.BDH(X$4,X$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
+        <f>_xll.BDH(X$4,X$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=189")</f>
         <v>221.59</v>
       </c>
       <c r="Y7">
-        <f>_xll.BDH(Y$4,Y$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=182")</f>
+        <f>_xll.BDH(Y$4,Y$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=189")</f>
         <v>1174.52</v>
       </c>
     </row>
@@ -1270,13 +1270,13 @@
         <v>261.66860000000003</v>
       </c>
       <c r="K8">
-        <v>582.75</v>
+        <v>582.75300000000004</v>
       </c>
       <c r="L8">
-        <v>1344.27</v>
+        <v>1344.268</v>
       </c>
       <c r="M8">
-        <v>12468.7682</v>
+        <v>12468.768</v>
       </c>
       <c r="N8">
         <v>1965.15</v>
@@ -1347,13 +1347,13 @@
         <v>255.42519999999999</v>
       </c>
       <c r="K9">
-        <v>575.83000000000004</v>
+        <v>575.83399999999995</v>
       </c>
       <c r="L9">
-        <v>1459.01</v>
+        <v>1459.009</v>
       </c>
       <c r="M9">
-        <v>12994.856299999999</v>
+        <v>12994.856</v>
       </c>
       <c r="N9">
         <v>2106.0329999999999</v>
@@ -1424,13 +1424,13 @@
         <v>254.5256</v>
       </c>
       <c r="K10">
-        <v>572.84</v>
+        <v>572.84400000000005</v>
       </c>
       <c r="L10">
-        <v>1415.2</v>
+        <v>1415.204</v>
       </c>
       <c r="M10">
-        <v>12836.166800000001</v>
+        <v>12836.166999999999</v>
       </c>
       <c r="N10">
         <v>2077.0700000000002</v>
@@ -1501,13 +1501,13 @@
         <v>262.93880000000001</v>
       </c>
       <c r="K11">
-        <v>596.71</v>
+        <v>596.70699999999999</v>
       </c>
       <c r="L11">
         <v>1405.95</v>
       </c>
       <c r="M11">
-        <v>12831.954900000001</v>
+        <v>12831.955</v>
       </c>
       <c r="N11">
         <v>2041.4290000000001</v>
@@ -1578,13 +1578,13 @@
         <v>264.8886</v>
       </c>
       <c r="K12">
-        <v>599.26</v>
+        <v>599.26300000000003</v>
       </c>
       <c r="L12">
-        <v>1430.86</v>
+        <v>1430.864</v>
       </c>
       <c r="M12">
-        <v>12986.5229</v>
+        <v>12986.522999999999</v>
       </c>
       <c r="N12">
         <v>2094.21</v>
@@ -1655,13 +1655,13 @@
         <v>265.29180000000002</v>
       </c>
       <c r="K13">
-        <v>583.21</v>
+        <v>583.20600000000002</v>
       </c>
       <c r="L13">
-        <v>1477.36</v>
+        <v>1477.3610000000001</v>
       </c>
       <c r="M13">
-        <v>13141.3627</v>
+        <v>13141.362999999999</v>
       </c>
       <c r="N13">
         <v>2207.183</v>
@@ -1732,13 +1732,13 @@
         <v>262.70940000000002</v>
       </c>
       <c r="K14">
-        <v>573.86</v>
+        <v>573.85900000000004</v>
       </c>
       <c r="L14">
         <v>1394.77</v>
       </c>
       <c r="M14">
-        <v>12796.566800000001</v>
+        <v>12796.566999999999</v>
       </c>
       <c r="N14">
         <v>2095.7800000000002</v>
@@ -1809,13 +1809,13 @@
         <v>262.5575</v>
       </c>
       <c r="K15">
-        <v>575.71</v>
+        <v>575.71100000000001</v>
       </c>
       <c r="L15">
-        <v>1339.78</v>
+        <v>1339.7809999999999</v>
       </c>
       <c r="M15">
-        <v>12645.730799999999</v>
+        <v>12645.731</v>
       </c>
       <c r="N15">
         <v>2035.0039999999999</v>
@@ -1886,13 +1886,13 @@
         <v>249.61969999999999</v>
       </c>
       <c r="K16">
-        <v>527.94000000000005</v>
+        <v>527.94200000000001</v>
       </c>
       <c r="L16">
-        <v>1328.39</v>
+        <v>1328.394</v>
       </c>
       <c r="M16">
-        <v>12492.1569</v>
+        <v>12492.156999999999</v>
       </c>
       <c r="N16">
         <v>2054.8670000000002</v>
@@ -1963,13 +1963,13 @@
         <v>217.0848</v>
       </c>
       <c r="K17">
-        <v>441.9</v>
+        <v>441.89600000000002</v>
       </c>
       <c r="L17">
-        <v>1304.98</v>
+        <v>1304.9829999999999</v>
       </c>
       <c r="M17">
-        <v>12695.992899999999</v>
+        <v>12695.993</v>
       </c>
       <c r="N17">
         <v>2205.1550000000002</v>
@@ -2040,13 +2040,13 @@
         <v>199.9513</v>
       </c>
       <c r="K18">
-        <v>404.63</v>
+        <v>404.63400000000001</v>
       </c>
       <c r="L18">
-        <v>1324.36</v>
+        <v>1324.355</v>
       </c>
       <c r="M18">
-        <v>12789.034900000001</v>
+        <v>12789.035</v>
       </c>
       <c r="N18">
         <v>2267.3110000000001</v>
@@ -2117,13 +2117,13 @@
         <v>192.38509999999999</v>
       </c>
       <c r="K19">
-        <v>434.88</v>
+        <v>434.87799999999999</v>
       </c>
       <c r="L19">
-        <v>1367.51</v>
+        <v>1367.5050000000001</v>
       </c>
       <c r="M19">
-        <v>12931.3459</v>
+        <v>12931.346</v>
       </c>
       <c r="N19">
         <v>2315.06</v>
@@ -2194,13 +2194,13 @@
         <v>203.49539999999999</v>
       </c>
       <c r="K20">
-        <v>457.96</v>
+        <v>457.96100000000001</v>
       </c>
       <c r="L20">
         <v>1387.26</v>
       </c>
       <c r="M20">
-        <v>12918.482099999999</v>
+        <v>12918.482</v>
       </c>
       <c r="N20">
         <v>2307.8919999999998</v>
@@ -2271,13 +2271,13 @@
         <v>204.20050000000001</v>
       </c>
       <c r="K21">
-        <v>442.09</v>
+        <v>442.08499999999998</v>
       </c>
       <c r="L21">
-        <v>1386.56</v>
+        <v>1386.559</v>
       </c>
       <c r="M21">
-        <v>12902.6587</v>
+        <v>12902.659</v>
       </c>
       <c r="N21">
         <v>2320.3330000000001</v>
@@ -2425,13 +2425,13 @@
         <v>222.69049999999999</v>
       </c>
       <c r="K23">
-        <v>509.05</v>
+        <v>509.05399999999997</v>
       </c>
       <c r="L23">
-        <v>1344.19</v>
+        <v>1344.194</v>
       </c>
       <c r="M23">
-        <v>12811.928599999999</v>
+        <v>12811.929</v>
       </c>
       <c r="N23">
         <v>2196.0830000000001</v>
@@ -2502,13 +2502,13 @@
         <v>235.3854</v>
       </c>
       <c r="K24">
-        <v>545.26</v>
+        <v>545.26300000000003</v>
       </c>
       <c r="L24">
-        <v>1330.23</v>
+        <v>1330.2260000000001</v>
       </c>
       <c r="M24">
-        <v>13264.861699999999</v>
+        <v>13264.861999999999</v>
       </c>
       <c r="N24">
         <v>2206.9</v>
@@ -2579,10 +2579,10 @@
         <v>244.51750000000001</v>
       </c>
       <c r="K25">
-        <v>562.6</v>
+        <v>562.601</v>
       </c>
       <c r="L25">
-        <v>1285.96</v>
+        <v>1285.9549999999999</v>
       </c>
       <c r="M25">
         <v>13109.794</v>
@@ -2656,13 +2656,13 @@
         <v>254.65369999999999</v>
       </c>
       <c r="K26">
-        <v>597.39</v>
+        <v>597.38699999999994</v>
       </c>
       <c r="L26">
-        <v>1286.8900000000001</v>
+        <v>1286.894</v>
       </c>
       <c r="M26">
-        <v>13174.286400000001</v>
+        <v>13174.286</v>
       </c>
       <c r="N26">
         <v>2141.98</v>
@@ -2733,13 +2733,13 @@
         <v>260.33589999999998</v>
       </c>
       <c r="K27">
-        <v>609.54</v>
+        <v>609.53700000000003</v>
       </c>
       <c r="L27">
-        <v>1276.6099999999999</v>
+        <v>1276.6079999999999</v>
       </c>
       <c r="M27">
-        <v>13223.647800000001</v>
+        <v>13223.647999999999</v>
       </c>
       <c r="N27">
         <v>2175.6089999999999</v>
@@ -2810,13 +2810,13 @@
         <v>268.88839999999999</v>
       </c>
       <c r="K28">
-        <v>645.96</v>
+        <v>645.96299999999997</v>
       </c>
       <c r="L28">
-        <v>1267.52</v>
+        <v>1267.5150000000001</v>
       </c>
       <c r="M28">
-        <v>13449.626700000001</v>
+        <v>13449.627</v>
       </c>
       <c r="N28">
         <v>2227.857</v>
@@ -2887,13 +2887,13 @@
         <v>270.64179999999999</v>
       </c>
       <c r="K29">
-        <v>657.5</v>
+        <v>657.50199999999995</v>
       </c>
       <c r="L29">
-        <v>1250.6199999999999</v>
+        <v>1250.6179999999999</v>
       </c>
       <c r="M29">
-        <v>13380.286099999999</v>
+        <v>13380.286</v>
       </c>
       <c r="N29">
         <v>2162.4050000000002</v>
@@ -2964,13 +2964,13 @@
         <v>271.42450000000002</v>
       </c>
       <c r="K30">
-        <v>664.16</v>
+        <v>664.16399999999999</v>
       </c>
       <c r="L30">
-        <v>1281.04</v>
+        <v>1281.0419999999999</v>
       </c>
       <c r="M30">
-        <v>13670.636699999999</v>
+        <v>13670.637000000001</v>
       </c>
       <c r="N30">
         <v>2274.2429999999999</v>
@@ -3041,10 +3041,10 @@
         <v>278.7047</v>
       </c>
       <c r="K31">
-        <v>684.98</v>
+        <v>684.98299999999995</v>
       </c>
       <c r="L31">
-        <v>1247.43</v>
+        <v>1247.434</v>
       </c>
       <c r="M31">
         <v>13492.601000000001</v>
@@ -3118,13 +3118,13 @@
         <v>283.74540000000002</v>
       </c>
       <c r="K32">
-        <v>695.36</v>
+        <v>695.36400000000003</v>
       </c>
       <c r="L32">
-        <v>1224.45</v>
+        <v>1224.4449999999999</v>
       </c>
       <c r="M32">
-        <v>13229.0828</v>
+        <v>13229.083000000001</v>
       </c>
       <c r="N32">
         <v>2119.4940000000001</v>
@@ -3195,13 +3195,13 @@
         <v>284.66649999999998</v>
       </c>
       <c r="K33">
-        <v>696.44</v>
+        <v>696.44100000000003</v>
       </c>
       <c r="L33">
-        <v>1241.75</v>
+        <v>1241.7539999999999</v>
       </c>
       <c r="M33">
-        <v>13250.2135</v>
+        <v>13250.214</v>
       </c>
       <c r="N33">
         <v>2161.3310000000001</v>
@@ -3272,13 +3272,13 @@
         <v>290.81540000000001</v>
       </c>
       <c r="K34">
-        <v>718</v>
+        <v>718.00099999999998</v>
       </c>
       <c r="L34">
-        <v>1255.06</v>
+        <v>1255.059</v>
       </c>
       <c r="M34">
-        <v>13460.915499999999</v>
+        <v>13460.915999999999</v>
       </c>
       <c r="N34">
         <v>2267.1979999999999</v>
@@ -3349,13 +3349,13 @@
         <v>294.53320000000002</v>
       </c>
       <c r="K35">
-        <v>734.08</v>
+        <v>734.077</v>
       </c>
       <c r="L35">
         <v>1246.22</v>
       </c>
       <c r="M35">
-        <v>13570.9728</v>
+        <v>13570.973</v>
       </c>
       <c r="N35">
         <v>2313.11</v>
@@ -3426,13 +3426,13 @@
         <v>288.47559999999999</v>
       </c>
       <c r="K36">
-        <v>708.23</v>
+        <v>708.23299999999995</v>
       </c>
       <c r="L36">
         <v>1234.72</v>
       </c>
       <c r="M36">
-        <v>13356.1283</v>
+        <v>13356.128000000001</v>
       </c>
       <c r="N36">
         <v>2208.9389999999999</v>
@@ -3503,13 +3503,13 @@
         <v>287.77719999999999</v>
       </c>
       <c r="K37">
-        <v>717.47</v>
+        <v>717.46699999999998</v>
       </c>
       <c r="L37">
-        <v>1218.45</v>
+        <v>1218.453</v>
       </c>
       <c r="M37">
-        <v>13340.6435</v>
+        <v>13340.644</v>
       </c>
       <c r="N37">
         <v>2196.9259999999999</v>
@@ -3580,10 +3580,10 @@
         <v>291.88330000000002</v>
       </c>
       <c r="K38">
-        <v>742.33</v>
+        <v>742.32799999999997</v>
       </c>
       <c r="L38">
-        <v>1210.82</v>
+        <v>1210.8219999999999</v>
       </c>
       <c r="M38">
         <v>13332.331</v>
@@ -3657,10 +3657,10 @@
         <v>292.94799999999998</v>
       </c>
       <c r="K39">
-        <v>743.49</v>
+        <v>743.48900000000003</v>
       </c>
       <c r="L39">
-        <v>1228.3499999999999</v>
+        <v>1228.3489999999999</v>
       </c>
       <c r="M39">
         <v>13557.523999999999</v>
@@ -3734,13 +3734,13 @@
         <v>296.69979999999998</v>
       </c>
       <c r="K40">
-        <v>765.56</v>
+        <v>765.56299999999999</v>
       </c>
       <c r="L40">
-        <v>1211.3499999999999</v>
+        <v>1211.347</v>
       </c>
       <c r="M40">
-        <v>13928.3614</v>
+        <v>13928.361000000001</v>
       </c>
       <c r="N40">
         <v>2339.1849999999999</v>
@@ -3814,10 +3814,10 @@
         <v>784.13</v>
       </c>
       <c r="L41">
-        <v>1223.1099999999999</v>
+        <v>1223.1110000000001</v>
       </c>
       <c r="M41">
-        <v>14239.0774</v>
+        <v>14239.076999999999</v>
       </c>
       <c r="N41">
         <v>2454.8679999999999</v>
@@ -3888,13 +3888,13 @@
         <v>302.4778</v>
       </c>
       <c r="K42">
-        <v>775.38</v>
+        <v>775.38199999999995</v>
       </c>
       <c r="L42">
-        <v>1209.6600000000001</v>
+        <v>1209.6569999999999</v>
       </c>
       <c r="M42">
-        <v>14108.606900000001</v>
+        <v>14108.607</v>
       </c>
       <c r="N42">
         <v>2359.6460000000002</v>
@@ -3965,13 +3965,13 @@
         <v>306.50450000000001</v>
       </c>
       <c r="K43">
-        <v>789.04</v>
+        <v>789.03499999999997</v>
       </c>
       <c r="L43">
-        <v>1225.8800000000001</v>
+        <v>1225.884</v>
       </c>
       <c r="M43">
-        <v>14579.778399999999</v>
+        <v>14579.778</v>
       </c>
       <c r="N43">
         <v>2493.3910000000001</v>
@@ -4042,10 +4042,10 @@
         <v>312.52589999999998</v>
       </c>
       <c r="K44">
-        <v>805.62</v>
+        <v>805.62400000000002</v>
       </c>
       <c r="L44">
-        <v>1227.69</v>
+        <v>1227.6890000000001</v>
       </c>
       <c r="M44">
         <v>14474.621999999999</v>
@@ -4119,13 +4119,13 @@
         <v>314.1893</v>
       </c>
       <c r="K45">
-        <v>816.4</v>
+        <v>816.39499999999998</v>
       </c>
       <c r="L45">
-        <v>1239.1600000000001</v>
+        <v>1239.1569999999999</v>
       </c>
       <c r="M45">
-        <v>14659.216200000001</v>
+        <v>14659.216</v>
       </c>
       <c r="N45">
         <v>2510.5619999999999</v>
@@ -4196,13 +4196,13 @@
         <v>314.62810000000002</v>
       </c>
       <c r="K46">
-        <v>819.83</v>
+        <v>819.82500000000005</v>
       </c>
       <c r="L46">
         <v>1243.9100000000001</v>
       </c>
       <c r="M46">
-        <v>14499.349700000001</v>
+        <v>14499.35</v>
       </c>
       <c r="N46">
         <v>2408.201</v>
@@ -4273,13 +4273,13 @@
         <v>316.52589999999998</v>
       </c>
       <c r="K47">
-        <v>832.29</v>
+        <v>832.28599999999994</v>
       </c>
       <c r="L47">
-        <v>1254.98</v>
+        <v>1254.981</v>
       </c>
       <c r="M47">
-        <v>14843.1054</v>
+        <v>14843.105</v>
       </c>
       <c r="N47">
         <v>2522.3739999999998</v>
@@ -4350,13 +4350,13 @@
         <v>316.71600000000001</v>
       </c>
       <c r="K48">
-        <v>836.36</v>
+        <v>836.35599999999999</v>
       </c>
       <c r="L48">
-        <v>1228.49</v>
+        <v>1228.4880000000001</v>
       </c>
       <c r="M48">
-        <v>14501.493200000001</v>
+        <v>14501.493</v>
       </c>
       <c r="N48">
         <v>2396.038</v>
@@ -4427,10 +4427,10 @@
         <v>315.6814</v>
       </c>
       <c r="K49">
-        <v>827.96</v>
+        <v>827.95500000000004</v>
       </c>
       <c r="L49">
-        <v>1199.6099999999999</v>
+        <v>1199.6089999999999</v>
       </c>
       <c r="M49">
         <v>14249.044</v>
@@ -4504,13 +4504,13 @@
         <v>316.2002</v>
       </c>
       <c r="K50">
-        <v>838.18</v>
+        <v>838.18399999999997</v>
       </c>
       <c r="L50">
-        <v>1214.8</v>
+        <v>1214.798</v>
       </c>
       <c r="M50">
-        <v>14484.9593</v>
+        <v>14484.959000000001</v>
       </c>
       <c r="N50">
         <v>2426.16</v>
@@ -4581,13 +4581,13 @@
         <v>303.04410000000001</v>
       </c>
       <c r="K51">
-        <v>804.6</v>
+        <v>804.59699999999998</v>
       </c>
       <c r="L51">
-        <v>1213.76</v>
+        <v>1213.7570000000001</v>
       </c>
       <c r="M51">
-        <v>14410.909799999999</v>
+        <v>14410.91</v>
       </c>
       <c r="N51">
         <v>2397.636</v>
@@ -4658,13 +4658,13 @@
         <v>303.81540000000001</v>
       </c>
       <c r="K52">
-        <v>775.67</v>
+        <v>775.67399999999998</v>
       </c>
       <c r="L52">
-        <v>1189.42</v>
+        <v>1189.424</v>
       </c>
       <c r="M52">
-        <v>14231.7312</v>
+        <v>14231.731</v>
       </c>
       <c r="N52">
         <v>2371.6529999999998</v>
@@ -4735,10 +4735,10 @@
         <v>311.6925</v>
       </c>
       <c r="K53">
-        <v>821.87</v>
+        <v>821.87099999999998</v>
       </c>
       <c r="L53">
-        <v>1165.81</v>
+        <v>1165.807</v>
       </c>
       <c r="M53">
         <v>14100.214</v>
@@ -4812,13 +4812,13 @@
         <v>310.50479999999999</v>
       </c>
       <c r="K54">
-        <v>803.7</v>
+        <v>803.69500000000005</v>
       </c>
       <c r="L54">
-        <v>1169.33</v>
+        <v>1169.3309999999999</v>
       </c>
       <c r="M54">
-        <v>14008.1811</v>
+        <v>14008.181</v>
       </c>
       <c r="N54">
         <v>2258.2049999999999</v>
@@ -4889,13 +4889,13 @@
         <v>312.07580000000002</v>
       </c>
       <c r="K55">
-        <v>823.62</v>
+        <v>823.61599999999999</v>
       </c>
       <c r="L55">
-        <v>1166.06</v>
+        <v>1166.059</v>
       </c>
       <c r="M55">
-        <v>13973.4763</v>
+        <v>13973.476000000001</v>
       </c>
       <c r="N55">
         <v>2295.5889999999999</v>
@@ -4966,13 +4966,13 @@
         <v>318.30500000000001</v>
       </c>
       <c r="K56">
-        <v>847.53</v>
+        <v>847.52499999999998</v>
       </c>
       <c r="L56">
-        <v>1167.1199999999999</v>
+        <v>1167.1220000000001</v>
       </c>
       <c r="M56">
-        <v>14150.578100000001</v>
+        <v>14150.578</v>
       </c>
       <c r="N56">
         <v>2319.9760000000001</v>
@@ -5043,13 +5043,13 @@
         <v>320.66320000000002</v>
       </c>
       <c r="K57">
-        <v>866.84</v>
+        <v>866.83600000000001</v>
       </c>
       <c r="L57">
-        <v>1169.6400000000001</v>
+        <v>1169.6369999999999</v>
       </c>
       <c r="M57">
-        <v>14262.293900000001</v>
+        <v>14262.294</v>
       </c>
       <c r="N57">
         <v>2355.634</v>
@@ -5120,13 +5120,13 @@
         <v>322.92290000000003</v>
       </c>
       <c r="K58">
-        <v>866.03</v>
+        <v>866.02499999999998</v>
       </c>
       <c r="L58">
-        <v>1150.97</v>
+        <v>1150.973</v>
       </c>
       <c r="M58">
-        <v>14074.2376</v>
+        <v>14074.237999999999</v>
       </c>
       <c r="N58">
         <v>2302.6779999999999</v>
@@ -5197,13 +5197,13 @@
         <v>325.4556</v>
       </c>
       <c r="K59">
-        <v>874.88</v>
+        <v>874.87800000000004</v>
       </c>
       <c r="L59">
-        <v>1155.8900000000001</v>
+        <v>1155.893</v>
       </c>
       <c r="M59">
-        <v>13992.7004</v>
+        <v>13992.7</v>
       </c>
       <c r="N59">
         <v>2319.3290000000002</v>
@@ -5274,13 +5274,13 @@
         <v>323.7833</v>
       </c>
       <c r="K60">
-        <v>864.32</v>
+        <v>864.31600000000003</v>
       </c>
       <c r="L60">
-        <v>1160.04</v>
+        <v>1160.0440000000001</v>
       </c>
       <c r="M60">
-        <v>14049.182500000001</v>
+        <v>14049.183000000001</v>
       </c>
       <c r="N60">
         <v>2387.8009999999999</v>
@@ -5351,13 +5351,13 @@
         <v>326.18639999999999</v>
       </c>
       <c r="K61">
-        <v>881.89</v>
+        <v>881.89400000000001</v>
       </c>
       <c r="L61">
-        <v>1144.99</v>
+        <v>1144.9949999999999</v>
       </c>
       <c r="M61">
-        <v>13849.6605</v>
+        <v>13849.661</v>
       </c>
       <c r="N61">
         <v>2274.5349999999999</v>
@@ -5428,13 +5428,13 @@
         <v>329.36090000000002</v>
       </c>
       <c r="K62">
-        <v>898.79</v>
+        <v>898.79399999999998</v>
       </c>
       <c r="L62">
-        <v>1161.99</v>
+        <v>1161.9860000000001</v>
       </c>
       <c r="M62">
-        <v>14127.8858</v>
+        <v>14127.886</v>
       </c>
       <c r="N62">
         <v>2392.2849999999999</v>
@@ -5505,13 +5505,13 @@
         <v>332.83499999999998</v>
       </c>
       <c r="K63">
-        <v>909.63</v>
+        <v>909.63199999999995</v>
       </c>
       <c r="L63">
-        <v>1161.73</v>
+        <v>1161.7260000000001</v>
       </c>
       <c r="M63">
-        <v>14095.6423</v>
+        <v>14095.642</v>
       </c>
       <c r="N63">
         <v>2344.402</v>
@@ -5582,13 +5582,13 @@
         <v>336.41629999999998</v>
       </c>
       <c r="K64">
-        <v>922.59</v>
+        <v>922.58799999999997</v>
       </c>
       <c r="L64">
-        <v>1155.73</v>
+        <v>1155.731</v>
       </c>
       <c r="M64">
-        <v>14091.388800000001</v>
+        <v>14091.388999999999</v>
       </c>
       <c r="N64">
         <v>2295.8310000000001</v>
@@ -5659,13 +5659,13 @@
         <v>337.67520000000002</v>
       </c>
       <c r="K65">
-        <v>930.2</v>
+        <v>930.197</v>
       </c>
       <c r="L65">
         <v>1143.44</v>
       </c>
       <c r="M65">
-        <v>13832.4846</v>
+        <v>13832.485000000001</v>
       </c>
       <c r="N65">
         <v>2184.299</v>
@@ -5736,13 +5736,13 @@
         <v>339.029</v>
       </c>
       <c r="K66">
-        <v>937.1</v>
+        <v>937.10199999999998</v>
       </c>
       <c r="L66">
-        <v>1146.95</v>
+        <v>1146.953</v>
       </c>
       <c r="M66">
-        <v>13823.5672</v>
+        <v>13823.566999999999</v>
       </c>
       <c r="N66">
         <v>2186.8069999999998</v>
@@ -5813,13 +5813,13 @@
         <v>341.51690000000002</v>
       </c>
       <c r="K67">
-        <v>951.96</v>
+        <v>951.96299999999997</v>
       </c>
       <c r="L67">
-        <v>1154.3599999999999</v>
+        <v>1154.355</v>
       </c>
       <c r="M67">
-        <v>13964.716700000001</v>
+        <v>13964.717000000001</v>
       </c>
       <c r="N67">
         <v>2214.6790000000001</v>
@@ -5967,10 +5967,10 @@
         <v>346.68119999999999</v>
       </c>
       <c r="K69">
-        <v>969.53</v>
+        <v>969.52599999999995</v>
       </c>
       <c r="L69">
-        <v>1154.5</v>
+        <v>1154.5029999999999</v>
       </c>
       <c r="M69">
         <v>14081.665999999999</v>
@@ -6044,13 +6044,13 @@
         <v>349.62169999999998</v>
       </c>
       <c r="K70">
-        <v>979.52</v>
+        <v>979.51800000000003</v>
       </c>
       <c r="L70">
-        <v>1154.83</v>
+        <v>1154.826</v>
       </c>
       <c r="M70">
-        <v>14139.034299999999</v>
+        <v>14139.034</v>
       </c>
       <c r="N70">
         <v>2296.1260000000002</v>
@@ -6121,13 +6121,13 @@
         <v>352.2414</v>
       </c>
       <c r="K71">
-        <v>997.71</v>
+        <v>997.70799999999997</v>
       </c>
       <c r="L71">
-        <v>1160.57</v>
+        <v>1160.5719999999999</v>
       </c>
       <c r="M71">
-        <v>14231.3532</v>
+        <v>14231.352999999999</v>
       </c>
       <c r="N71">
         <v>2384.665</v>
@@ -6198,13 +6198,13 @@
         <v>353.04329999999999</v>
       </c>
       <c r="K72">
-        <v>992.41</v>
+        <v>992.41099999999994</v>
       </c>
       <c r="L72">
-        <v>1149.57</v>
+        <v>1149.5719999999999</v>
       </c>
       <c r="M72">
-        <v>14053.3143</v>
+        <v>14053.314</v>
       </c>
       <c r="N72">
         <v>2297.422</v>
@@ -6275,13 +6275,13 @@
         <v>351.11869999999999</v>
       </c>
       <c r="K73">
-        <v>966.25</v>
+        <v>966.25099999999998</v>
       </c>
       <c r="L73">
-        <v>1141.97</v>
+        <v>1141.9670000000001</v>
       </c>
       <c r="M73">
-        <v>13832.831399999999</v>
+        <v>13832.831</v>
       </c>
       <c r="N73">
         <v>2231.511</v>
@@ -6352,13 +6352,13 @@
         <v>354.86489999999998</v>
       </c>
       <c r="K74">
-        <v>984.42</v>
+        <v>984.42200000000003</v>
       </c>
       <c r="L74">
-        <v>1135.83</v>
+        <v>1135.8340000000001</v>
       </c>
       <c r="M74">
-        <v>13825.0689</v>
+        <v>13825.069</v>
       </c>
       <c r="N74">
         <v>2213.9580000000001</v>
@@ -6429,10 +6429,10 @@
         <v>354.99880000000002</v>
       </c>
       <c r="K75">
-        <v>978.32</v>
+        <v>978.31799999999998</v>
       </c>
       <c r="L75">
-        <v>1126.32</v>
+        <v>1126.316</v>
       </c>
       <c r="M75">
         <v>13675.416999999999</v>
@@ -6506,13 +6506,13 @@
         <v>356.03160000000003</v>
       </c>
       <c r="K76">
-        <v>988.02</v>
+        <v>988.01700000000005</v>
       </c>
       <c r="L76">
-        <v>1123.3499999999999</v>
+        <v>1123.3520000000001</v>
       </c>
       <c r="M76">
-        <v>13652.6752</v>
+        <v>13652.674999999999</v>
       </c>
       <c r="N76">
         <v>2145.154</v>
@@ -6583,13 +6583,13 @@
         <v>358.88979999999998</v>
       </c>
       <c r="K77">
-        <v>1012.31</v>
+        <v>1012.3049999999999</v>
       </c>
       <c r="L77">
-        <v>1130.57</v>
+        <v>1130.566</v>
       </c>
       <c r="M77">
-        <v>13765.9161</v>
+        <v>13765.915999999999</v>
       </c>
       <c r="N77">
         <v>2199.8159999999998</v>
@@ -6660,13 +6660,13 @@
         <v>360.60160000000002</v>
       </c>
       <c r="K78">
-        <v>1017.01</v>
+        <v>1017.013</v>
       </c>
       <c r="L78">
-        <v>1134.19</v>
+        <v>1134.1869999999999</v>
       </c>
       <c r="M78">
-        <v>13838.021500000001</v>
+        <v>13838.022000000001</v>
       </c>
       <c r="N78">
         <v>2259.2640000000001</v>
@@ -6737,13 +6737,13 @@
         <v>362.5283</v>
       </c>
       <c r="K79">
-        <v>1022.59</v>
+        <v>1022.586</v>
       </c>
       <c r="L79">
-        <v>1133.6600000000001</v>
+        <v>1133.6610000000001</v>
       </c>
       <c r="M79">
-        <v>13903.1242</v>
+        <v>13903.124</v>
       </c>
       <c r="N79">
         <v>2273.8609999999999</v>
@@ -6814,13 +6814,13 @@
         <v>365.08629999999999</v>
       </c>
       <c r="K80">
-        <v>1030.1500000000001</v>
+        <v>1030.1510000000001</v>
       </c>
       <c r="L80">
         <v>1132.8900000000001</v>
       </c>
       <c r="M80">
-        <v>13784.743899999999</v>
+        <v>13784.744000000001</v>
       </c>
       <c r="N80">
         <v>2171.3519999999999</v>
@@ -6891,13 +6891,13 @@
         <v>365.90249999999997</v>
       </c>
       <c r="K81">
-        <v>1050.8</v>
+        <v>1050.797</v>
       </c>
       <c r="L81">
         <v>1124.3699999999999</v>
       </c>
       <c r="M81">
-        <v>13983.1011</v>
+        <v>13983.101000000001</v>
       </c>
       <c r="N81">
         <v>2185.3049999999998</v>
@@ -6968,13 +6968,13 @@
         <v>367.24169999999998</v>
       </c>
       <c r="K82">
-        <v>1053.23</v>
+        <v>1053.229</v>
       </c>
       <c r="L82">
         <v>1121.8599999999999</v>
       </c>
       <c r="M82">
-        <v>13857.130499999999</v>
+        <v>13857.130999999999</v>
       </c>
       <c r="N82">
         <v>2139.87</v>
@@ -7045,13 +7045,13 @@
         <v>368.08049999999997</v>
       </c>
       <c r="K83">
-        <v>1060.53</v>
+        <v>1060.5250000000001</v>
       </c>
       <c r="L83">
         <v>1115.6099999999999</v>
       </c>
       <c r="M83">
-        <v>13865.789500000001</v>
+        <v>13865.79</v>
       </c>
       <c r="N83">
         <v>2162.9859999999999</v>
@@ -7122,13 +7122,13 @@
         <v>370.34370000000001</v>
       </c>
       <c r="K84">
-        <v>1071.2</v>
+        <v>1071.203</v>
       </c>
       <c r="L84">
         <v>1124.43</v>
       </c>
       <c r="M84">
-        <v>13944.688599999999</v>
+        <v>13944.689</v>
       </c>
       <c r="N84">
         <v>2227.085</v>
@@ -7199,13 +7199,13 @@
         <v>372.57870000000003</v>
       </c>
       <c r="K85">
-        <v>1080.26</v>
+        <v>1080.2560000000001</v>
       </c>
       <c r="L85">
         <v>1125.3599999999999</v>
       </c>
       <c r="M85">
-        <v>14041.676299999999</v>
+        <v>14041.675999999999</v>
       </c>
       <c r="N85">
         <v>2258.1</v>
@@ -7276,13 +7276,13 @@
         <v>372.416</v>
       </c>
       <c r="K86">
-        <v>1065.97</v>
+        <v>1065.971</v>
       </c>
       <c r="L86">
         <v>1131.24</v>
       </c>
       <c r="M86">
-        <v>13986.182199999999</v>
+        <v>13986.182000000001</v>
       </c>
       <c r="N86">
         <v>2234.0169999999998</v>
@@ -7353,13 +7353,13 @@
         <v>373.2801</v>
       </c>
       <c r="K87">
-        <v>1082.17</v>
+        <v>1082.174</v>
       </c>
       <c r="L87">
         <v>1144.9000000000001</v>
       </c>
       <c r="M87">
-        <v>14195.9997</v>
+        <v>14196</v>
       </c>
       <c r="N87">
         <v>2357.018</v>
@@ -7430,13 +7430,13 @@
         <v>371.35480000000001</v>
       </c>
       <c r="K88">
-        <v>1059.47</v>
+        <v>1059.4670000000001</v>
       </c>
       <c r="L88">
         <v>1162.53</v>
       </c>
       <c r="M88">
-        <v>14349.293299999999</v>
+        <v>14349.293</v>
       </c>
       <c r="N88">
         <v>2435.6019999999999</v>
@@ -7507,13 +7507,13 @@
         <v>372.41359999999997</v>
       </c>
       <c r="K89">
-        <v>1071.53</v>
+        <v>1071.528</v>
       </c>
       <c r="L89">
         <v>1169.58</v>
       </c>
       <c r="M89">
-        <v>14320.528399999999</v>
+        <v>14320.528</v>
       </c>
       <c r="N89">
         <v>2478.6019999999999</v>
@@ -7584,13 +7584,13 @@
         <v>374.10939999999999</v>
       </c>
       <c r="K90">
-        <v>1063.8699999999999</v>
+        <v>1063.8689999999999</v>
       </c>
       <c r="L90">
         <v>1189.05</v>
       </c>
       <c r="M90">
-        <v>14642.9534</v>
+        <v>14642.953</v>
       </c>
       <c r="N90">
         <v>2659.299</v>
@@ -7661,13 +7661,13 @@
         <v>369.9796</v>
       </c>
       <c r="K91">
-        <v>1048.18</v>
+        <v>1048.184</v>
       </c>
       <c r="L91">
         <v>1193.05</v>
       </c>
       <c r="M91">
-        <v>14678.342500000001</v>
+        <v>14678.343000000001</v>
       </c>
       <c r="N91">
         <v>2721.7869999999998</v>
@@ -7738,13 +7738,13 @@
         <v>370.92840000000001</v>
       </c>
       <c r="K92">
-        <v>1055.4100000000001</v>
+        <v>1055.413</v>
       </c>
       <c r="L92">
         <v>1216.8399999999999</v>
       </c>
       <c r="M92">
-        <v>15047.019700000001</v>
+        <v>15047.02</v>
       </c>
       <c r="N92">
         <v>2861.0079999999998</v>
@@ -7815,13 +7815,13 @@
         <v>376.14550000000003</v>
       </c>
       <c r="K93">
-        <v>1080.5899999999999</v>
+        <v>1080.5930000000001</v>
       </c>
       <c r="L93">
         <v>1224.99</v>
       </c>
       <c r="M93">
-        <v>15076.506100000001</v>
+        <v>15076.505999999999</v>
       </c>
       <c r="N93">
         <v>2855.143</v>
@@ -7892,13 +7892,13 @@
         <v>377.6302</v>
       </c>
       <c r="K94">
-        <v>1074.8499999999999</v>
+        <v>1074.8530000000001</v>
       </c>
       <c r="L94">
         <v>1233.6400000000001</v>
       </c>
       <c r="M94">
-        <v>15161.163200000001</v>
+        <v>15161.163</v>
       </c>
       <c r="N94">
         <v>2929.2930000000001</v>
@@ -8046,13 +8046,13 @@
         <v>381.7903</v>
       </c>
       <c r="K96">
-        <v>1090.96</v>
+        <v>1090.962</v>
       </c>
       <c r="L96">
         <v>1209.01</v>
       </c>
       <c r="M96">
-        <v>14972.890299999999</v>
+        <v>14972.89</v>
       </c>
       <c r="N96">
         <v>2789.703</v>
@@ -8123,13 +8123,13 @@
         <v>380.59679999999997</v>
       </c>
       <c r="K97">
-        <v>1074.32</v>
+        <v>1074.3209999999999</v>
       </c>
       <c r="L97">
         <v>1176.9000000000001</v>
       </c>
       <c r="M97">
-        <v>14626.769899999999</v>
+        <v>14626.77</v>
       </c>
       <c r="N97">
         <v>2654.02</v>
@@ -8200,13 +8200,13 @@
         <v>380.9366</v>
       </c>
       <c r="K98">
-        <v>1067.71</v>
+        <v>1067.7070000000001</v>
       </c>
       <c r="L98">
         <v>1204.1199999999999</v>
       </c>
       <c r="M98">
-        <v>14757.0355</v>
+        <v>14757.036</v>
       </c>
       <c r="N98">
         <v>2760.348</v>
@@ -8277,13 +8277,13 @@
         <v>378.45819999999998</v>
       </c>
       <c r="K99">
-        <v>1048.9000000000001</v>
+        <v>1048.903</v>
       </c>
       <c r="L99">
         <v>1181.02</v>
       </c>
       <c r="M99">
-        <v>14520.1258</v>
+        <v>14520.126</v>
       </c>
       <c r="N99">
         <v>2701.4830000000002</v>
@@ -8354,13 +8354,13 @@
         <v>375.935</v>
       </c>
       <c r="K100">
-        <v>1021.69</v>
+        <v>1021.693</v>
       </c>
       <c r="L100">
         <v>1174.48</v>
       </c>
       <c r="M100">
-        <v>14513.8194</v>
+        <v>14513.819</v>
       </c>
       <c r="N100">
         <v>2763.31</v>
@@ -8431,13 +8431,13 @@
         <v>375.42520000000002</v>
       </c>
       <c r="K101">
-        <v>1049.54</v>
+        <v>1049.5440000000001</v>
       </c>
       <c r="L101">
         <v>1163.3900000000001</v>
       </c>
       <c r="M101">
-        <v>14501.5378</v>
+        <v>14501.538</v>
       </c>
       <c r="N101">
         <v>2691.3589999999999</v>
@@ -8508,7 +8508,7 @@
         <v>372.08960000000002</v>
       </c>
       <c r="K102">
-        <v>1025.98</v>
+        <v>1025.982</v>
       </c>
       <c r="L102">
         <v>1186.28</v>
@@ -8585,7 +8585,7 @@
         <v>368.55599999999998</v>
       </c>
       <c r="K103">
-        <v>999.52</v>
+        <v>999.51700000000005</v>
       </c>
       <c r="L103">
         <v>1169.6199999999999</v>
@@ -8662,7 +8662,7 @@
         <v>365.88080000000002</v>
       </c>
       <c r="K104">
-        <v>983.71</v>
+        <v>983.70799999999997</v>
       </c>
       <c r="L104">
         <v>1180.24</v>
@@ -8739,7 +8739,7 @@
         <v>363.84429999999998</v>
       </c>
       <c r="K105">
-        <v>988.28</v>
+        <v>988.28300000000002</v>
       </c>
       <c r="L105">
         <v>1183.75</v>
@@ -8816,7 +8816,7 @@
         <v>373.45389999999998</v>
       </c>
       <c r="K106">
-        <v>1031.97</v>
+        <v>1031.9690000000001</v>
       </c>
       <c r="L106">
         <v>1170.55</v>
@@ -8893,7 +8893,7 @@
         <v>380.5421</v>
       </c>
       <c r="K107">
-        <v>1073.2</v>
+        <v>1073.204</v>
       </c>
       <c r="L107">
         <v>1174.4100000000001</v>
@@ -8970,7 +8970,7 @@
         <v>384.01139999999998</v>
       </c>
       <c r="K108">
-        <v>1080.95</v>
+        <v>1080.9480000000001</v>
       </c>
       <c r="L108">
         <v>1154.26</v>
@@ -9047,7 +9047,7 @@
         <v>384.13850000000002</v>
       </c>
       <c r="K109">
-        <v>1092.6600000000001</v>
+        <v>1092.664</v>
       </c>
       <c r="L109">
         <v>1165.76</v>
@@ -9124,7 +9124,7 @@
         <v>389.53660000000002</v>
       </c>
       <c r="K110">
-        <v>1120.26</v>
+        <v>1120.2619999999999</v>
       </c>
       <c r="L110">
         <v>1169.28</v>
@@ -9201,7 +9201,7 @@
         <v>392.6105</v>
       </c>
       <c r="K111">
-        <v>1145.21</v>
+        <v>1145.2149999999999</v>
       </c>
       <c r="L111">
         <v>1157.81</v>
@@ -9278,7 +9278,7 @@
         <v>396.03949999999998</v>
       </c>
       <c r="K112">
-        <v>1152.6199999999999</v>
+        <v>1152.624</v>
       </c>
       <c r="L112">
         <v>1156.1199999999999</v>
@@ -9355,7 +9355,7 @@
         <v>399.08030000000002</v>
       </c>
       <c r="K113">
-        <v>1156.23</v>
+        <v>1156.2260000000001</v>
       </c>
       <c r="L113">
         <v>1137.8</v>
@@ -9432,7 +9432,7 @@
         <v>400.37619999999998</v>
       </c>
       <c r="K114">
-        <v>1151.67</v>
+        <v>1151.6659999999999</v>
       </c>
       <c r="L114">
         <v>1129.95</v>
@@ -9509,7 +9509,7 @@
         <v>404.9606</v>
       </c>
       <c r="K115">
-        <v>1174.32</v>
+        <v>1174.319</v>
       </c>
       <c r="L115">
         <v>1135.3599999999999</v>
@@ -9586,7 +9586,7 @@
         <v>407.12240000000003</v>
       </c>
       <c r="K116">
-        <v>1190.0899999999999</v>
+        <v>1190.088</v>
       </c>
       <c r="L116">
         <v>1124.55</v>
@@ -9663,7 +9663,7 @@
         <v>409.50909999999999</v>
       </c>
       <c r="K117">
-        <v>1208.6600000000001</v>
+        <v>1208.6590000000001</v>
       </c>
       <c r="L117">
         <v>1137.81</v>
@@ -9740,7 +9740,7 @@
         <v>409.8263</v>
       </c>
       <c r="K118">
-        <v>1206.1199999999999</v>
+        <v>1206.123</v>
       </c>
       <c r="L118">
         <v>1126.77</v>
@@ -9817,7 +9817,7 @@
         <v>411.61130000000003</v>
       </c>
       <c r="K119">
-        <v>1219.79</v>
+        <v>1219.789</v>
       </c>
       <c r="L119">
         <v>1126.01</v>
@@ -9894,7 +9894,7 @@
         <v>413.17660000000001</v>
       </c>
       <c r="K120">
-        <v>1230.68</v>
+        <v>1230.684</v>
       </c>
       <c r="L120">
         <v>1131.48</v>
@@ -9971,7 +9971,7 @@
         <v>412.91320000000002</v>
       </c>
       <c r="K121">
-        <v>1231.98</v>
+        <v>1231.9829999999999</v>
       </c>
       <c r="L121">
         <v>1126.83</v>
@@ -10048,7 +10048,7 @@
         <v>416.14530000000002</v>
       </c>
       <c r="K122">
-        <v>1246.19</v>
+        <v>1246.193</v>
       </c>
       <c r="L122">
         <v>1137.44</v>
@@ -10202,7 +10202,7 @@
         <v>417.27420000000001</v>
       </c>
       <c r="K124">
-        <v>1257.06</v>
+        <v>1257.0630000000001</v>
       </c>
       <c r="L124">
         <v>1134.28</v>
@@ -10279,7 +10279,7 @@
         <v>420.03120000000001</v>
       </c>
       <c r="K125">
-        <v>1261.9100000000001</v>
+        <v>1261.914</v>
       </c>
       <c r="L125">
         <v>1156.0899999999999</v>
@@ -10356,7 +10356,7 @@
         <v>420.53440000000001</v>
       </c>
       <c r="K126">
-        <v>1258.53</v>
+        <v>1258.528</v>
       </c>
       <c r="L126">
         <v>1154.3499999999999</v>
@@ -10433,7 +10433,7 @@
         <v>422.16019999999997</v>
       </c>
       <c r="K127">
-        <v>1262.2</v>
+        <v>1262.1959999999999</v>
       </c>
       <c r="L127">
         <v>1163.8699999999999</v>
@@ -10510,7 +10510,7 @@
         <v>426.71300000000002</v>
       </c>
       <c r="K128">
-        <v>1270.29</v>
+        <v>1270.289</v>
       </c>
       <c r="L128">
         <v>1208.0999999999999</v>
@@ -10587,7 +10587,7 @@
         <v>427.47710000000001</v>
       </c>
       <c r="K129">
-        <v>1258.45</v>
+        <v>1258.4459999999999</v>
       </c>
       <c r="L129">
         <v>1149.3900000000001</v>
@@ -10664,7 +10664,7 @@
         <v>428.83859999999999</v>
       </c>
       <c r="K130">
-        <v>1250.68</v>
+        <v>1250.6769999999999</v>
       </c>
       <c r="L130">
         <v>1140.28</v>
@@ -10741,7 +10741,7 @@
         <v>430.92849999999999</v>
       </c>
       <c r="K131">
-        <v>1259</v>
+        <v>1258.9960000000001</v>
       </c>
       <c r="L131">
         <v>1145.54</v>
@@ -10818,7 +10818,7 @@
         <v>431.76209999999998</v>
       </c>
       <c r="K132">
-        <v>1258.81</v>
+        <v>1258.806</v>
       </c>
       <c r="L132">
         <v>1141.3699999999999</v>
@@ -10895,7 +10895,7 @@
         <v>432.1986</v>
       </c>
       <c r="K133">
-        <v>1263.1500000000001</v>
+        <v>1263.153</v>
       </c>
       <c r="L133">
         <v>1142.77</v>
@@ -10972,7 +10972,7 @@
         <v>435.77850000000001</v>
       </c>
       <c r="K134">
-        <v>1277.27</v>
+        <v>1277.268</v>
       </c>
       <c r="L134">
         <v>1130.1600000000001</v>
@@ -11049,7 +11049,7 @@
         <v>437.56849999999997</v>
       </c>
       <c r="K135">
-        <v>1286.52</v>
+        <v>1286.518</v>
       </c>
       <c r="L135">
         <v>1157.3699999999999</v>
@@ -11126,7 +11126,7 @@
         <v>440.55239999999998</v>
       </c>
       <c r="K136">
-        <v>1293.99</v>
+        <v>1293.9939999999999</v>
       </c>
       <c r="L136">
         <v>1150.1099999999999</v>
@@ -11203,7 +11203,7 @@
         <v>440.57920000000001</v>
       </c>
       <c r="K137">
-        <v>1272.8</v>
+        <v>1272.8030000000001</v>
       </c>
       <c r="L137">
         <v>1119.6300000000001</v>
@@ -11280,7 +11280,7 @@
         <v>436.98590000000002</v>
       </c>
       <c r="K138">
-        <v>1261.25</v>
+        <v>1261.2529999999999</v>
       </c>
       <c r="L138">
         <v>1117.54</v>
@@ -11357,7 +11357,7 @@
         <v>426.97919999999999</v>
       </c>
       <c r="K139">
-        <v>1233.6099999999999</v>
+        <v>1233.6079999999999</v>
       </c>
       <c r="L139">
         <v>1126.0899999999999</v>
@@ -11434,7 +11434,7 @@
         <v>436.80489999999998</v>
       </c>
       <c r="K140">
-        <v>1290.27</v>
+        <v>1290.2670000000001</v>
       </c>
       <c r="L140">
         <v>1104.58</v>
@@ -11511,7 +11511,7 @@
         <v>443.65249999999997</v>
       </c>
       <c r="K141">
-        <v>1312.05</v>
+        <v>1312.0530000000001</v>
       </c>
       <c r="L141">
         <v>1112.99</v>
@@ -11588,10 +11588,10 @@
         <v>443.11380000000003</v>
       </c>
       <c r="K142">
-        <v>1324.91</v>
+        <v>1324.9090000000001</v>
       </c>
       <c r="L142">
-        <v>1116.33</v>
+        <v>1116.328</v>
       </c>
       <c r="M142">
         <v>14681.66</v>
@@ -11630,7 +11630,7 @@
         <v>392.83</v>
       </c>
       <c r="Y142">
-        <v>1064.01</v>
+        <v>1064.0050000000001</v>
       </c>
     </row>
     <row r="143" spans="1:25" x14ac:dyDescent="0.25">
@@ -11665,10 +11665,10 @@
         <v>450.14179999999999</v>
       </c>
       <c r="K143">
-        <v>1343.45</v>
+        <v>1343.4449999999999</v>
       </c>
       <c r="L143">
-        <v>1129.1300000000001</v>
+        <v>1129.1289999999999</v>
       </c>
       <c r="M143">
         <v>14836.621999999999</v>
@@ -11707,7 +11707,7 @@
         <v>387.91</v>
       </c>
       <c r="Y143">
-        <v>1067.04</v>
+        <v>1067.0419999999999</v>
       </c>
     </row>
     <row r="144" spans="1:25" x14ac:dyDescent="0.25">
@@ -11742,10 +11742,10 @@
         <v>449.12759999999997</v>
       </c>
       <c r="K144">
-        <v>1326.37</v>
+        <v>1326.3689999999999</v>
       </c>
       <c r="L144">
-        <v>1126.0899999999999</v>
+        <v>1126.0940000000001</v>
       </c>
       <c r="M144">
         <v>14707.329</v>
@@ -11784,7 +11784,7 @@
         <v>406.85</v>
       </c>
       <c r="Y144">
-        <v>1067.57</v>
+        <v>1067.566</v>
       </c>
     </row>
     <row r="145" spans="1:25" x14ac:dyDescent="0.25">
@@ -11819,7 +11819,7 @@
         <v>450.11630000000002</v>
       </c>
       <c r="K145">
-        <v>1358.89</v>
+        <v>1358.893</v>
       </c>
       <c r="L145">
         <v>1155.1099999999999</v>
@@ -11896,7 +11896,7 @@
         <v>453.63990000000001</v>
       </c>
       <c r="K146">
-        <v>1365.85</v>
+        <v>1365.8510000000001</v>
       </c>
       <c r="L146">
         <v>1176.26</v>
@@ -11973,7 +11973,7 @@
         <v>452.3603</v>
       </c>
       <c r="K147">
-        <v>1371.18</v>
+        <v>1371.181</v>
       </c>
       <c r="L147">
         <v>1195.94</v>
@@ -12050,7 +12050,7 @@
         <v>454.2679</v>
       </c>
       <c r="K148">
-        <v>1375.53</v>
+        <v>1375.528</v>
       </c>
       <c r="L148">
         <v>1183.01</v>
@@ -12127,7 +12127,7 @@
         <v>452.06330000000003</v>
       </c>
       <c r="K149">
-        <v>1378.72</v>
+        <v>1378.722</v>
       </c>
       <c r="L149">
         <v>1166.43</v>
@@ -12204,7 +12204,7 @@
         <v>454.55160000000001</v>
       </c>
       <c r="K150">
-        <v>1382.49</v>
+        <v>1382.4870000000001</v>
       </c>
       <c r="L150">
         <v>1177.05</v>
@@ -12281,7 +12281,7 @@
         <v>461.8843</v>
       </c>
       <c r="K151">
-        <v>1411.39</v>
+        <v>1411.3869999999999</v>
       </c>
       <c r="L151">
         <v>1180.6199999999999</v>
@@ -12358,7 +12358,7 @@
         <v>464.33879999999999</v>
       </c>
       <c r="K152">
-        <v>1411.45</v>
+        <v>1411.4469999999999</v>
       </c>
       <c r="L152">
         <v>1190.33</v>
@@ -12435,7 +12435,7 @@
         <v>458.06479999999999</v>
       </c>
       <c r="K153">
-        <v>1389.57</v>
+        <v>1389.5709999999999</v>
       </c>
       <c r="L153">
         <v>1176.22</v>
@@ -12512,7 +12512,7 @@
         <v>400.9701</v>
       </c>
       <c r="K154">
-        <v>1226.17</v>
+        <v>1226.174</v>
       </c>
       <c r="L154">
         <v>1166.67</v>
@@ -12589,7 +12589,7 @@
         <v>418.16950000000003</v>
       </c>
       <c r="K155">
-        <v>1272.77</v>
+        <v>1272.7729999999999</v>
       </c>
       <c r="L155">
         <v>1172.4100000000001</v>
@@ -12666,7 +12666,7 @@
         <v>434.06650000000002</v>
       </c>
       <c r="K156">
-        <v>1330.99</v>
+        <v>1330.9849999999999</v>
       </c>
       <c r="L156">
         <v>1175.5</v>
@@ -12743,7 +12743,7 @@
         <v>439.91300000000001</v>
       </c>
       <c r="K157">
-        <v>1343.96</v>
+        <v>1343.9580000000001</v>
       </c>
       <c r="L157">
         <v>1172.0999999999999</v>
@@ -12820,7 +12820,7 @@
         <v>448.18779999999998</v>
       </c>
       <c r="K158">
-        <v>1408.17</v>
+        <v>1408.173</v>
       </c>
       <c r="L158">
         <v>1192.95</v>
@@ -12974,7 +12974,7 @@
         <v>458.06110000000001</v>
       </c>
       <c r="K160">
-        <v>1407.21</v>
+        <v>1407.2059999999999</v>
       </c>
       <c r="L160">
         <v>1181.9000000000001</v>
@@ -13051,7 +13051,7 @@
         <v>458.85820000000001</v>
       </c>
       <c r="K161">
-        <v>1413.79</v>
+        <v>1413.7860000000001</v>
       </c>
       <c r="L161">
         <v>1175.82</v>
@@ -13128,7 +13128,7 @@
         <v>468.62920000000003</v>
       </c>
       <c r="K162">
-        <v>1470.38</v>
+        <v>1470.376</v>
       </c>
       <c r="L162">
         <v>1195.79</v>
@@ -13205,7 +13205,7 @@
         <v>474.71800000000002</v>
       </c>
       <c r="K163">
-        <v>1498.42</v>
+        <v>1498.421</v>
       </c>
       <c r="L163">
         <v>1231.32</v>
@@ -13282,7 +13282,7 @@
         <v>480.7278</v>
       </c>
       <c r="K164">
-        <v>1504.16</v>
+        <v>1504.1559999999999</v>
       </c>
       <c r="L164">
         <v>1224.18</v>
@@ -13359,7 +13359,7 @@
         <v>483.96280000000002</v>
       </c>
       <c r="K165">
-        <v>1509.4</v>
+        <v>1509.3969999999999</v>
       </c>
       <c r="L165">
         <v>1240.02</v>
@@ -13436,7 +13436,7 @@
         <v>484.25209999999998</v>
       </c>
       <c r="K166">
-        <v>1511.97</v>
+        <v>1511.9670000000001</v>
       </c>
       <c r="L166">
         <v>1237.72</v>
@@ -13513,7 +13513,7 @@
         <v>486.71570000000003</v>
       </c>
       <c r="K167">
-        <v>1528.55</v>
+        <v>1528.5519999999999</v>
       </c>
       <c r="L167">
         <v>1251.33</v>
@@ -13590,7 +13590,7 @@
         <v>489.24040000000002</v>
       </c>
       <c r="K168">
-        <v>1532.96</v>
+        <v>1532.9639999999999</v>
       </c>
       <c r="L168">
         <v>1258.02</v>
@@ -13667,7 +13667,7 @@
         <v>491.24099999999999</v>
       </c>
       <c r="K169">
-        <v>1553.91</v>
+        <v>1553.9090000000001</v>
       </c>
       <c r="L169">
         <v>1250.5</v>
@@ -13821,7 +13821,7 @@
         <v>493.61149999999998</v>
       </c>
       <c r="K171">
-        <v>1567.95</v>
+        <v>1567.9449999999999</v>
       </c>
       <c r="L171">
         <v>1247.31</v>
@@ -13898,7 +13898,7 @@
         <v>496.8091</v>
       </c>
       <c r="K172">
-        <v>1568.47</v>
+        <v>1568.471</v>
       </c>
       <c r="L172">
         <v>1231.8599999999999</v>
@@ -13975,7 +13975,7 @@
         <v>497.9812</v>
       </c>
       <c r="K173">
-        <v>1565.68</v>
+        <v>1565.681</v>
       </c>
       <c r="L173">
         <v>1244.81</v>
@@ -14052,7 +14052,7 @@
         <v>497.22050000000002</v>
       </c>
       <c r="K174">
-        <v>1549.64</v>
+        <v>1549.636</v>
       </c>
       <c r="L174">
         <v>1210.92</v>
@@ -14283,7 +14283,7 @@
         <v>499.65269999999998</v>
       </c>
       <c r="K177">
-        <v>1521.6</v>
+        <v>1521.604</v>
       </c>
       <c r="L177">
         <v>1194.8599999999999</v>
@@ -14360,7 +14360,7 @@
         <v>499.84949999999998</v>
       </c>
       <c r="K178">
-        <v>1507.53</v>
+        <v>1507.5250000000001</v>
       </c>
       <c r="L178">
         <v>1231.8699999999999</v>
@@ -14437,7 +14437,7 @@
         <v>500.70659999999998</v>
       </c>
       <c r="K179">
-        <v>1452.69</v>
+        <v>1452.6869999999999</v>
       </c>
       <c r="L179">
         <v>1255.32</v>
@@ -14514,7 +14514,7 @@
         <v>488.13490000000002</v>
       </c>
       <c r="K180">
-        <v>1456.32</v>
+        <v>1456.3240000000001</v>
       </c>
       <c r="L180">
         <v>1243.99</v>
@@ -14591,7 +14591,7 @@
         <v>478.0942</v>
       </c>
       <c r="K181">
-        <v>1357.2</v>
+        <v>1357.1969999999999</v>
       </c>
       <c r="L181">
         <v>1261.07</v>
@@ -14745,7 +14745,7 @@
         <v>494.48860000000002</v>
       </c>
       <c r="K183">
-        <v>1404.48</v>
+        <v>1404.481</v>
       </c>
       <c r="L183">
         <v>1257.82</v>
@@ -14822,7 +14822,7 @@
         <v>483.77879999999999</v>
       </c>
       <c r="K184">
-        <v>1348</v>
+        <v>1347.9949999999999</v>
       </c>
       <c r="L184">
         <v>1295.3699999999999</v>
@@ -14899,7 +14899,7 @@
         <v>487.8895</v>
       </c>
       <c r="K185">
-        <v>1386.37</v>
+        <v>1386.3679999999999</v>
       </c>
       <c r="L185">
         <v>1297.27</v>
@@ -15053,7 +15053,7 @@
         <v>495.06270000000001</v>
       </c>
       <c r="K187">
-        <v>1401.68</v>
+        <v>1401.683</v>
       </c>
       <c r="L187">
         <v>1266.8900000000001</v>
@@ -15080,7 +15080,7 @@
         <v>4.3983636739999996</v>
       </c>
       <c r="T187">
-        <v>4976.87</v>
+        <v>5079.05</v>
       </c>
       <c r="U187">
         <v>1536.73</v>
@@ -15130,13 +15130,13 @@
         <v>507.7645</v>
       </c>
       <c r="K188">
-        <v>1456.48</v>
+        <v>1456.4829999999999</v>
       </c>
       <c r="L188">
         <v>1267.28</v>
       </c>
       <c r="M188">
-        <v>18959.123</v>
+        <v>18975.955000000002</v>
       </c>
       <c r="N188">
         <v>3817.4569999999999</v>
@@ -15157,7 +15157,7 @@
         <v>4.6489987660000001</v>
       </c>
       <c r="T188">
-        <v>4976.87</v>
+        <v>5079.05</v>
       </c>
       <c r="U188">
         <v>1648.91</v>
@@ -15173,6 +15173,545 @@
       </c>
       <c r="Y188">
         <v>1168.94</v>
+      </c>
+    </row>
+    <row r="189" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A189" s="1">
+        <v>44985</v>
+      </c>
+      <c r="B189">
+        <v>136.36000000000001</v>
+      </c>
+      <c r="C189">
+        <v>3934.93</v>
+      </c>
+      <c r="D189">
+        <v>168.9444</v>
+      </c>
+      <c r="E189">
+        <v>3970.15</v>
+      </c>
+      <c r="F189">
+        <v>629.02</v>
+      </c>
+      <c r="G189">
+        <v>1896.991</v>
+      </c>
+      <c r="H189">
+        <v>2053.69</v>
+      </c>
+      <c r="I189">
+        <v>964.01</v>
+      </c>
+      <c r="J189">
+        <v>510.96210000000002</v>
+      </c>
+      <c r="K189">
+        <v>1437.635</v>
+      </c>
+      <c r="L189">
+        <v>1273.56</v>
+      </c>
+      <c r="M189">
+        <v>18958.985000000001</v>
+      </c>
+      <c r="N189">
+        <v>3888.33</v>
+      </c>
+      <c r="O189">
+        <v>1718.69</v>
+      </c>
+      <c r="P189">
+        <v>382.53</v>
+      </c>
+      <c r="Q189">
+        <v>162.4709</v>
+      </c>
+      <c r="R189">
+        <v>4.67272</v>
+      </c>
+      <c r="S189">
+        <v>4.8077261</v>
+      </c>
+      <c r="T189">
+        <v>5079.05</v>
+      </c>
+      <c r="U189">
+        <v>1601.19</v>
+      </c>
+      <c r="V189">
+        <v>2308.3960000000002</v>
+      </c>
+      <c r="W189">
+        <v>134.5625</v>
+      </c>
+      <c r="X189">
+        <v>366.54</v>
+      </c>
+      <c r="Y189">
+        <v>1166.95</v>
+      </c>
+    </row>
+    <row r="190" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A190" s="1">
+        <v>45016</v>
+      </c>
+      <c r="B190">
+        <v>143.85</v>
+      </c>
+      <c r="C190">
+        <v>4104.91</v>
+      </c>
+      <c r="D190">
+        <v>176.52780000000001</v>
+      </c>
+      <c r="E190">
+        <v>4109.3100000000004</v>
+      </c>
+      <c r="F190">
+        <v>646.76</v>
+      </c>
+      <c r="G190">
+        <v>1802.4839999999999</v>
+      </c>
+      <c r="H190">
+        <v>2092.6</v>
+      </c>
+      <c r="I190">
+        <v>990.28</v>
+      </c>
+      <c r="J190">
+        <v>510.464</v>
+      </c>
+      <c r="K190">
+        <v>1453.818</v>
+      </c>
+      <c r="L190">
+        <v>1235.1600000000001</v>
+      </c>
+      <c r="M190">
+        <v>18448.667000000001</v>
+      </c>
+      <c r="N190">
+        <v>3587.8829999999998</v>
+      </c>
+      <c r="O190">
+        <v>1718.69</v>
+      </c>
+      <c r="P190">
+        <v>373.22</v>
+      </c>
+      <c r="Q190">
+        <v>162.4709</v>
+      </c>
+      <c r="R190">
+        <v>4.6408199999999997</v>
+      </c>
+      <c r="S190">
+        <v>4.7309068339999998</v>
+      </c>
+      <c r="T190">
+        <v>5215.8100000000004</v>
+      </c>
+      <c r="U190">
+        <v>1636.36</v>
+      </c>
+      <c r="V190">
+        <v>2366.27</v>
+      </c>
+      <c r="W190">
+        <v>141.125</v>
+      </c>
+      <c r="X190">
+        <v>385.5</v>
+      </c>
+      <c r="Y190">
+        <v>1165.6300000000001</v>
+      </c>
+    </row>
+    <row r="191" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A191" s="1">
+        <v>45044</v>
+      </c>
+      <c r="B191">
+        <v>144.24</v>
+      </c>
+      <c r="C191">
+        <v>4135.75</v>
+      </c>
+      <c r="D191">
+        <v>176.87960000000001</v>
+      </c>
+      <c r="E191">
+        <v>4169.4799999999996</v>
+      </c>
+      <c r="F191">
+        <v>655</v>
+      </c>
+      <c r="G191">
+        <v>1768.9870000000001</v>
+      </c>
+      <c r="H191">
+        <v>2143.85</v>
+      </c>
+      <c r="I191">
+        <v>977.05</v>
+      </c>
+      <c r="J191">
+        <v>515.30060000000003</v>
+      </c>
+      <c r="K191">
+        <v>1467.85</v>
+      </c>
+      <c r="L191">
+        <v>1252.01</v>
+      </c>
+      <c r="M191">
+        <v>18601.562999999998</v>
+      </c>
+      <c r="N191">
+        <v>3691.1089999999999</v>
+      </c>
+      <c r="O191">
+        <v>1718.69</v>
+      </c>
+      <c r="P191">
+        <v>373.66</v>
+      </c>
+      <c r="Q191">
+        <v>162.4709</v>
+      </c>
+      <c r="R191">
+        <v>4.9508999999999999</v>
+      </c>
+      <c r="S191">
+        <v>5.1306892120000001</v>
+      </c>
+      <c r="T191">
+        <v>5215.8100000000004</v>
+      </c>
+      <c r="U191">
+        <v>1654.5</v>
+      </c>
+      <c r="V191">
+        <v>2389.3040000000001</v>
+      </c>
+      <c r="W191">
+        <v>141.40625</v>
+      </c>
+      <c r="X191">
+        <v>388.47</v>
+      </c>
+      <c r="Y191">
+        <v>1168.26</v>
+      </c>
+    </row>
+    <row r="192" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A192" s="1">
+        <v>45077</v>
+      </c>
+      <c r="B192">
+        <v>138.65</v>
+      </c>
+      <c r="C192">
+        <v>4020.88</v>
+      </c>
+      <c r="D192">
+        <v>170.57380000000001</v>
+      </c>
+      <c r="E192">
+        <v>4179.83</v>
+      </c>
+      <c r="F192">
+        <v>646.37</v>
+      </c>
+      <c r="G192">
+        <v>1749.65</v>
+      </c>
+      <c r="H192">
+        <v>2041.81</v>
+      </c>
+      <c r="I192">
+        <v>958.53</v>
+      </c>
+      <c r="J192">
+        <v>514.86080000000004</v>
+      </c>
+      <c r="K192">
+        <v>1453.913</v>
+      </c>
+      <c r="L192">
+        <v>1263.18</v>
+      </c>
+      <c r="M192">
+        <v>18548.652999999998</v>
+      </c>
+      <c r="N192">
+        <v>3798.5059999999999</v>
+      </c>
+      <c r="O192">
+        <v>1718.69</v>
+      </c>
+      <c r="P192">
+        <v>357.38</v>
+      </c>
+      <c r="Q192">
+        <v>162.4709</v>
+      </c>
+      <c r="R192">
+        <v>5.1535799999999998</v>
+      </c>
+      <c r="S192">
+        <v>5.3719694689999997</v>
+      </c>
+      <c r="T192">
+        <v>5215.8100000000004</v>
+      </c>
+      <c r="U192">
+        <v>1630.51</v>
+      </c>
+      <c r="V192">
+        <v>2394.2890000000002</v>
+      </c>
+      <c r="W192">
+        <v>136.375</v>
+      </c>
+      <c r="X192">
+        <v>379.55</v>
+      </c>
+      <c r="Y192">
+        <v>1161.44</v>
+      </c>
+    </row>
+    <row r="193" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A193" s="1">
+        <v>45107</v>
+      </c>
+      <c r="B193">
+        <v>139.72999999999999</v>
+      </c>
+      <c r="C193">
+        <v>4082.76</v>
+      </c>
+      <c r="D193">
+        <v>169.756</v>
+      </c>
+      <c r="E193">
+        <v>4450.38</v>
+      </c>
+      <c r="F193">
+        <v>682.84</v>
+      </c>
+      <c r="G193">
+        <v>1888.7339999999999</v>
+      </c>
+      <c r="H193">
+        <v>2131.7199999999998</v>
+      </c>
+      <c r="I193">
+        <v>989.48</v>
+      </c>
+      <c r="J193">
+        <v>526.38220000000001</v>
+      </c>
+      <c r="K193">
+        <v>1477.579</v>
+      </c>
+      <c r="L193">
+        <v>1270.1099999999999</v>
+      </c>
+      <c r="M193">
+        <v>18754.213</v>
+      </c>
+      <c r="N193">
+        <v>3875.848</v>
+      </c>
+      <c r="O193">
+        <v>1718.69</v>
+      </c>
+      <c r="P193">
+        <v>373.51</v>
+      </c>
+      <c r="Q193">
+        <v>162.4709</v>
+      </c>
+      <c r="R193">
+        <v>5.2157900000000001</v>
+      </c>
+      <c r="S193">
+        <v>5.2487262379999997</v>
+      </c>
+      <c r="T193">
+        <v>5362.12</v>
+      </c>
+      <c r="U193">
+        <v>1722.87</v>
+      </c>
+      <c r="V193">
+        <v>2554.4879999999998</v>
+      </c>
+      <c r="W193">
+        <v>136.21875</v>
+      </c>
+      <c r="X193">
+        <v>376.94</v>
+      </c>
+      <c r="Y193">
+        <v>1170.99</v>
+      </c>
+    </row>
+    <row r="194" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A194" s="1">
+        <v>45138</v>
+      </c>
+      <c r="B194">
+        <v>134.74</v>
+      </c>
+      <c r="C194">
+        <v>4077.42</v>
+      </c>
+      <c r="D194">
+        <v>164.77119999999999</v>
+      </c>
+      <c r="E194">
+        <v>4588.96</v>
+      </c>
+      <c r="F194">
+        <v>707.11</v>
+      </c>
+      <c r="G194">
+        <v>2003.1769999999999</v>
+      </c>
+      <c r="H194">
+        <v>2199.36</v>
+      </c>
+      <c r="I194">
+        <v>1046.9100000000001</v>
+      </c>
+      <c r="J194">
+        <v>533.23329999999999</v>
+      </c>
+      <c r="K194">
+        <v>1498.62</v>
+      </c>
+      <c r="L194">
+        <v>1256.76</v>
+      </c>
+      <c r="M194">
+        <v>18878.060000000001</v>
+      </c>
+      <c r="N194">
+        <v>3815.0520000000001</v>
+      </c>
+      <c r="O194">
+        <v>1718.69</v>
+      </c>
+      <c r="P194">
+        <v>380.33</v>
+      </c>
+      <c r="Q194">
+        <v>162.4709</v>
+      </c>
+      <c r="R194">
+        <v>5.2787199999999999</v>
+      </c>
+      <c r="S194">
+        <v>5.3514236679999998</v>
+      </c>
+      <c r="T194">
+        <v>5362.12</v>
+      </c>
+      <c r="U194">
+        <v>1786.91</v>
+      </c>
+      <c r="V194">
+        <v>2643.6860000000001</v>
+      </c>
+      <c r="W194">
+        <v>132.21875</v>
+      </c>
+      <c r="X194">
+        <v>371.29</v>
+      </c>
+      <c r="Y194">
+        <v>1168.9000000000001</v>
+      </c>
+    </row>
+    <row r="195" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A195" s="1">
+        <v>45169</v>
+      </c>
+      <c r="B195">
+        <v>128.56</v>
+      </c>
+      <c r="C195">
+        <v>3997.94</v>
+      </c>
+      <c r="D195">
+        <v>159.50399999999999</v>
+      </c>
+      <c r="E195">
+        <v>4507.66</v>
+      </c>
+      <c r="F195">
+        <v>686.15</v>
+      </c>
+      <c r="G195">
+        <v>1899.6759999999999</v>
+      </c>
+      <c r="H195">
+        <v>2109.16</v>
+      </c>
+      <c r="I195">
+        <v>980.33</v>
+      </c>
+      <c r="J195">
+        <v>539.38930000000005</v>
+      </c>
+      <c r="K195">
+        <v>1502.896</v>
+      </c>
+      <c r="L195">
+        <v>1256.23</v>
+      </c>
+      <c r="M195">
+        <v>18785.47</v>
+      </c>
+      <c r="N195">
+        <v>3778.9369999999999</v>
+      </c>
+      <c r="O195">
+        <v>1718.69</v>
+      </c>
+      <c r="P195">
+        <v>366.99</v>
+      </c>
+      <c r="Q195">
+        <v>162.4709</v>
+      </c>
+      <c r="R195">
+        <v>5.3294600000000001</v>
+      </c>
+      <c r="S195">
+        <v>5.413067388</v>
+      </c>
+      <c r="T195">
+        <v>5362.12</v>
+      </c>
+      <c r="U195">
+        <v>1732.63</v>
+      </c>
+      <c r="V195">
+        <v>2588.1060000000002</v>
+      </c>
+      <c r="W195">
+        <v>127.96875</v>
+      </c>
+      <c r="X195">
+        <v>364.19</v>
+      </c>
+      <c r="Y195">
+        <v>1177.27</v>
       </c>
     </row>
   </sheetData>
@@ -15182,10 +15721,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y183"/>
+  <dimension ref="A1:Y190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A149" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D189" sqref="D189"/>
+    <sheetView tabSelected="1" topLeftCell="A160" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D185" sqref="D185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29252,13 +29791,13 @@
         <v>507.7645</v>
       </c>
       <c r="K183">
-        <v>1456.48</v>
+        <v>1456.4829999999999</v>
       </c>
       <c r="L183">
         <v>1267.28</v>
       </c>
       <c r="M183">
-        <v>18959.123</v>
+        <v>18975.955000000002</v>
       </c>
       <c r="N183">
         <v>3817.4569999999999</v>
@@ -29279,7 +29818,7 @@
         <v>4.6489987660000001</v>
       </c>
       <c r="T183">
-        <v>4976.87</v>
+        <v>5079.05</v>
       </c>
       <c r="U183">
         <v>1648.91</v>
@@ -29295,6 +29834,545 @@
       </c>
       <c r="Y183">
         <v>1168.94</v>
+      </c>
+    </row>
+    <row r="184" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A184" s="1">
+        <v>44985</v>
+      </c>
+      <c r="B184">
+        <v>136.36000000000001</v>
+      </c>
+      <c r="C184">
+        <v>3934.93</v>
+      </c>
+      <c r="D184">
+        <v>168.9444</v>
+      </c>
+      <c r="E184">
+        <v>3970.15</v>
+      </c>
+      <c r="F184">
+        <v>629.02</v>
+      </c>
+      <c r="G184">
+        <v>1896.991</v>
+      </c>
+      <c r="H184">
+        <v>2053.69</v>
+      </c>
+      <c r="I184">
+        <v>964.01</v>
+      </c>
+      <c r="J184">
+        <v>510.96210000000002</v>
+      </c>
+      <c r="K184">
+        <v>1437.635</v>
+      </c>
+      <c r="L184">
+        <v>1273.56</v>
+      </c>
+      <c r="M184">
+        <v>18958.985000000001</v>
+      </c>
+      <c r="N184">
+        <v>3888.33</v>
+      </c>
+      <c r="O184">
+        <v>1718.69</v>
+      </c>
+      <c r="P184">
+        <v>382.53</v>
+      </c>
+      <c r="Q184">
+        <v>162.4709</v>
+      </c>
+      <c r="R184">
+        <v>4.67272</v>
+      </c>
+      <c r="S184">
+        <v>4.8077261</v>
+      </c>
+      <c r="T184">
+        <v>5079.05</v>
+      </c>
+      <c r="U184">
+        <v>1601.19</v>
+      </c>
+      <c r="V184">
+        <v>2308.3960000000002</v>
+      </c>
+      <c r="W184">
+        <v>134.5625</v>
+      </c>
+      <c r="X184">
+        <v>366.54</v>
+      </c>
+      <c r="Y184">
+        <v>1166.95</v>
+      </c>
+    </row>
+    <row r="185" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A185" s="1">
+        <v>45016</v>
+      </c>
+      <c r="B185">
+        <v>143.85</v>
+      </c>
+      <c r="C185">
+        <v>4104.91</v>
+      </c>
+      <c r="D185">
+        <v>176.52780000000001</v>
+      </c>
+      <c r="E185">
+        <v>4109.3100000000004</v>
+      </c>
+      <c r="F185">
+        <v>646.76</v>
+      </c>
+      <c r="G185">
+        <v>1802.4839999999999</v>
+      </c>
+      <c r="H185">
+        <v>2092.6</v>
+      </c>
+      <c r="I185">
+        <v>990.28</v>
+      </c>
+      <c r="J185">
+        <v>510.464</v>
+      </c>
+      <c r="K185">
+        <v>1453.818</v>
+      </c>
+      <c r="L185">
+        <v>1235.1600000000001</v>
+      </c>
+      <c r="M185">
+        <v>18448.667000000001</v>
+      </c>
+      <c r="N185">
+        <v>3587.8829999999998</v>
+      </c>
+      <c r="O185">
+        <v>1718.69</v>
+      </c>
+      <c r="P185">
+        <v>373.22</v>
+      </c>
+      <c r="Q185">
+        <v>162.4709</v>
+      </c>
+      <c r="R185">
+        <v>4.6408199999999997</v>
+      </c>
+      <c r="S185">
+        <v>4.7309068339999998</v>
+      </c>
+      <c r="T185">
+        <v>5215.8100000000004</v>
+      </c>
+      <c r="U185">
+        <v>1636.36</v>
+      </c>
+      <c r="V185">
+        <v>2366.27</v>
+      </c>
+      <c r="W185">
+        <v>141.125</v>
+      </c>
+      <c r="X185">
+        <v>385.5</v>
+      </c>
+      <c r="Y185">
+        <v>1165.6300000000001</v>
+      </c>
+    </row>
+    <row r="186" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A186" s="1">
+        <v>45044</v>
+      </c>
+      <c r="B186">
+        <v>144.24</v>
+      </c>
+      <c r="C186">
+        <v>4135.75</v>
+      </c>
+      <c r="D186">
+        <v>176.87960000000001</v>
+      </c>
+      <c r="E186">
+        <v>4169.4799999999996</v>
+      </c>
+      <c r="F186">
+        <v>655</v>
+      </c>
+      <c r="G186">
+        <v>1768.9870000000001</v>
+      </c>
+      <c r="H186">
+        <v>2143.85</v>
+      </c>
+      <c r="I186">
+        <v>977.05</v>
+      </c>
+      <c r="J186">
+        <v>515.30060000000003</v>
+      </c>
+      <c r="K186">
+        <v>1467.85</v>
+      </c>
+      <c r="L186">
+        <v>1252.01</v>
+      </c>
+      <c r="M186">
+        <v>18601.562999999998</v>
+      </c>
+      <c r="N186">
+        <v>3691.1089999999999</v>
+      </c>
+      <c r="O186">
+        <v>1718.69</v>
+      </c>
+      <c r="P186">
+        <v>373.66</v>
+      </c>
+      <c r="Q186">
+        <v>162.4709</v>
+      </c>
+      <c r="R186">
+        <v>4.9508999999999999</v>
+      </c>
+      <c r="S186">
+        <v>5.1306892120000001</v>
+      </c>
+      <c r="T186">
+        <v>5215.8100000000004</v>
+      </c>
+      <c r="U186">
+        <v>1654.5</v>
+      </c>
+      <c r="V186">
+        <v>2389.3040000000001</v>
+      </c>
+      <c r="W186">
+        <v>141.40625</v>
+      </c>
+      <c r="X186">
+        <v>388.47</v>
+      </c>
+      <c r="Y186">
+        <v>1168.26</v>
+      </c>
+    </row>
+    <row r="187" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A187" s="1">
+        <v>45077</v>
+      </c>
+      <c r="B187">
+        <v>138.65</v>
+      </c>
+      <c r="C187">
+        <v>4020.88</v>
+      </c>
+      <c r="D187">
+        <v>170.57380000000001</v>
+      </c>
+      <c r="E187">
+        <v>4179.83</v>
+      </c>
+      <c r="F187">
+        <v>646.37</v>
+      </c>
+      <c r="G187">
+        <v>1749.65</v>
+      </c>
+      <c r="H187">
+        <v>2041.81</v>
+      </c>
+      <c r="I187">
+        <v>958.53</v>
+      </c>
+      <c r="J187">
+        <v>514.86080000000004</v>
+      </c>
+      <c r="K187">
+        <v>1453.913</v>
+      </c>
+      <c r="L187">
+        <v>1263.18</v>
+      </c>
+      <c r="M187">
+        <v>18548.652999999998</v>
+      </c>
+      <c r="N187">
+        <v>3798.5059999999999</v>
+      </c>
+      <c r="O187">
+        <v>1718.69</v>
+      </c>
+      <c r="P187">
+        <v>357.38</v>
+      </c>
+      <c r="Q187">
+        <v>162.4709</v>
+      </c>
+      <c r="R187">
+        <v>5.1535799999999998</v>
+      </c>
+      <c r="S187">
+        <v>5.3719694689999997</v>
+      </c>
+      <c r="T187">
+        <v>5215.8100000000004</v>
+      </c>
+      <c r="U187">
+        <v>1630.51</v>
+      </c>
+      <c r="V187">
+        <v>2394.2890000000002</v>
+      </c>
+      <c r="W187">
+        <v>136.375</v>
+      </c>
+      <c r="X187">
+        <v>379.55</v>
+      </c>
+      <c r="Y187">
+        <v>1161.44</v>
+      </c>
+    </row>
+    <row r="188" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A188" s="1">
+        <v>45107</v>
+      </c>
+      <c r="B188">
+        <v>139.72999999999999</v>
+      </c>
+      <c r="C188">
+        <v>4082.76</v>
+      </c>
+      <c r="D188">
+        <v>169.756</v>
+      </c>
+      <c r="E188">
+        <v>4450.38</v>
+      </c>
+      <c r="F188">
+        <v>682.84</v>
+      </c>
+      <c r="G188">
+        <v>1888.7339999999999</v>
+      </c>
+      <c r="H188">
+        <v>2131.7199999999998</v>
+      </c>
+      <c r="I188">
+        <v>989.48</v>
+      </c>
+      <c r="J188">
+        <v>526.38220000000001</v>
+      </c>
+      <c r="K188">
+        <v>1477.579</v>
+      </c>
+      <c r="L188">
+        <v>1270.1099999999999</v>
+      </c>
+      <c r="M188">
+        <v>18754.213</v>
+      </c>
+      <c r="N188">
+        <v>3875.848</v>
+      </c>
+      <c r="O188">
+        <v>1718.69</v>
+      </c>
+      <c r="P188">
+        <v>373.51</v>
+      </c>
+      <c r="Q188">
+        <v>162.4709</v>
+      </c>
+      <c r="R188">
+        <v>5.2157900000000001</v>
+      </c>
+      <c r="S188">
+        <v>5.2487262379999997</v>
+      </c>
+      <c r="T188">
+        <v>5362.12</v>
+      </c>
+      <c r="U188">
+        <v>1722.87</v>
+      </c>
+      <c r="V188">
+        <v>2554.4879999999998</v>
+      </c>
+      <c r="W188">
+        <v>136.21875</v>
+      </c>
+      <c r="X188">
+        <v>376.94</v>
+      </c>
+      <c r="Y188">
+        <v>1170.99</v>
+      </c>
+    </row>
+    <row r="189" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A189" s="1">
+        <v>45138</v>
+      </c>
+      <c r="B189">
+        <v>134.74</v>
+      </c>
+      <c r="C189">
+        <v>4077.42</v>
+      </c>
+      <c r="D189">
+        <v>164.77119999999999</v>
+      </c>
+      <c r="E189">
+        <v>4588.96</v>
+      </c>
+      <c r="F189">
+        <v>707.11</v>
+      </c>
+      <c r="G189">
+        <v>2003.1769999999999</v>
+      </c>
+      <c r="H189">
+        <v>2199.36</v>
+      </c>
+      <c r="I189">
+        <v>1046.9100000000001</v>
+      </c>
+      <c r="J189">
+        <v>533.23329999999999</v>
+      </c>
+      <c r="K189">
+        <v>1498.62</v>
+      </c>
+      <c r="L189">
+        <v>1256.76</v>
+      </c>
+      <c r="M189">
+        <v>18878.060000000001</v>
+      </c>
+      <c r="N189">
+        <v>3815.0520000000001</v>
+      </c>
+      <c r="O189">
+        <v>1718.69</v>
+      </c>
+      <c r="P189">
+        <v>380.33</v>
+      </c>
+      <c r="Q189">
+        <v>162.4709</v>
+      </c>
+      <c r="R189">
+        <v>5.2787199999999999</v>
+      </c>
+      <c r="S189">
+        <v>5.3514236679999998</v>
+      </c>
+      <c r="T189">
+        <v>5362.12</v>
+      </c>
+      <c r="U189">
+        <v>1786.91</v>
+      </c>
+      <c r="V189">
+        <v>2643.6860000000001</v>
+      </c>
+      <c r="W189">
+        <v>132.21875</v>
+      </c>
+      <c r="X189">
+        <v>371.29</v>
+      </c>
+      <c r="Y189">
+        <v>1168.9000000000001</v>
+      </c>
+    </row>
+    <row r="190" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A190" s="1">
+        <v>45169</v>
+      </c>
+      <c r="B190">
+        <v>128.56</v>
+      </c>
+      <c r="C190">
+        <v>3997.94</v>
+      </c>
+      <c r="D190">
+        <v>159.50399999999999</v>
+      </c>
+      <c r="E190">
+        <v>4507.66</v>
+      </c>
+      <c r="F190">
+        <v>686.15</v>
+      </c>
+      <c r="G190">
+        <v>1899.6759999999999</v>
+      </c>
+      <c r="H190">
+        <v>2109.16</v>
+      </c>
+      <c r="I190">
+        <v>980.33</v>
+      </c>
+      <c r="J190">
+        <v>539.38930000000005</v>
+      </c>
+      <c r="K190">
+        <v>1502.896</v>
+      </c>
+      <c r="L190">
+        <v>1256.23</v>
+      </c>
+      <c r="M190">
+        <v>18785.47</v>
+      </c>
+      <c r="N190">
+        <v>3778.9369999999999</v>
+      </c>
+      <c r="O190">
+        <v>1718.69</v>
+      </c>
+      <c r="P190">
+        <v>366.99</v>
+      </c>
+      <c r="Q190">
+        <v>162.4709</v>
+      </c>
+      <c r="R190">
+        <v>5.3294600000000001</v>
+      </c>
+      <c r="S190">
+        <v>5.413067388</v>
+      </c>
+      <c r="T190">
+        <v>5362.12</v>
+      </c>
+      <c r="U190">
+        <v>1732.63</v>
+      </c>
+      <c r="V190">
+        <v>2588.1060000000002</v>
+      </c>
+      <c r="W190">
+        <v>127.96875</v>
+      </c>
+      <c r="X190">
+        <v>364.19</v>
+      </c>
+      <c r="Y190">
+        <v>1177.27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update index data 11/30/2023
</commit_message>
<xml_diff>
--- a/data/index_data.xlsx
+++ b/data/index_data.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="28">
   <si>
     <t>Start Date</t>
   </si>
@@ -124,10 +124,6 @@
   <si>
     <t>SPUSTBTR Index</t>
   </si>
-  <si>
-    <t>12/31
-/2022</t>
-  </si>
 </sst>
 </file>
 
@@ -208,74 +204,62 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|16260322941572045888</stp>
-        <tr r="S7" s="1"/>
+        <stp>BDH|18353857057369631726</stp>
+        <tr r="W7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|15186403787347702677</stp>
+        <stp>BDH|12375187216603128887</stp>
+        <tr r="E7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|15637698320093187126</stp>
+        <tr r="N7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|10544755452679912856</stp>
+        <tr r="J7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|17008031545871345295</stp>
         <tr r="D7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|17715390876150307109</stp>
-        <tr r="G7" s="1"/>
+        <stp>BDH|18051710263079419431</stp>
+        <tr r="I7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|14406751109895676413</stp>
+        <stp>BDH|17906278738741851393</stp>
         <tr r="R7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|17616552325801162125</stp>
-        <tr r="T7" s="1"/>
+        <stp>BDH|15076265050800807667</stp>
+        <tr r="A7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|10209224655710149712</stp>
-        <tr r="U7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|17591541156537809071</stp>
-        <tr r="P7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|14289313393759269664</stp>
-        <tr r="I7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|10354867160237036826</stp>
+        <stp>BDH|14532257514907526562</stp>
         <tr r="V7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|17339952999957269647</stp>
-        <tr r="W7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|12836079640644446547</stp>
-        <tr r="Q7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|13340564228128127892</stp>
-        <tr r="C7" s="1"/>
+        <stp>BDH|11680503742052798740</stp>
+        <tr r="T7" s="1"/>
       </tp>
     </main>
     <main first="bloomberg.rtd">
@@ -342,14 +326,6 @@
         <stp>[index_data.xlsx]bbg!R5C2</stp>
         <stp>PX_LAST</stp>
         <tr r="B5" s="1"/>
-      </tp>
-    </main>
-    <main first="bofaddin.rtdserver">
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|2583946357844558468</stp>
-        <tr r="F7" s="1"/>
       </tp>
     </main>
     <main first="bloomberg.rtd">
@@ -478,62 +454,80 @@
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|8715571147982884261</stp>
-        <tr r="A7" s="1"/>
+        <stp>BDH|4698709259818338682</stp>
+        <tr r="L7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|5337857811456651135</stp>
+        <stp>BDH|3156902016925940470</stp>
+        <tr r="G7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|9021653845256816778</stp>
         <tr r="M7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|1937304033633197694</stp>
+        <stp>BDH|9878140236898161867</stp>
+        <tr r="S7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|3127725000869849948</stp>
+        <tr r="P7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|7880740441696071762</stp>
+        <tr r="X7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|8987355549103844967</stp>
+        <tr r="K7" s="1"/>
+      </tp>
+      <tp t="s">
+        <v>#N/A N/A</v>
+        <stp/>
+        <stp>BDH|7253797949649611807</stp>
         <tr r="H7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|5148256585428118167</stp>
-        <tr r="L7" s="1"/>
+        <stp>BDH|7662456251601122105</stp>
+        <tr r="F7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|1536785358873787645</stp>
-        <tr r="N7" s="1"/>
+        <stp>BDH|2208639251642318485</stp>
+        <tr r="U7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|2449917877528190397</stp>
-        <tr r="X7" s="1"/>
+        <stp>BDH|1246031807909967823</stp>
+        <tr r="Q7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|1570140149985888625</stp>
-        <tr r="E7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|3329653219596187212</stp>
+        <stp>BDH|3873689679061216397</stp>
         <tr r="O7" s="1"/>
       </tp>
       <tp t="s">
         <v>#N/A N/A</v>
         <stp/>
-        <stp>BDH|9930674116049078781</stp>
-        <tr r="J7" s="1"/>
-      </tp>
-      <tp t="s">
-        <v>#N/A N/A</v>
-        <stp/>
-        <stp>BDH|2079352188799857328</stp>
-        <tr r="K7" s="1"/>
+        <stp>BDH|7736316424220650774</stp>
+        <tr r="C7" s="1"/>
       </tp>
     </main>
   </volType>
@@ -837,10 +831,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X187"/>
+  <dimension ref="A1:X198"/>
   <sheetViews>
-    <sheetView topLeftCell="A133" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A187" sqref="A187:X187"/>
+    <sheetView topLeftCell="A151" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A198" sqref="A160:X198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -869,12 +863,12 @@
         <v>39447</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>28</v>
+      <c r="B2" s="7">
+        <v>45260</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
@@ -1118,98 +1112,98 @@
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <f>_xll.BDH(B$4,B$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=S","cols=2;rows=181")</f>
+        <f>_xll.BDH(B$4,B$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=S","cols=2;rows=192")</f>
         <v>39447</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
       </c>
       <c r="C7">
-        <f>_xll.BDH(C$4,C$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(C$4,C$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=192")</f>
         <v>1902.17</v>
       </c>
       <c r="D7" t="str">
-        <f>_xll.BDH(D$4,D$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(D$4,D$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=192")</f>
         <v>#N/A N/A</v>
       </c>
       <c r="E7">
-        <f>_xll.BDH(E$4,E$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(E$4,E$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=192")</f>
         <v>1468.36</v>
       </c>
       <c r="F7">
-        <f>_xll.BDH(F$4,F$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(F$4,F$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=192")</f>
         <v>403.25</v>
       </c>
       <c r="G7">
-        <f>_xll.BDH(G$4,G$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(G$4,G$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=192")</f>
         <v>766.03700000000003</v>
       </c>
       <c r="H7">
-        <f>_xll.BDH(H$4,H$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(H$4,H$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=192")</f>
         <v>2253.36</v>
       </c>
       <c r="I7">
-        <f>_xll.BDH(I$4,I$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(I$4,I$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=192")</f>
         <v>1245.5899999999999</v>
       </c>
       <c r="J7">
-        <f>_xll.BDH(J$4,J$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(J$4,J$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=192")</f>
         <v>270.02620000000002</v>
       </c>
       <c r="K7">
-        <f>_xll.BDH(K$4,K$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(K$4,K$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=192")</f>
         <v>590.78</v>
       </c>
       <c r="L7">
-        <f>_xll.BDH(L$4,L$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
-        <v>1294.82</v>
+        <f>_xll.BDH(L$4,L$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=192")</f>
+        <v>1294.818</v>
       </c>
       <c r="M7">
-        <f>_xll.BDH(M$4,M$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(M$4,M$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=192")</f>
         <v>12335.221</v>
       </c>
       <c r="N7">
-        <f>_xll.BDH(N$4,N$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(N$4,N$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=192")</f>
         <v>1915.1320000000001</v>
       </c>
       <c r="O7">
-        <f>_xll.BDH(O$4,O$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(O$4,O$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=192")</f>
         <v>1389.21</v>
       </c>
       <c r="P7">
-        <f>_xll.BDH(P$4,P$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(P$4,P$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=192")</f>
         <v>255.67</v>
       </c>
       <c r="Q7">
-        <f>_xll.BDH(Q$4,Q$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(Q$4,Q$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=192")</f>
         <v>141.76349999999999</v>
       </c>
       <c r="R7">
-        <f>_xll.BDH(R$4,R$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(R$4,R$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=192")</f>
         <v>3.1589900000000002</v>
       </c>
       <c r="S7">
-        <f>_xll.BDH(S$4,S$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(S$4,S$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=192")</f>
         <v>3.33792826</v>
       </c>
       <c r="T7">
-        <f>_xll.BDH(T$4,T$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(T$4,T$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=192")</f>
         <v>1412.28</v>
       </c>
       <c r="U7">
-        <f>_xll.BDH(U$4,U$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(U$4,U$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=192")</f>
         <v>996.96</v>
       </c>
       <c r="V7">
-        <f>_xll.BDH(V$4,V$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(V$4,V$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=192")</f>
         <v>849.221</v>
       </c>
       <c r="W7" t="str">
-        <f>_xll.BDH(W$4,W$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(W$4,W$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=192")</f>
         <v>#N/A N/A</v>
       </c>
       <c r="X7">
-        <f>_xll.BDH(X$4,X$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=181")</f>
+        <f>_xll.BDH(X$4,X$6,$B1,$B2,"Dir=V","Per=M","Days=A","Dts=H","cols=1;rows=192")</f>
         <v>221.59</v>
       </c>
     </row>
@@ -1245,13 +1239,13 @@
         <v>261.66860000000003</v>
       </c>
       <c r="K8">
-        <v>582.75</v>
+        <v>582.75300000000004</v>
       </c>
       <c r="L8">
-        <v>1344.27</v>
+        <v>1344.268</v>
       </c>
       <c r="M8">
-        <v>12468.7682</v>
+        <v>12468.768</v>
       </c>
       <c r="N8">
         <v>1965.15</v>
@@ -1319,13 +1313,13 @@
         <v>255.42519999999999</v>
       </c>
       <c r="K9">
-        <v>575.83000000000004</v>
+        <v>575.83399999999995</v>
       </c>
       <c r="L9">
-        <v>1459.01</v>
+        <v>1459.009</v>
       </c>
       <c r="M9">
-        <v>12994.856299999999</v>
+        <v>12994.856</v>
       </c>
       <c r="N9">
         <v>2106.0329999999999</v>
@@ -1393,13 +1387,13 @@
         <v>254.5256</v>
       </c>
       <c r="K10">
-        <v>572.84</v>
+        <v>572.84400000000005</v>
       </c>
       <c r="L10">
-        <v>1415.2</v>
+        <v>1415.204</v>
       </c>
       <c r="M10">
-        <v>12836.166800000001</v>
+        <v>12836.166999999999</v>
       </c>
       <c r="N10">
         <v>2077.0700000000002</v>
@@ -1467,13 +1461,13 @@
         <v>262.93880000000001</v>
       </c>
       <c r="K11">
-        <v>596.71</v>
+        <v>596.70699999999999</v>
       </c>
       <c r="L11">
         <v>1405.95</v>
       </c>
       <c r="M11">
-        <v>12831.954900000001</v>
+        <v>12831.955</v>
       </c>
       <c r="N11">
         <v>2041.4290000000001</v>
@@ -1541,13 +1535,13 @@
         <v>264.8886</v>
       </c>
       <c r="K12">
-        <v>599.26</v>
+        <v>599.26300000000003</v>
       </c>
       <c r="L12">
-        <v>1430.86</v>
+        <v>1430.864</v>
       </c>
       <c r="M12">
-        <v>12986.5229</v>
+        <v>12986.522999999999</v>
       </c>
       <c r="N12">
         <v>2094.21</v>
@@ -1615,13 +1609,13 @@
         <v>265.29180000000002</v>
       </c>
       <c r="K13">
-        <v>583.21</v>
+        <v>583.20600000000002</v>
       </c>
       <c r="L13">
-        <v>1477.36</v>
+        <v>1477.3610000000001</v>
       </c>
       <c r="M13">
-        <v>13141.3627</v>
+        <v>13141.362999999999</v>
       </c>
       <c r="N13">
         <v>2207.183</v>
@@ -1689,13 +1683,13 @@
         <v>262.70940000000002</v>
       </c>
       <c r="K14">
-        <v>573.86</v>
+        <v>573.85900000000004</v>
       </c>
       <c r="L14">
         <v>1394.77</v>
       </c>
       <c r="M14">
-        <v>12796.566800000001</v>
+        <v>12796.566999999999</v>
       </c>
       <c r="N14">
         <v>2095.7800000000002</v>
@@ -1763,13 +1757,13 @@
         <v>262.5575</v>
       </c>
       <c r="K15">
-        <v>575.71</v>
+        <v>575.71100000000001</v>
       </c>
       <c r="L15">
-        <v>1339.78</v>
+        <v>1339.7809999999999</v>
       </c>
       <c r="M15">
-        <v>12645.730799999999</v>
+        <v>12645.731</v>
       </c>
       <c r="N15">
         <v>2035.0039999999999</v>
@@ -1837,13 +1831,13 @@
         <v>249.61969999999999</v>
       </c>
       <c r="K16">
-        <v>527.94000000000005</v>
+        <v>527.94200000000001</v>
       </c>
       <c r="L16">
-        <v>1328.39</v>
+        <v>1328.394</v>
       </c>
       <c r="M16">
-        <v>12492.1569</v>
+        <v>12492.156999999999</v>
       </c>
       <c r="N16">
         <v>2054.8670000000002</v>
@@ -1911,13 +1905,13 @@
         <v>217.0848</v>
       </c>
       <c r="K17">
-        <v>441.9</v>
+        <v>441.89600000000002</v>
       </c>
       <c r="L17">
-        <v>1304.98</v>
+        <v>1304.9829999999999</v>
       </c>
       <c r="M17">
-        <v>12695.992899999999</v>
+        <v>12695.993</v>
       </c>
       <c r="N17">
         <v>2205.1550000000002</v>
@@ -1985,13 +1979,13 @@
         <v>199.9513</v>
       </c>
       <c r="K18">
-        <v>404.63</v>
+        <v>404.63400000000001</v>
       </c>
       <c r="L18">
-        <v>1324.36</v>
+        <v>1324.355</v>
       </c>
       <c r="M18">
-        <v>12789.034900000001</v>
+        <v>12789.035</v>
       </c>
       <c r="N18">
         <v>2267.3110000000001</v>
@@ -2059,13 +2053,13 @@
         <v>192.38509999999999</v>
       </c>
       <c r="K19">
-        <v>434.88</v>
+        <v>434.87799999999999</v>
       </c>
       <c r="L19">
-        <v>1367.51</v>
+        <v>1367.5050000000001</v>
       </c>
       <c r="M19">
-        <v>12931.3459</v>
+        <v>12931.346</v>
       </c>
       <c r="N19">
         <v>2315.06</v>
@@ -2133,13 +2127,13 @@
         <v>203.49539999999999</v>
       </c>
       <c r="K20">
-        <v>457.96</v>
+        <v>457.96100000000001</v>
       </c>
       <c r="L20">
         <v>1387.26</v>
       </c>
       <c r="M20">
-        <v>12918.482099999999</v>
+        <v>12918.482</v>
       </c>
       <c r="N20">
         <v>2307.8919999999998</v>
@@ -2207,13 +2201,13 @@
         <v>204.20050000000001</v>
       </c>
       <c r="K21">
-        <v>442.09</v>
+        <v>442.08499999999998</v>
       </c>
       <c r="L21">
-        <v>1386.56</v>
+        <v>1386.559</v>
       </c>
       <c r="M21">
-        <v>12902.6587</v>
+        <v>12902.659</v>
       </c>
       <c r="N21">
         <v>2320.3330000000001</v>
@@ -2355,13 +2349,13 @@
         <v>222.69049999999999</v>
       </c>
       <c r="K23">
-        <v>509.05</v>
+        <v>509.05399999999997</v>
       </c>
       <c r="L23">
-        <v>1344.19</v>
+        <v>1344.194</v>
       </c>
       <c r="M23">
-        <v>12811.928599999999</v>
+        <v>12811.929</v>
       </c>
       <c r="N23">
         <v>2196.0830000000001</v>
@@ -2429,13 +2423,13 @@
         <v>235.3854</v>
       </c>
       <c r="K24">
-        <v>545.26</v>
+        <v>545.26300000000003</v>
       </c>
       <c r="L24">
-        <v>1330.23</v>
+        <v>1330.2260000000001</v>
       </c>
       <c r="M24">
-        <v>13264.861699999999</v>
+        <v>13264.861999999999</v>
       </c>
       <c r="N24">
         <v>2206.9</v>
@@ -2503,10 +2497,10 @@
         <v>244.51750000000001</v>
       </c>
       <c r="K25">
-        <v>562.6</v>
+        <v>562.601</v>
       </c>
       <c r="L25">
-        <v>1285.96</v>
+        <v>1285.9549999999999</v>
       </c>
       <c r="M25">
         <v>13109.794</v>
@@ -2577,13 +2571,13 @@
         <v>254.65369999999999</v>
       </c>
       <c r="K26">
-        <v>597.39</v>
+        <v>597.38699999999994</v>
       </c>
       <c r="L26">
-        <v>1286.8900000000001</v>
+        <v>1286.894</v>
       </c>
       <c r="M26">
-        <v>13174.286400000001</v>
+        <v>13174.286</v>
       </c>
       <c r="N26">
         <v>2141.98</v>
@@ -2651,13 +2645,13 @@
         <v>260.33589999999998</v>
       </c>
       <c r="K27">
-        <v>609.54</v>
+        <v>609.53700000000003</v>
       </c>
       <c r="L27">
-        <v>1276.6099999999999</v>
+        <v>1276.6079999999999</v>
       </c>
       <c r="M27">
-        <v>13223.647800000001</v>
+        <v>13223.647999999999</v>
       </c>
       <c r="N27">
         <v>2175.6089999999999</v>
@@ -2725,13 +2719,13 @@
         <v>268.88839999999999</v>
       </c>
       <c r="K28">
-        <v>645.96</v>
+        <v>645.96299999999997</v>
       </c>
       <c r="L28">
-        <v>1267.52</v>
+        <v>1267.5150000000001</v>
       </c>
       <c r="M28">
-        <v>13449.626700000001</v>
+        <v>13449.627</v>
       </c>
       <c r="N28">
         <v>2227.857</v>
@@ -2799,13 +2793,13 @@
         <v>270.64179999999999</v>
       </c>
       <c r="K29">
-        <v>657.5</v>
+        <v>657.50199999999995</v>
       </c>
       <c r="L29">
-        <v>1250.6199999999999</v>
+        <v>1250.6179999999999</v>
       </c>
       <c r="M29">
-        <v>13380.286099999999</v>
+        <v>13380.286</v>
       </c>
       <c r="N29">
         <v>2162.4050000000002</v>
@@ -2873,13 +2867,13 @@
         <v>271.42450000000002</v>
       </c>
       <c r="K30">
-        <v>664.16</v>
+        <v>664.16399999999999</v>
       </c>
       <c r="L30">
-        <v>1281.04</v>
+        <v>1281.0419999999999</v>
       </c>
       <c r="M30">
-        <v>13670.636699999999</v>
+        <v>13670.637000000001</v>
       </c>
       <c r="N30">
         <v>2274.2429999999999</v>
@@ -2947,10 +2941,10 @@
         <v>278.7047</v>
       </c>
       <c r="K31">
-        <v>684.98</v>
+        <v>684.98299999999995</v>
       </c>
       <c r="L31">
-        <v>1247.43</v>
+        <v>1247.434</v>
       </c>
       <c r="M31">
         <v>13492.601000000001</v>
@@ -3021,13 +3015,13 @@
         <v>283.74540000000002</v>
       </c>
       <c r="K32">
-        <v>695.36</v>
+        <v>695.36400000000003</v>
       </c>
       <c r="L32">
-        <v>1224.45</v>
+        <v>1224.4449999999999</v>
       </c>
       <c r="M32">
-        <v>13229.0828</v>
+        <v>13229.083000000001</v>
       </c>
       <c r="N32">
         <v>2119.4940000000001</v>
@@ -3095,13 +3089,13 @@
         <v>284.66649999999998</v>
       </c>
       <c r="K33">
-        <v>696.44</v>
+        <v>696.44100000000003</v>
       </c>
       <c r="L33">
-        <v>1241.75</v>
+        <v>1241.7539999999999</v>
       </c>
       <c r="M33">
-        <v>13250.2135</v>
+        <v>13250.214</v>
       </c>
       <c r="N33">
         <v>2161.3310000000001</v>
@@ -3169,13 +3163,13 @@
         <v>290.81540000000001</v>
       </c>
       <c r="K34">
-        <v>718</v>
+        <v>718.00099999999998</v>
       </c>
       <c r="L34">
-        <v>1255.06</v>
+        <v>1255.059</v>
       </c>
       <c r="M34">
-        <v>13460.915499999999</v>
+        <v>13460.915999999999</v>
       </c>
       <c r="N34">
         <v>2267.1979999999999</v>
@@ -3243,13 +3237,13 @@
         <v>294.53320000000002</v>
       </c>
       <c r="K35">
-        <v>734.08</v>
+        <v>734.077</v>
       </c>
       <c r="L35">
         <v>1246.22</v>
       </c>
       <c r="M35">
-        <v>13570.9728</v>
+        <v>13570.973</v>
       </c>
       <c r="N35">
         <v>2313.11</v>
@@ -3317,13 +3311,13 @@
         <v>288.47559999999999</v>
       </c>
       <c r="K36">
-        <v>708.23</v>
+        <v>708.23299999999995</v>
       </c>
       <c r="L36">
         <v>1234.72</v>
       </c>
       <c r="M36">
-        <v>13356.1283</v>
+        <v>13356.128000000001</v>
       </c>
       <c r="N36">
         <v>2208.9389999999999</v>
@@ -3391,13 +3385,13 @@
         <v>287.77719999999999</v>
       </c>
       <c r="K37">
-        <v>717.47</v>
+        <v>717.46699999999998</v>
       </c>
       <c r="L37">
-        <v>1218.45</v>
+        <v>1218.453</v>
       </c>
       <c r="M37">
-        <v>13340.6435</v>
+        <v>13340.644</v>
       </c>
       <c r="N37">
         <v>2196.9259999999999</v>
@@ -3465,10 +3459,10 @@
         <v>291.88330000000002</v>
       </c>
       <c r="K38">
-        <v>742.33</v>
+        <v>742.32799999999997</v>
       </c>
       <c r="L38">
-        <v>1210.82</v>
+        <v>1210.8219999999999</v>
       </c>
       <c r="M38">
         <v>13332.331</v>
@@ -3539,10 +3533,10 @@
         <v>292.94799999999998</v>
       </c>
       <c r="K39">
-        <v>743.49</v>
+        <v>743.48900000000003</v>
       </c>
       <c r="L39">
-        <v>1228.3499999999999</v>
+        <v>1228.3489999999999</v>
       </c>
       <c r="M39">
         <v>13557.523999999999</v>
@@ -3613,13 +3607,13 @@
         <v>296.69979999999998</v>
       </c>
       <c r="K40">
-        <v>765.56</v>
+        <v>765.56299999999999</v>
       </c>
       <c r="L40">
-        <v>1211.3499999999999</v>
+        <v>1211.347</v>
       </c>
       <c r="M40">
-        <v>13928.3614</v>
+        <v>13928.361000000001</v>
       </c>
       <c r="N40">
         <v>2339.1849999999999</v>
@@ -3690,10 +3684,10 @@
         <v>784.13</v>
       </c>
       <c r="L41">
-        <v>1223.1099999999999</v>
+        <v>1223.1110000000001</v>
       </c>
       <c r="M41">
-        <v>14239.0774</v>
+        <v>14239.076999999999</v>
       </c>
       <c r="N41">
         <v>2454.8679999999999</v>
@@ -3761,13 +3755,13 @@
         <v>302.4778</v>
       </c>
       <c r="K42">
-        <v>775.38</v>
+        <v>775.38199999999995</v>
       </c>
       <c r="L42">
-        <v>1209.6600000000001</v>
+        <v>1209.6569999999999</v>
       </c>
       <c r="M42">
-        <v>14108.606900000001</v>
+        <v>14108.607</v>
       </c>
       <c r="N42">
         <v>2359.6460000000002</v>
@@ -3835,13 +3829,13 @@
         <v>306.50450000000001</v>
       </c>
       <c r="K43">
-        <v>789.04</v>
+        <v>789.03499999999997</v>
       </c>
       <c r="L43">
-        <v>1225.8800000000001</v>
+        <v>1225.884</v>
       </c>
       <c r="M43">
-        <v>14579.778399999999</v>
+        <v>14579.778</v>
       </c>
       <c r="N43">
         <v>2493.3910000000001</v>
@@ -3909,10 +3903,10 @@
         <v>312.52589999999998</v>
       </c>
       <c r="K44">
-        <v>805.62</v>
+        <v>805.62400000000002</v>
       </c>
       <c r="L44">
-        <v>1227.69</v>
+        <v>1227.6890000000001</v>
       </c>
       <c r="M44">
         <v>14474.621999999999</v>
@@ -3983,13 +3977,13 @@
         <v>314.1893</v>
       </c>
       <c r="K45">
-        <v>816.4</v>
+        <v>816.39499999999998</v>
       </c>
       <c r="L45">
-        <v>1239.1600000000001</v>
+        <v>1239.1569999999999</v>
       </c>
       <c r="M45">
-        <v>14659.216200000001</v>
+        <v>14659.216</v>
       </c>
       <c r="N45">
         <v>2510.5619999999999</v>
@@ -4057,13 +4051,13 @@
         <v>314.62810000000002</v>
       </c>
       <c r="K46">
-        <v>819.83</v>
+        <v>819.82500000000005</v>
       </c>
       <c r="L46">
         <v>1243.9100000000001</v>
       </c>
       <c r="M46">
-        <v>14499.349700000001</v>
+        <v>14499.35</v>
       </c>
       <c r="N46">
         <v>2408.201</v>
@@ -4131,13 +4125,13 @@
         <v>316.52589999999998</v>
       </c>
       <c r="K47">
-        <v>832.29</v>
+        <v>832.28599999999994</v>
       </c>
       <c r="L47">
-        <v>1254.98</v>
+        <v>1254.981</v>
       </c>
       <c r="M47">
-        <v>14843.1054</v>
+        <v>14843.105</v>
       </c>
       <c r="N47">
         <v>2522.3739999999998</v>
@@ -4205,13 +4199,13 @@
         <v>316.71600000000001</v>
       </c>
       <c r="K48">
-        <v>836.36</v>
+        <v>836.35599999999999</v>
       </c>
       <c r="L48">
-        <v>1228.49</v>
+        <v>1228.4880000000001</v>
       </c>
       <c r="M48">
-        <v>14501.493200000001</v>
+        <v>14501.493</v>
       </c>
       <c r="N48">
         <v>2396.038</v>
@@ -4279,10 +4273,10 @@
         <v>315.6814</v>
       </c>
       <c r="K49">
-        <v>827.96</v>
+        <v>827.95500000000004</v>
       </c>
       <c r="L49">
-        <v>1199.6099999999999</v>
+        <v>1199.6089999999999</v>
       </c>
       <c r="M49">
         <v>14249.044</v>
@@ -4353,13 +4347,13 @@
         <v>316.2002</v>
       </c>
       <c r="K50">
-        <v>838.18</v>
+        <v>838.18399999999997</v>
       </c>
       <c r="L50">
-        <v>1214.8</v>
+        <v>1214.798</v>
       </c>
       <c r="M50">
-        <v>14484.9593</v>
+        <v>14484.959000000001</v>
       </c>
       <c r="N50">
         <v>2426.16</v>
@@ -4427,13 +4421,13 @@
         <v>303.04410000000001</v>
       </c>
       <c r="K51">
-        <v>804.6</v>
+        <v>804.59699999999998</v>
       </c>
       <c r="L51">
-        <v>1213.76</v>
+        <v>1213.7570000000001</v>
       </c>
       <c r="M51">
-        <v>14410.909799999999</v>
+        <v>14410.91</v>
       </c>
       <c r="N51">
         <v>2397.636</v>
@@ -4501,13 +4495,13 @@
         <v>303.81540000000001</v>
       </c>
       <c r="K52">
-        <v>775.67</v>
+        <v>775.67399999999998</v>
       </c>
       <c r="L52">
-        <v>1189.42</v>
+        <v>1189.424</v>
       </c>
       <c r="M52">
-        <v>14231.7312</v>
+        <v>14231.731</v>
       </c>
       <c r="N52">
         <v>2371.6529999999998</v>
@@ -4575,10 +4569,10 @@
         <v>311.6925</v>
       </c>
       <c r="K53">
-        <v>821.87</v>
+        <v>821.87099999999998</v>
       </c>
       <c r="L53">
-        <v>1165.81</v>
+        <v>1165.807</v>
       </c>
       <c r="M53">
         <v>14100.214</v>
@@ -4649,13 +4643,13 @@
         <v>310.50479999999999</v>
       </c>
       <c r="K54">
-        <v>803.7</v>
+        <v>803.69500000000005</v>
       </c>
       <c r="L54">
-        <v>1169.33</v>
+        <v>1169.3309999999999</v>
       </c>
       <c r="M54">
-        <v>14008.1811</v>
+        <v>14008.181</v>
       </c>
       <c r="N54">
         <v>2258.2049999999999</v>
@@ -4723,13 +4717,13 @@
         <v>312.07580000000002</v>
       </c>
       <c r="K55">
-        <v>823.62</v>
+        <v>823.61599999999999</v>
       </c>
       <c r="L55">
-        <v>1166.06</v>
+        <v>1166.059</v>
       </c>
       <c r="M55">
-        <v>13973.4763</v>
+        <v>13973.476000000001</v>
       </c>
       <c r="N55">
         <v>2295.5889999999999</v>
@@ -4797,13 +4791,13 @@
         <v>318.30500000000001</v>
       </c>
       <c r="K56">
-        <v>847.53</v>
+        <v>847.52499999999998</v>
       </c>
       <c r="L56">
-        <v>1167.1199999999999</v>
+        <v>1167.1220000000001</v>
       </c>
       <c r="M56">
-        <v>14150.578100000001</v>
+        <v>14150.578</v>
       </c>
       <c r="N56">
         <v>2319.9760000000001</v>
@@ -4871,13 +4865,13 @@
         <v>320.66320000000002</v>
       </c>
       <c r="K57">
-        <v>866.84</v>
+        <v>866.83600000000001</v>
       </c>
       <c r="L57">
-        <v>1169.6400000000001</v>
+        <v>1169.6369999999999</v>
       </c>
       <c r="M57">
-        <v>14262.293900000001</v>
+        <v>14262.294</v>
       </c>
       <c r="N57">
         <v>2355.634</v>
@@ -4945,13 +4939,13 @@
         <v>322.92290000000003</v>
       </c>
       <c r="K58">
-        <v>866.03</v>
+        <v>866.02499999999998</v>
       </c>
       <c r="L58">
-        <v>1150.97</v>
+        <v>1150.973</v>
       </c>
       <c r="M58">
-        <v>14074.2376</v>
+        <v>14074.237999999999</v>
       </c>
       <c r="N58">
         <v>2302.6779999999999</v>
@@ -5019,13 +5013,13 @@
         <v>325.4556</v>
       </c>
       <c r="K59">
-        <v>874.88</v>
+        <v>874.87800000000004</v>
       </c>
       <c r="L59">
-        <v>1155.8900000000001</v>
+        <v>1155.893</v>
       </c>
       <c r="M59">
-        <v>13992.7004</v>
+        <v>13992.7</v>
       </c>
       <c r="N59">
         <v>2319.3290000000002</v>
@@ -5093,13 +5087,13 @@
         <v>323.7833</v>
       </c>
       <c r="K60">
-        <v>864.32</v>
+        <v>864.31600000000003</v>
       </c>
       <c r="L60">
-        <v>1160.04</v>
+        <v>1160.0440000000001</v>
       </c>
       <c r="M60">
-        <v>14049.182500000001</v>
+        <v>14049.183000000001</v>
       </c>
       <c r="N60">
         <v>2387.8009999999999</v>
@@ -5167,13 +5161,13 @@
         <v>326.18639999999999</v>
       </c>
       <c r="K61">
-        <v>881.89</v>
+        <v>881.89400000000001</v>
       </c>
       <c r="L61">
-        <v>1144.99</v>
+        <v>1144.9949999999999</v>
       </c>
       <c r="M61">
-        <v>13849.6605</v>
+        <v>13849.661</v>
       </c>
       <c r="N61">
         <v>2274.5349999999999</v>
@@ -5241,13 +5235,13 @@
         <v>329.36090000000002</v>
       </c>
       <c r="K62">
-        <v>898.79</v>
+        <v>898.79399999999998</v>
       </c>
       <c r="L62">
-        <v>1161.99</v>
+        <v>1161.9860000000001</v>
       </c>
       <c r="M62">
-        <v>14127.8858</v>
+        <v>14127.886</v>
       </c>
       <c r="N62">
         <v>2392.2849999999999</v>
@@ -5315,13 +5309,13 @@
         <v>332.83499999999998</v>
       </c>
       <c r="K63">
-        <v>909.63</v>
+        <v>909.63199999999995</v>
       </c>
       <c r="L63">
-        <v>1161.73</v>
+        <v>1161.7260000000001</v>
       </c>
       <c r="M63">
-        <v>14095.6423</v>
+        <v>14095.642</v>
       </c>
       <c r="N63">
         <v>2344.402</v>
@@ -5389,13 +5383,13 @@
         <v>336.41629999999998</v>
       </c>
       <c r="K64">
-        <v>922.59</v>
+        <v>922.58799999999997</v>
       </c>
       <c r="L64">
-        <v>1155.73</v>
+        <v>1155.731</v>
       </c>
       <c r="M64">
-        <v>14091.388800000001</v>
+        <v>14091.388999999999</v>
       </c>
       <c r="N64">
         <v>2295.8310000000001</v>
@@ -5463,13 +5457,13 @@
         <v>337.67520000000002</v>
       </c>
       <c r="K65">
-        <v>930.2</v>
+        <v>930.197</v>
       </c>
       <c r="L65">
         <v>1143.44</v>
       </c>
       <c r="M65">
-        <v>13832.4846</v>
+        <v>13832.485000000001</v>
       </c>
       <c r="N65">
         <v>2184.299</v>
@@ -5537,13 +5531,13 @@
         <v>339.029</v>
       </c>
       <c r="K66">
-        <v>937.1</v>
+        <v>937.10199999999998</v>
       </c>
       <c r="L66">
-        <v>1146.95</v>
+        <v>1146.953</v>
       </c>
       <c r="M66">
-        <v>13823.5672</v>
+        <v>13823.566999999999</v>
       </c>
       <c r="N66">
         <v>2186.8069999999998</v>
@@ -5611,13 +5605,13 @@
         <v>341.51690000000002</v>
       </c>
       <c r="K67">
-        <v>951.96</v>
+        <v>951.96299999999997</v>
       </c>
       <c r="L67">
-        <v>1154.3599999999999</v>
+        <v>1154.355</v>
       </c>
       <c r="M67">
-        <v>13964.716700000001</v>
+        <v>13964.717000000001</v>
       </c>
       <c r="N67">
         <v>2214.6790000000001</v>
@@ -5759,10 +5753,10 @@
         <v>346.68119999999999</v>
       </c>
       <c r="K69">
-        <v>969.53</v>
+        <v>969.52599999999995</v>
       </c>
       <c r="L69">
-        <v>1154.5</v>
+        <v>1154.5029999999999</v>
       </c>
       <c r="M69">
         <v>14081.665999999999</v>
@@ -5833,13 +5827,13 @@
         <v>349.62169999999998</v>
       </c>
       <c r="K70">
-        <v>979.52</v>
+        <v>979.51800000000003</v>
       </c>
       <c r="L70">
-        <v>1154.83</v>
+        <v>1154.826</v>
       </c>
       <c r="M70">
-        <v>14139.034299999999</v>
+        <v>14139.034</v>
       </c>
       <c r="N70">
         <v>2296.1260000000002</v>
@@ -5907,13 +5901,13 @@
         <v>352.2414</v>
       </c>
       <c r="K71">
-        <v>997.71</v>
+        <v>997.70799999999997</v>
       </c>
       <c r="L71">
-        <v>1160.57</v>
+        <v>1160.5719999999999</v>
       </c>
       <c r="M71">
-        <v>14231.3532</v>
+        <v>14231.352999999999</v>
       </c>
       <c r="N71">
         <v>2384.665</v>
@@ -5981,13 +5975,13 @@
         <v>353.04329999999999</v>
       </c>
       <c r="K72">
-        <v>992.41</v>
+        <v>992.41099999999994</v>
       </c>
       <c r="L72">
-        <v>1149.57</v>
+        <v>1149.5719999999999</v>
       </c>
       <c r="M72">
-        <v>14053.3143</v>
+        <v>14053.314</v>
       </c>
       <c r="N72">
         <v>2297.422</v>
@@ -6055,13 +6049,13 @@
         <v>351.11869999999999</v>
       </c>
       <c r="K73">
-        <v>966.25</v>
+        <v>966.25099999999998</v>
       </c>
       <c r="L73">
-        <v>1141.97</v>
+        <v>1141.9670000000001</v>
       </c>
       <c r="M73">
-        <v>13832.831399999999</v>
+        <v>13832.831</v>
       </c>
       <c r="N73">
         <v>2231.511</v>
@@ -6129,13 +6123,13 @@
         <v>354.86489999999998</v>
       </c>
       <c r="K74">
-        <v>984.42</v>
+        <v>984.42200000000003</v>
       </c>
       <c r="L74">
-        <v>1135.83</v>
+        <v>1135.8340000000001</v>
       </c>
       <c r="M74">
-        <v>13825.0689</v>
+        <v>13825.069</v>
       </c>
       <c r="N74">
         <v>2213.9580000000001</v>
@@ -6203,10 +6197,10 @@
         <v>354.99880000000002</v>
       </c>
       <c r="K75">
-        <v>978.32</v>
+        <v>978.31799999999998</v>
       </c>
       <c r="L75">
-        <v>1126.32</v>
+        <v>1126.316</v>
       </c>
       <c r="M75">
         <v>13675.416999999999</v>
@@ -6277,13 +6271,13 @@
         <v>356.03160000000003</v>
       </c>
       <c r="K76">
-        <v>988.02</v>
+        <v>988.01700000000005</v>
       </c>
       <c r="L76">
-        <v>1123.3499999999999</v>
+        <v>1123.3520000000001</v>
       </c>
       <c r="M76">
-        <v>13652.6752</v>
+        <v>13652.674999999999</v>
       </c>
       <c r="N76">
         <v>2145.154</v>
@@ -6351,13 +6345,13 @@
         <v>358.88979999999998</v>
       </c>
       <c r="K77">
-        <v>1012.31</v>
+        <v>1012.3049999999999</v>
       </c>
       <c r="L77">
-        <v>1130.57</v>
+        <v>1130.566</v>
       </c>
       <c r="M77">
-        <v>13765.9161</v>
+        <v>13765.915999999999</v>
       </c>
       <c r="N77">
         <v>2199.8159999999998</v>
@@ -6425,13 +6419,13 @@
         <v>360.60160000000002</v>
       </c>
       <c r="K78">
-        <v>1017.01</v>
+        <v>1017.013</v>
       </c>
       <c r="L78">
-        <v>1134.19</v>
+        <v>1134.1869999999999</v>
       </c>
       <c r="M78">
-        <v>13838.021500000001</v>
+        <v>13838.022000000001</v>
       </c>
       <c r="N78">
         <v>2259.2640000000001</v>
@@ -6499,13 +6493,13 @@
         <v>362.5283</v>
       </c>
       <c r="K79">
-        <v>1022.59</v>
+        <v>1022.586</v>
       </c>
       <c r="L79">
-        <v>1133.6600000000001</v>
+        <v>1133.6610000000001</v>
       </c>
       <c r="M79">
-        <v>13903.1242</v>
+        <v>13903.124</v>
       </c>
       <c r="N79">
         <v>2273.8609999999999</v>
@@ -6573,13 +6567,13 @@
         <v>365.08629999999999</v>
       </c>
       <c r="K80">
-        <v>1030.1500000000001</v>
+        <v>1030.1510000000001</v>
       </c>
       <c r="L80">
         <v>1132.8900000000001</v>
       </c>
       <c r="M80">
-        <v>13784.743899999999</v>
+        <v>13784.744000000001</v>
       </c>
       <c r="N80">
         <v>2171.3519999999999</v>
@@ -6647,13 +6641,13 @@
         <v>365.90249999999997</v>
       </c>
       <c r="K81">
-        <v>1050.8</v>
+        <v>1050.797</v>
       </c>
       <c r="L81">
         <v>1124.3699999999999</v>
       </c>
       <c r="M81">
-        <v>13983.1011</v>
+        <v>13983.101000000001</v>
       </c>
       <c r="N81">
         <v>2185.3049999999998</v>
@@ -6721,13 +6715,13 @@
         <v>367.24169999999998</v>
       </c>
       <c r="K82">
-        <v>1053.23</v>
+        <v>1053.229</v>
       </c>
       <c r="L82">
         <v>1121.8599999999999</v>
       </c>
       <c r="M82">
-        <v>13857.130499999999</v>
+        <v>13857.130999999999</v>
       </c>
       <c r="N82">
         <v>2139.87</v>
@@ -6795,13 +6789,13 @@
         <v>368.08049999999997</v>
       </c>
       <c r="K83">
-        <v>1060.53</v>
+        <v>1060.5250000000001</v>
       </c>
       <c r="L83">
         <v>1115.6099999999999</v>
       </c>
       <c r="M83">
-        <v>13865.789500000001</v>
+        <v>13865.79</v>
       </c>
       <c r="N83">
         <v>2162.9859999999999</v>
@@ -6869,13 +6863,13 @@
         <v>370.34370000000001</v>
       </c>
       <c r="K84">
-        <v>1071.2</v>
+        <v>1071.203</v>
       </c>
       <c r="L84">
         <v>1124.43</v>
       </c>
       <c r="M84">
-        <v>13944.688599999999</v>
+        <v>13944.689</v>
       </c>
       <c r="N84">
         <v>2227.085</v>
@@ -6943,13 +6937,13 @@
         <v>372.57870000000003</v>
       </c>
       <c r="K85">
-        <v>1080.26</v>
+        <v>1080.2560000000001</v>
       </c>
       <c r="L85">
         <v>1125.3599999999999</v>
       </c>
       <c r="M85">
-        <v>14041.676299999999</v>
+        <v>14041.675999999999</v>
       </c>
       <c r="N85">
         <v>2258.1</v>
@@ -7017,13 +7011,13 @@
         <v>372.416</v>
       </c>
       <c r="K86">
-        <v>1065.97</v>
+        <v>1065.971</v>
       </c>
       <c r="L86">
         <v>1131.24</v>
       </c>
       <c r="M86">
-        <v>13986.182199999999</v>
+        <v>13986.182000000001</v>
       </c>
       <c r="N86">
         <v>2234.0169999999998</v>
@@ -7091,13 +7085,13 @@
         <v>373.2801</v>
       </c>
       <c r="K87">
-        <v>1082.17</v>
+        <v>1082.174</v>
       </c>
       <c r="L87">
         <v>1144.9000000000001</v>
       </c>
       <c r="M87">
-        <v>14195.9997</v>
+        <v>14196</v>
       </c>
       <c r="N87">
         <v>2357.018</v>
@@ -7165,13 +7159,13 @@
         <v>371.35480000000001</v>
       </c>
       <c r="K88">
-        <v>1059.47</v>
+        <v>1059.4670000000001</v>
       </c>
       <c r="L88">
         <v>1162.53</v>
       </c>
       <c r="M88">
-        <v>14349.293299999999</v>
+        <v>14349.293</v>
       </c>
       <c r="N88">
         <v>2435.6019999999999</v>
@@ -7239,13 +7233,13 @@
         <v>372.41359999999997</v>
       </c>
       <c r="K89">
-        <v>1071.53</v>
+        <v>1071.528</v>
       </c>
       <c r="L89">
         <v>1169.58</v>
       </c>
       <c r="M89">
-        <v>14320.528399999999</v>
+        <v>14320.528</v>
       </c>
       <c r="N89">
         <v>2478.6019999999999</v>
@@ -7313,13 +7307,13 @@
         <v>374.10939999999999</v>
       </c>
       <c r="K90">
-        <v>1063.8699999999999</v>
+        <v>1063.8689999999999</v>
       </c>
       <c r="L90">
         <v>1189.05</v>
       </c>
       <c r="M90">
-        <v>14642.9534</v>
+        <v>14642.953</v>
       </c>
       <c r="N90">
         <v>2659.299</v>
@@ -7387,13 +7381,13 @@
         <v>369.9796</v>
       </c>
       <c r="K91">
-        <v>1048.18</v>
+        <v>1048.184</v>
       </c>
       <c r="L91">
         <v>1193.05</v>
       </c>
       <c r="M91">
-        <v>14678.342500000001</v>
+        <v>14678.343000000001</v>
       </c>
       <c r="N91">
         <v>2721.7869999999998</v>
@@ -7461,13 +7455,13 @@
         <v>370.92840000000001</v>
       </c>
       <c r="K92">
-        <v>1055.4100000000001</v>
+        <v>1055.413</v>
       </c>
       <c r="L92">
         <v>1216.8399999999999</v>
       </c>
       <c r="M92">
-        <v>15047.019700000001</v>
+        <v>15047.02</v>
       </c>
       <c r="N92">
         <v>2861.0079999999998</v>
@@ -7535,13 +7529,13 @@
         <v>376.14550000000003</v>
       </c>
       <c r="K93">
-        <v>1080.5899999999999</v>
+        <v>1080.5930000000001</v>
       </c>
       <c r="L93">
         <v>1224.99</v>
       </c>
       <c r="M93">
-        <v>15076.506100000001</v>
+        <v>15076.505999999999</v>
       </c>
       <c r="N93">
         <v>2855.143</v>
@@ -7609,13 +7603,13 @@
         <v>377.6302</v>
       </c>
       <c r="K94">
-        <v>1074.8499999999999</v>
+        <v>1074.8530000000001</v>
       </c>
       <c r="L94">
         <v>1233.6400000000001</v>
       </c>
       <c r="M94">
-        <v>15161.163200000001</v>
+        <v>15161.163</v>
       </c>
       <c r="N94">
         <v>2929.2930000000001</v>
@@ -7757,13 +7751,13 @@
         <v>381.7903</v>
       </c>
       <c r="K96">
-        <v>1090.96</v>
+        <v>1090.962</v>
       </c>
       <c r="L96">
         <v>1209.01</v>
       </c>
       <c r="M96">
-        <v>14972.890299999999</v>
+        <v>14972.89</v>
       </c>
       <c r="N96">
         <v>2789.703</v>
@@ -7831,13 +7825,13 @@
         <v>380.59679999999997</v>
       </c>
       <c r="K97">
-        <v>1074.32</v>
+        <v>1074.3209999999999</v>
       </c>
       <c r="L97">
         <v>1176.9000000000001</v>
       </c>
       <c r="M97">
-        <v>14626.769899999999</v>
+        <v>14626.77</v>
       </c>
       <c r="N97">
         <v>2654.02</v>
@@ -7905,13 +7899,13 @@
         <v>380.9366</v>
       </c>
       <c r="K98">
-        <v>1067.71</v>
+        <v>1067.7070000000001</v>
       </c>
       <c r="L98">
         <v>1204.1199999999999</v>
       </c>
       <c r="M98">
-        <v>14757.0355</v>
+        <v>14757.036</v>
       </c>
       <c r="N98">
         <v>2760.348</v>
@@ -7979,13 +7973,13 @@
         <v>378.45819999999998</v>
       </c>
       <c r="K99">
-        <v>1048.9000000000001</v>
+        <v>1048.903</v>
       </c>
       <c r="L99">
         <v>1181.02</v>
       </c>
       <c r="M99">
-        <v>14520.1258</v>
+        <v>14520.126</v>
       </c>
       <c r="N99">
         <v>2701.4830000000002</v>
@@ -8053,13 +8047,13 @@
         <v>375.935</v>
       </c>
       <c r="K100">
-        <v>1021.69</v>
+        <v>1021.693</v>
       </c>
       <c r="L100">
         <v>1174.48</v>
       </c>
       <c r="M100">
-        <v>14513.8194</v>
+        <v>14513.819</v>
       </c>
       <c r="N100">
         <v>2763.31</v>
@@ -8127,13 +8121,13 @@
         <v>375.42520000000002</v>
       </c>
       <c r="K101">
-        <v>1049.54</v>
+        <v>1049.5440000000001</v>
       </c>
       <c r="L101">
         <v>1163.3900000000001</v>
       </c>
       <c r="M101">
-        <v>14501.5378</v>
+        <v>14501.538</v>
       </c>
       <c r="N101">
         <v>2691.3589999999999</v>
@@ -8201,7 +8195,7 @@
         <v>372.08960000000002</v>
       </c>
       <c r="K102">
-        <v>1025.98</v>
+        <v>1025.982</v>
       </c>
       <c r="L102">
         <v>1186.28</v>
@@ -8275,7 +8269,7 @@
         <v>368.55599999999998</v>
       </c>
       <c r="K103">
-        <v>999.52</v>
+        <v>999.51700000000005</v>
       </c>
       <c r="L103">
         <v>1169.6199999999999</v>
@@ -8349,7 +8343,7 @@
         <v>365.88080000000002</v>
       </c>
       <c r="K104">
-        <v>983.71</v>
+        <v>983.70799999999997</v>
       </c>
       <c r="L104">
         <v>1180.24</v>
@@ -8423,7 +8417,7 @@
         <v>363.84429999999998</v>
       </c>
       <c r="K105">
-        <v>988.28</v>
+        <v>988.28300000000002</v>
       </c>
       <c r="L105">
         <v>1183.75</v>
@@ -8497,7 +8491,7 @@
         <v>373.45389999999998</v>
       </c>
       <c r="K106">
-        <v>1031.97</v>
+        <v>1031.9690000000001</v>
       </c>
       <c r="L106">
         <v>1170.55</v>
@@ -8571,7 +8565,7 @@
         <v>380.5421</v>
       </c>
       <c r="K107">
-        <v>1073.2</v>
+        <v>1073.204</v>
       </c>
       <c r="L107">
         <v>1174.4100000000001</v>
@@ -8645,7 +8639,7 @@
         <v>384.01139999999998</v>
       </c>
       <c r="K108">
-        <v>1080.95</v>
+        <v>1080.9480000000001</v>
       </c>
       <c r="L108">
         <v>1154.26</v>
@@ -8719,7 +8713,7 @@
         <v>384.13850000000002</v>
       </c>
       <c r="K109">
-        <v>1092.6600000000001</v>
+        <v>1092.664</v>
       </c>
       <c r="L109">
         <v>1165.76</v>
@@ -8793,7 +8787,7 @@
         <v>389.53660000000002</v>
       </c>
       <c r="K110">
-        <v>1120.26</v>
+        <v>1120.2619999999999</v>
       </c>
       <c r="L110">
         <v>1169.28</v>
@@ -8867,7 +8861,7 @@
         <v>392.6105</v>
       </c>
       <c r="K111">
-        <v>1145.21</v>
+        <v>1145.2149999999999</v>
       </c>
       <c r="L111">
         <v>1157.81</v>
@@ -8941,7 +8935,7 @@
         <v>396.03949999999998</v>
       </c>
       <c r="K112">
-        <v>1152.6199999999999</v>
+        <v>1152.624</v>
       </c>
       <c r="L112">
         <v>1156.1199999999999</v>
@@ -9015,7 +9009,7 @@
         <v>399.08030000000002</v>
       </c>
       <c r="K113">
-        <v>1156.23</v>
+        <v>1156.2260000000001</v>
       </c>
       <c r="L113">
         <v>1137.8</v>
@@ -9089,7 +9083,7 @@
         <v>400.37619999999998</v>
       </c>
       <c r="K114">
-        <v>1151.67</v>
+        <v>1151.6659999999999</v>
       </c>
       <c r="L114">
         <v>1129.95</v>
@@ -9163,7 +9157,7 @@
         <v>404.9606</v>
       </c>
       <c r="K115">
-        <v>1174.32</v>
+        <v>1174.319</v>
       </c>
       <c r="L115">
         <v>1135.3599999999999</v>
@@ -9237,7 +9231,7 @@
         <v>407.12240000000003</v>
       </c>
       <c r="K116">
-        <v>1190.0899999999999</v>
+        <v>1190.088</v>
       </c>
       <c r="L116">
         <v>1124.55</v>
@@ -9311,7 +9305,7 @@
         <v>409.50909999999999</v>
       </c>
       <c r="K117">
-        <v>1208.6600000000001</v>
+        <v>1208.6590000000001</v>
       </c>
       <c r="L117">
         <v>1137.81</v>
@@ -9385,7 +9379,7 @@
         <v>409.8263</v>
       </c>
       <c r="K118">
-        <v>1206.1199999999999</v>
+        <v>1206.123</v>
       </c>
       <c r="L118">
         <v>1126.77</v>
@@ -9459,7 +9453,7 @@
         <v>411.61130000000003</v>
       </c>
       <c r="K119">
-        <v>1219.79</v>
+        <v>1219.789</v>
       </c>
       <c r="L119">
         <v>1126.01</v>
@@ -9533,7 +9527,7 @@
         <v>413.17660000000001</v>
       </c>
       <c r="K120">
-        <v>1230.68</v>
+        <v>1230.684</v>
       </c>
       <c r="L120">
         <v>1131.48</v>
@@ -9607,7 +9601,7 @@
         <v>412.91320000000002</v>
       </c>
       <c r="K121">
-        <v>1231.98</v>
+        <v>1231.9829999999999</v>
       </c>
       <c r="L121">
         <v>1126.83</v>
@@ -9681,7 +9675,7 @@
         <v>416.14530000000002</v>
       </c>
       <c r="K122">
-        <v>1246.19</v>
+        <v>1246.193</v>
       </c>
       <c r="L122">
         <v>1137.44</v>
@@ -9829,7 +9823,7 @@
         <v>417.27420000000001</v>
       </c>
       <c r="K124">
-        <v>1257.06</v>
+        <v>1257.0630000000001</v>
       </c>
       <c r="L124">
         <v>1134.28</v>
@@ -9903,7 +9897,7 @@
         <v>420.03120000000001</v>
       </c>
       <c r="K125">
-        <v>1261.9100000000001</v>
+        <v>1261.914</v>
       </c>
       <c r="L125">
         <v>1156.0899999999999</v>
@@ -9977,7 +9971,7 @@
         <v>420.53440000000001</v>
       </c>
       <c r="K126">
-        <v>1258.53</v>
+        <v>1258.528</v>
       </c>
       <c r="L126">
         <v>1154.3499999999999</v>
@@ -10051,7 +10045,7 @@
         <v>422.16019999999997</v>
       </c>
       <c r="K127">
-        <v>1262.2</v>
+        <v>1262.1959999999999</v>
       </c>
       <c r="L127">
         <v>1163.8699999999999</v>
@@ -10125,7 +10119,7 @@
         <v>426.71300000000002</v>
       </c>
       <c r="K128">
-        <v>1270.29</v>
+        <v>1270.289</v>
       </c>
       <c r="L128">
         <v>1208.0999999999999</v>
@@ -10199,7 +10193,7 @@
         <v>427.47710000000001</v>
       </c>
       <c r="K129">
-        <v>1258.45</v>
+        <v>1258.4459999999999</v>
       </c>
       <c r="L129">
         <v>1149.3900000000001</v>
@@ -10273,7 +10267,7 @@
         <v>428.83859999999999</v>
       </c>
       <c r="K130">
-        <v>1250.68</v>
+        <v>1250.6769999999999</v>
       </c>
       <c r="L130">
         <v>1140.28</v>
@@ -10347,7 +10341,7 @@
         <v>430.92849999999999</v>
       </c>
       <c r="K131">
-        <v>1259</v>
+        <v>1258.9960000000001</v>
       </c>
       <c r="L131">
         <v>1145.54</v>
@@ -10421,7 +10415,7 @@
         <v>431.76209999999998</v>
       </c>
       <c r="K132">
-        <v>1258.81</v>
+        <v>1258.806</v>
       </c>
       <c r="L132">
         <v>1141.3699999999999</v>
@@ -10495,7 +10489,7 @@
         <v>432.1986</v>
       </c>
       <c r="K133">
-        <v>1263.1500000000001</v>
+        <v>1263.153</v>
       </c>
       <c r="L133">
         <v>1142.77</v>
@@ -10569,7 +10563,7 @@
         <v>435.77850000000001</v>
       </c>
       <c r="K134">
-        <v>1277.27</v>
+        <v>1277.268</v>
       </c>
       <c r="L134">
         <v>1130.1600000000001</v>
@@ -10643,7 +10637,7 @@
         <v>437.56849999999997</v>
       </c>
       <c r="K135">
-        <v>1286.52</v>
+        <v>1286.518</v>
       </c>
       <c r="L135">
         <v>1157.3699999999999</v>
@@ -10717,7 +10711,7 @@
         <v>440.55239999999998</v>
       </c>
       <c r="K136">
-        <v>1293.99</v>
+        <v>1293.9939999999999</v>
       </c>
       <c r="L136">
         <v>1150.1099999999999</v>
@@ -10791,7 +10785,7 @@
         <v>440.57920000000001</v>
       </c>
       <c r="K137">
-        <v>1272.8</v>
+        <v>1272.8030000000001</v>
       </c>
       <c r="L137">
         <v>1119.6300000000001</v>
@@ -10865,7 +10859,7 @@
         <v>436.98590000000002</v>
       </c>
       <c r="K138">
-        <v>1261.25</v>
+        <v>1261.2529999999999</v>
       </c>
       <c r="L138">
         <v>1117.54</v>
@@ -10939,7 +10933,7 @@
         <v>426.97919999999999</v>
       </c>
       <c r="K139">
-        <v>1233.6099999999999</v>
+        <v>1233.6079999999999</v>
       </c>
       <c r="L139">
         <v>1126.0899999999999</v>
@@ -11013,7 +11007,7 @@
         <v>436.80489999999998</v>
       </c>
       <c r="K140">
-        <v>1290.27</v>
+        <v>1290.2670000000001</v>
       </c>
       <c r="L140">
         <v>1104.58</v>
@@ -11087,7 +11081,7 @@
         <v>443.65249999999997</v>
       </c>
       <c r="K141">
-        <v>1312.05</v>
+        <v>1312.0530000000001</v>
       </c>
       <c r="L141">
         <v>1112.99</v>
@@ -11161,10 +11155,10 @@
         <v>443.11380000000003</v>
       </c>
       <c r="K142">
-        <v>1324.91</v>
+        <v>1324.9090000000001</v>
       </c>
       <c r="L142">
-        <v>1116.33</v>
+        <v>1116.328</v>
       </c>
       <c r="M142">
         <v>14681.66</v>
@@ -11235,10 +11229,10 @@
         <v>450.14179999999999</v>
       </c>
       <c r="K143">
-        <v>1343.45</v>
+        <v>1343.4449999999999</v>
       </c>
       <c r="L143">
-        <v>1129.1300000000001</v>
+        <v>1129.1289999999999</v>
       </c>
       <c r="M143">
         <v>14836.621999999999</v>
@@ -11309,10 +11303,10 @@
         <v>449.12759999999997</v>
       </c>
       <c r="K144">
-        <v>1326.37</v>
+        <v>1326.3689999999999</v>
       </c>
       <c r="L144">
-        <v>1126.0899999999999</v>
+        <v>1126.0940000000001</v>
       </c>
       <c r="M144">
         <v>14707.329</v>
@@ -11383,7 +11377,7 @@
         <v>450.11630000000002</v>
       </c>
       <c r="K145">
-        <v>1358.89</v>
+        <v>1358.893</v>
       </c>
       <c r="L145">
         <v>1155.1099999999999</v>
@@ -11457,7 +11451,7 @@
         <v>453.63990000000001</v>
       </c>
       <c r="K146">
-        <v>1365.85</v>
+        <v>1365.8510000000001</v>
       </c>
       <c r="L146">
         <v>1176.26</v>
@@ -11531,7 +11525,7 @@
         <v>452.3603</v>
       </c>
       <c r="K147">
-        <v>1371.18</v>
+        <v>1371.181</v>
       </c>
       <c r="L147">
         <v>1195.94</v>
@@ -11605,7 +11599,7 @@
         <v>454.2679</v>
       </c>
       <c r="K148">
-        <v>1375.53</v>
+        <v>1375.528</v>
       </c>
       <c r="L148">
         <v>1183.01</v>
@@ -11679,7 +11673,7 @@
         <v>452.06330000000003</v>
       </c>
       <c r="K149">
-        <v>1378.72</v>
+        <v>1378.722</v>
       </c>
       <c r="L149">
         <v>1166.43</v>
@@ -11753,7 +11747,7 @@
         <v>454.55160000000001</v>
       </c>
       <c r="K150">
-        <v>1382.49</v>
+        <v>1382.4870000000001</v>
       </c>
       <c r="L150">
         <v>1177.05</v>
@@ -11827,7 +11821,7 @@
         <v>461.8843</v>
       </c>
       <c r="K151">
-        <v>1411.39</v>
+        <v>1411.3869999999999</v>
       </c>
       <c r="L151">
         <v>1180.6199999999999</v>
@@ -11901,7 +11895,7 @@
         <v>464.33879999999999</v>
       </c>
       <c r="K152">
-        <v>1411.45</v>
+        <v>1411.4469999999999</v>
       </c>
       <c r="L152">
         <v>1190.33</v>
@@ -11975,7 +11969,7 @@
         <v>458.06479999999999</v>
       </c>
       <c r="K153">
-        <v>1389.57</v>
+        <v>1389.5709999999999</v>
       </c>
       <c r="L153">
         <v>1176.22</v>
@@ -12049,7 +12043,7 @@
         <v>400.9701</v>
       </c>
       <c r="K154">
-        <v>1226.17</v>
+        <v>1226.174</v>
       </c>
       <c r="L154">
         <v>1166.67</v>
@@ -12123,7 +12117,7 @@
         <v>418.16950000000003</v>
       </c>
       <c r="K155">
-        <v>1272.77</v>
+        <v>1272.7729999999999</v>
       </c>
       <c r="L155">
         <v>1172.4100000000001</v>
@@ -12197,7 +12191,7 @@
         <v>434.06650000000002</v>
       </c>
       <c r="K156">
-        <v>1330.99</v>
+        <v>1330.9849999999999</v>
       </c>
       <c r="L156">
         <v>1175.5</v>
@@ -12271,7 +12265,7 @@
         <v>439.91300000000001</v>
       </c>
       <c r="K157">
-        <v>1343.96</v>
+        <v>1343.9580000000001</v>
       </c>
       <c r="L157">
         <v>1172.0999999999999</v>
@@ -12345,7 +12339,7 @@
         <v>448.18779999999998</v>
       </c>
       <c r="K158">
-        <v>1408.17</v>
+        <v>1408.173</v>
       </c>
       <c r="L158">
         <v>1192.95</v>
@@ -12493,7 +12487,7 @@
         <v>458.06110000000001</v>
       </c>
       <c r="K160">
-        <v>1407.21</v>
+        <v>1407.2059999999999</v>
       </c>
       <c r="L160">
         <v>1181.9000000000001</v>
@@ -12567,7 +12561,7 @@
         <v>458.85820000000001</v>
       </c>
       <c r="K161">
-        <v>1413.79</v>
+        <v>1413.7860000000001</v>
       </c>
       <c r="L161">
         <v>1175.82</v>
@@ -12641,7 +12635,7 @@
         <v>468.62920000000003</v>
       </c>
       <c r="K162">
-        <v>1470.38</v>
+        <v>1470.376</v>
       </c>
       <c r="L162">
         <v>1195.79</v>
@@ -12715,7 +12709,7 @@
         <v>474.71800000000002</v>
       </c>
       <c r="K163">
-        <v>1498.42</v>
+        <v>1498.421</v>
       </c>
       <c r="L163">
         <v>1231.32</v>
@@ -12789,7 +12783,7 @@
         <v>480.7278</v>
       </c>
       <c r="K164">
-        <v>1504.16</v>
+        <v>1504.1559999999999</v>
       </c>
       <c r="L164">
         <v>1224.18</v>
@@ -12863,7 +12857,7 @@
         <v>483.96280000000002</v>
       </c>
       <c r="K165">
-        <v>1509.4</v>
+        <v>1509.3969999999999</v>
       </c>
       <c r="L165">
         <v>1240.02</v>
@@ -12937,7 +12931,7 @@
         <v>484.25209999999998</v>
       </c>
       <c r="K166">
-        <v>1511.97</v>
+        <v>1511.9670000000001</v>
       </c>
       <c r="L166">
         <v>1237.72</v>
@@ -13011,7 +13005,7 @@
         <v>486.71570000000003</v>
       </c>
       <c r="K167">
-        <v>1528.55</v>
+        <v>1528.5519999999999</v>
       </c>
       <c r="L167">
         <v>1251.33</v>
@@ -13085,7 +13079,7 @@
         <v>489.24040000000002</v>
       </c>
       <c r="K168">
-        <v>1532.96</v>
+        <v>1532.9639999999999</v>
       </c>
       <c r="L168">
         <v>1258.02</v>
@@ -13159,7 +13153,7 @@
         <v>491.24099999999999</v>
       </c>
       <c r="K169">
-        <v>1553.91</v>
+        <v>1553.9090000000001</v>
       </c>
       <c r="L169">
         <v>1250.5</v>
@@ -13307,7 +13301,7 @@
         <v>493.61149999999998</v>
       </c>
       <c r="K171">
-        <v>1567.95</v>
+        <v>1567.9449999999999</v>
       </c>
       <c r="L171">
         <v>1247.31</v>
@@ -13381,7 +13375,7 @@
         <v>496.8091</v>
       </c>
       <c r="K172">
-        <v>1568.47</v>
+        <v>1568.471</v>
       </c>
       <c r="L172">
         <v>1231.8599999999999</v>
@@ -13455,7 +13449,7 @@
         <v>497.9812</v>
       </c>
       <c r="K173">
-        <v>1565.68</v>
+        <v>1565.681</v>
       </c>
       <c r="L173">
         <v>1244.81</v>
@@ -13529,7 +13523,7 @@
         <v>497.22050000000002</v>
       </c>
       <c r="K174">
-        <v>1549.64</v>
+        <v>1549.636</v>
       </c>
       <c r="L174">
         <v>1210.92</v>
@@ -13686,7 +13680,7 @@
         <v>17491.125</v>
       </c>
       <c r="N176">
-        <v>3145.7220000000002</v>
+        <v>3145.6610000000001</v>
       </c>
       <c r="O176">
         <v>1759.42</v>
@@ -13751,7 +13745,7 @@
         <v>499.65269999999998</v>
       </c>
       <c r="K177">
-        <v>1521.6</v>
+        <v>1521.604</v>
       </c>
       <c r="L177">
         <v>1194.8599999999999</v>
@@ -13760,7 +13754,7 @@
         <v>17708.370999999999</v>
       </c>
       <c r="N177">
-        <v>3261.5569999999998</v>
+        <v>3261.4670000000001</v>
       </c>
       <c r="O177">
         <v>1779.61</v>
@@ -13825,7 +13819,7 @@
         <v>499.84949999999998</v>
       </c>
       <c r="K178">
-        <v>1507.53</v>
+        <v>1507.5250000000001</v>
       </c>
       <c r="L178">
         <v>1231.8699999999999</v>
@@ -13834,7 +13828,7 @@
         <v>18513.787</v>
       </c>
       <c r="N178">
-        <v>3576.8649999999998</v>
+        <v>3576.799</v>
       </c>
       <c r="O178">
         <v>1708.65</v>
@@ -13899,7 +13893,7 @@
         <v>500.70659999999998</v>
       </c>
       <c r="K179">
-        <v>1452.69</v>
+        <v>1452.6869999999999</v>
       </c>
       <c r="L179">
         <v>1255.32</v>
@@ -13908,7 +13902,7 @@
         <v>19027.263999999999</v>
       </c>
       <c r="N179">
-        <v>3829.3389999999999</v>
+        <v>3829.2640000000001</v>
       </c>
       <c r="O179">
         <v>1718.69</v>
@@ -13973,7 +13967,7 @@
         <v>488.13490000000002</v>
       </c>
       <c r="K180">
-        <v>1456.32</v>
+        <v>1456.3240000000001</v>
       </c>
       <c r="L180">
         <v>1243.99</v>
@@ -13982,7 +13976,7 @@
         <v>18991.223000000002</v>
       </c>
       <c r="N180">
-        <v>3821.6329999999998</v>
+        <v>3821.616</v>
       </c>
       <c r="O180">
         <v>1718.69</v>
@@ -14047,7 +14041,7 @@
         <v>478.0942</v>
       </c>
       <c r="K181">
-        <v>1357.2</v>
+        <v>1357.1969999999999</v>
       </c>
       <c r="L181">
         <v>1261.07</v>
@@ -14056,7 +14050,7 @@
         <v>18830.867999999999</v>
       </c>
       <c r="N181">
-        <v>3919.7809999999999</v>
+        <v>3919.8330000000001</v>
       </c>
       <c r="O181">
         <v>1718.69</v>
@@ -14130,7 +14124,7 @@
         <v>18679.645</v>
       </c>
       <c r="N182">
-        <v>3747.0160000000001</v>
+        <v>3747.049</v>
       </c>
       <c r="O182">
         <v>1718.69</v>
@@ -14195,7 +14189,7 @@
         <v>494.48860000000002</v>
       </c>
       <c r="K183">
-        <v>1404.48</v>
+        <v>1404.481</v>
       </c>
       <c r="L183">
         <v>1257.82</v>
@@ -14204,7 +14198,7 @@
         <v>18922.542000000001</v>
       </c>
       <c r="N183">
-        <v>3896.473</v>
+        <v>3896.4749999999999</v>
       </c>
       <c r="O183">
         <v>1718.69</v>
@@ -14269,7 +14263,7 @@
         <v>483.77879999999999</v>
       </c>
       <c r="K184">
-        <v>1348</v>
+        <v>1347.9949999999999</v>
       </c>
       <c r="L184">
         <v>1295.3699999999999</v>
@@ -14278,7 +14272,7 @@
         <v>19166.885999999999</v>
       </c>
       <c r="N184">
-        <v>4120.9750000000004</v>
+        <v>4121.0169999999998</v>
       </c>
       <c r="O184">
         <v>1718.69</v>
@@ -14343,7 +14337,7 @@
         <v>487.8895</v>
       </c>
       <c r="K185">
-        <v>1386.37</v>
+        <v>1386.3679999999999</v>
       </c>
       <c r="L185">
         <v>1297.27</v>
@@ -14352,7 +14346,7 @@
         <v>19286.981</v>
       </c>
       <c r="N185">
-        <v>4128.7719999999999</v>
+        <v>4128.8620000000001</v>
       </c>
       <c r="O185">
         <v>1718.69</v>
@@ -14426,7 +14420,7 @@
         <v>18880.728999999999</v>
       </c>
       <c r="N186">
-        <v>3879.6979999999999</v>
+        <v>3879.7849999999999</v>
       </c>
       <c r="O186">
         <v>1718.69</v>
@@ -14491,16 +14485,16 @@
         <v>495.06270000000001</v>
       </c>
       <c r="K187">
-        <v>1401.68</v>
+        <v>1401.683</v>
       </c>
       <c r="L187">
         <v>1266.8900000000001</v>
       </c>
       <c r="M187">
-        <v>18968.453000000001</v>
+        <v>18910.451000000001</v>
       </c>
       <c r="N187">
-        <v>3870.6570000000002</v>
+        <v>3870.7959999999998</v>
       </c>
       <c r="O187">
         <v>1718.69</v>
@@ -14518,7 +14512,7 @@
         <v>4.3983636739999996</v>
       </c>
       <c r="T187">
-        <v>4976.87</v>
+        <v>5079.05</v>
       </c>
       <c r="U187">
         <v>1536.73</v>
@@ -14531,6 +14525,820 @@
       </c>
       <c r="X187">
         <v>367.56</v>
+      </c>
+    </row>
+    <row r="188" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A188" s="1">
+        <v>44957</v>
+      </c>
+      <c r="B188">
+        <v>145.46</v>
+      </c>
+      <c r="C188">
+        <v>4161.7</v>
+      </c>
+      <c r="D188">
+        <v>178.0941</v>
+      </c>
+      <c r="E188">
+        <v>4076.6</v>
+      </c>
+      <c r="F188">
+        <v>648.37</v>
+      </c>
+      <c r="G188">
+        <v>1931.9449999999999</v>
+      </c>
+      <c r="H188">
+        <v>2100.44</v>
+      </c>
+      <c r="I188">
+        <v>1031.5</v>
+      </c>
+      <c r="J188">
+        <v>507.7645</v>
+      </c>
+      <c r="K188">
+        <v>1456.4829999999999</v>
+      </c>
+      <c r="L188">
+        <v>1267.28</v>
+      </c>
+      <c r="M188">
+        <v>18975.955000000002</v>
+      </c>
+      <c r="N188">
+        <v>3817.5610000000001</v>
+      </c>
+      <c r="O188">
+        <v>1718.69</v>
+      </c>
+      <c r="P188">
+        <v>407.11</v>
+      </c>
+      <c r="Q188">
+        <v>162.4709</v>
+      </c>
+      <c r="R188">
+        <v>4.5090300000000001</v>
+      </c>
+      <c r="S188">
+        <v>4.6489987660000001</v>
+      </c>
+      <c r="T188">
+        <v>5079.05</v>
+      </c>
+      <c r="U188">
+        <v>1648.91</v>
+      </c>
+      <c r="V188">
+        <v>2367.614</v>
+      </c>
+      <c r="W188">
+        <v>141.75</v>
+      </c>
+      <c r="X188">
+        <v>382.39</v>
+      </c>
+    </row>
+    <row r="189" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A189" s="1">
+        <v>44985</v>
+      </c>
+      <c r="B189">
+        <v>136.36000000000001</v>
+      </c>
+      <c r="C189">
+        <v>3934.93</v>
+      </c>
+      <c r="D189">
+        <v>168.9444</v>
+      </c>
+      <c r="E189">
+        <v>3970.15</v>
+      </c>
+      <c r="F189">
+        <v>629.02</v>
+      </c>
+      <c r="G189">
+        <v>1896.991</v>
+      </c>
+      <c r="H189">
+        <v>2053.69</v>
+      </c>
+      <c r="I189">
+        <v>964.01</v>
+      </c>
+      <c r="J189">
+        <v>510.96210000000002</v>
+      </c>
+      <c r="K189">
+        <v>1437.635</v>
+      </c>
+      <c r="L189">
+        <v>1273.56</v>
+      </c>
+      <c r="M189">
+        <v>18958.985000000001</v>
+      </c>
+      <c r="N189">
+        <v>3888.4479999999999</v>
+      </c>
+      <c r="O189">
+        <v>1718.69</v>
+      </c>
+      <c r="P189">
+        <v>382.53</v>
+      </c>
+      <c r="Q189">
+        <v>162.4709</v>
+      </c>
+      <c r="R189">
+        <v>4.67272</v>
+      </c>
+      <c r="S189">
+        <v>4.8077261</v>
+      </c>
+      <c r="T189">
+        <v>5079.05</v>
+      </c>
+      <c r="U189">
+        <v>1601.19</v>
+      </c>
+      <c r="V189">
+        <v>2308.3960000000002</v>
+      </c>
+      <c r="W189">
+        <v>134.5625</v>
+      </c>
+      <c r="X189">
+        <v>366.54</v>
+      </c>
+    </row>
+    <row r="190" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A190" s="1">
+        <v>45016</v>
+      </c>
+      <c r="B190">
+        <v>143.85</v>
+      </c>
+      <c r="C190">
+        <v>4104.91</v>
+      </c>
+      <c r="D190">
+        <v>176.52780000000001</v>
+      </c>
+      <c r="E190">
+        <v>4109.3100000000004</v>
+      </c>
+      <c r="F190">
+        <v>646.76</v>
+      </c>
+      <c r="G190">
+        <v>1802.4839999999999</v>
+      </c>
+      <c r="H190">
+        <v>2092.6</v>
+      </c>
+      <c r="I190">
+        <v>990.28</v>
+      </c>
+      <c r="J190">
+        <v>510.464</v>
+      </c>
+      <c r="K190">
+        <v>1453.818</v>
+      </c>
+      <c r="L190">
+        <v>1235.1600000000001</v>
+      </c>
+      <c r="M190">
+        <v>18448.667000000001</v>
+      </c>
+      <c r="N190">
+        <v>3588.0039999999999</v>
+      </c>
+      <c r="O190">
+        <v>1718.69</v>
+      </c>
+      <c r="P190">
+        <v>373.22</v>
+      </c>
+      <c r="Q190">
+        <v>162.4709</v>
+      </c>
+      <c r="R190">
+        <v>4.6408199999999997</v>
+      </c>
+      <c r="S190">
+        <v>4.7309068339999998</v>
+      </c>
+      <c r="T190">
+        <v>5215.8100000000004</v>
+      </c>
+      <c r="U190">
+        <v>1636.36</v>
+      </c>
+      <c r="V190">
+        <v>2366.27</v>
+      </c>
+      <c r="W190">
+        <v>141.125</v>
+      </c>
+      <c r="X190">
+        <v>385.5</v>
+      </c>
+    </row>
+    <row r="191" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A191" s="1">
+        <v>45044</v>
+      </c>
+      <c r="B191">
+        <v>144.24</v>
+      </c>
+      <c r="C191">
+        <v>4135.75</v>
+      </c>
+      <c r="D191">
+        <v>176.87960000000001</v>
+      </c>
+      <c r="E191">
+        <v>4169.4799999999996</v>
+      </c>
+      <c r="F191">
+        <v>655</v>
+      </c>
+      <c r="G191">
+        <v>1768.9870000000001</v>
+      </c>
+      <c r="H191">
+        <v>2143.85</v>
+      </c>
+      <c r="I191">
+        <v>977.05</v>
+      </c>
+      <c r="J191">
+        <v>515.30060000000003</v>
+      </c>
+      <c r="K191">
+        <v>1467.85</v>
+      </c>
+      <c r="L191">
+        <v>1252.01</v>
+      </c>
+      <c r="M191">
+        <v>18601.562999999998</v>
+      </c>
+      <c r="N191">
+        <v>3691.3</v>
+      </c>
+      <c r="O191">
+        <v>1718.69</v>
+      </c>
+      <c r="P191">
+        <v>373.66</v>
+      </c>
+      <c r="Q191">
+        <v>162.4709</v>
+      </c>
+      <c r="R191">
+        <v>4.9508999999999999</v>
+      </c>
+      <c r="S191">
+        <v>5.1306892120000001</v>
+      </c>
+      <c r="T191">
+        <v>5215.8100000000004</v>
+      </c>
+      <c r="U191">
+        <v>1654.5</v>
+      </c>
+      <c r="V191">
+        <v>2389.3040000000001</v>
+      </c>
+      <c r="W191">
+        <v>141.40625</v>
+      </c>
+      <c r="X191">
+        <v>388.47</v>
+      </c>
+    </row>
+    <row r="192" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A192" s="1">
+        <v>45077</v>
+      </c>
+      <c r="B192">
+        <v>138.65</v>
+      </c>
+      <c r="C192">
+        <v>4020.88</v>
+      </c>
+      <c r="D192">
+        <v>170.57380000000001</v>
+      </c>
+      <c r="E192">
+        <v>4179.83</v>
+      </c>
+      <c r="F192">
+        <v>646.37</v>
+      </c>
+      <c r="G192">
+        <v>1749.65</v>
+      </c>
+      <c r="H192">
+        <v>2041.81</v>
+      </c>
+      <c r="I192">
+        <v>958.53</v>
+      </c>
+      <c r="J192">
+        <v>514.86080000000004</v>
+      </c>
+      <c r="K192">
+        <v>1453.913</v>
+      </c>
+      <c r="L192">
+        <v>1263.18</v>
+      </c>
+      <c r="M192">
+        <v>18548.652999999998</v>
+      </c>
+      <c r="N192">
+        <v>3798.7719999999999</v>
+      </c>
+      <c r="O192">
+        <v>1718.69</v>
+      </c>
+      <c r="P192">
+        <v>357.38</v>
+      </c>
+      <c r="Q192">
+        <v>162.4709</v>
+      </c>
+      <c r="R192">
+        <v>5.1535799999999998</v>
+      </c>
+      <c r="S192">
+        <v>5.3719694689999997</v>
+      </c>
+      <c r="T192">
+        <v>5215.8100000000004</v>
+      </c>
+      <c r="U192">
+        <v>1630.51</v>
+      </c>
+      <c r="V192">
+        <v>2394.2890000000002</v>
+      </c>
+      <c r="W192">
+        <v>136.375</v>
+      </c>
+      <c r="X192">
+        <v>379.55</v>
+      </c>
+    </row>
+    <row r="193" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A193" s="1">
+        <v>45107</v>
+      </c>
+      <c r="B193">
+        <v>139.72999999999999</v>
+      </c>
+      <c r="C193">
+        <v>4082.76</v>
+      </c>
+      <c r="D193">
+        <v>169.756</v>
+      </c>
+      <c r="E193">
+        <v>4450.38</v>
+      </c>
+      <c r="F193">
+        <v>682.84</v>
+      </c>
+      <c r="G193">
+        <v>1888.7339999999999</v>
+      </c>
+      <c r="H193">
+        <v>2131.7199999999998</v>
+      </c>
+      <c r="I193">
+        <v>989.48</v>
+      </c>
+      <c r="J193">
+        <v>526.38220000000001</v>
+      </c>
+      <c r="K193">
+        <v>1477.579</v>
+      </c>
+      <c r="L193">
+        <v>1270.1099999999999</v>
+      </c>
+      <c r="M193">
+        <v>18754.213</v>
+      </c>
+      <c r="N193">
+        <v>3876.107</v>
+      </c>
+      <c r="O193">
+        <v>1718.69</v>
+      </c>
+      <c r="P193">
+        <v>373.51</v>
+      </c>
+      <c r="Q193">
+        <v>162.4709</v>
+      </c>
+      <c r="R193">
+        <v>5.2157900000000001</v>
+      </c>
+      <c r="S193">
+        <v>5.2487262379999997</v>
+      </c>
+      <c r="T193">
+        <v>5362.12</v>
+      </c>
+      <c r="U193">
+        <v>1722.87</v>
+      </c>
+      <c r="V193">
+        <v>2554.4879999999998</v>
+      </c>
+      <c r="W193">
+        <v>136.21875</v>
+      </c>
+      <c r="X193">
+        <v>376.94</v>
+      </c>
+    </row>
+    <row r="194" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A194" s="1">
+        <v>45138</v>
+      </c>
+      <c r="B194">
+        <v>134.74</v>
+      </c>
+      <c r="C194">
+        <v>4077.42</v>
+      </c>
+      <c r="D194">
+        <v>164.77119999999999</v>
+      </c>
+      <c r="E194">
+        <v>4588.96</v>
+      </c>
+      <c r="F194">
+        <v>707.11</v>
+      </c>
+      <c r="G194">
+        <v>2003.1769999999999</v>
+      </c>
+      <c r="H194">
+        <v>2199.36</v>
+      </c>
+      <c r="I194">
+        <v>1046.9100000000001</v>
+      </c>
+      <c r="J194">
+        <v>533.23329999999999</v>
+      </c>
+      <c r="K194">
+        <v>1498.62</v>
+      </c>
+      <c r="L194">
+        <v>1256.76</v>
+      </c>
+      <c r="M194">
+        <v>18878.060000000001</v>
+      </c>
+      <c r="N194">
+        <v>3815.27</v>
+      </c>
+      <c r="O194">
+        <v>1718.69</v>
+      </c>
+      <c r="P194">
+        <v>380.33</v>
+      </c>
+      <c r="Q194">
+        <v>162.4709</v>
+      </c>
+      <c r="R194">
+        <v>5.2787199999999999</v>
+      </c>
+      <c r="S194">
+        <v>5.3514236679999998</v>
+      </c>
+      <c r="T194">
+        <v>5362.12</v>
+      </c>
+      <c r="U194">
+        <v>1786.91</v>
+      </c>
+      <c r="V194">
+        <v>2643.6860000000001</v>
+      </c>
+      <c r="W194">
+        <v>132.21875</v>
+      </c>
+      <c r="X194">
+        <v>371.29</v>
+      </c>
+    </row>
+    <row r="195" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A195" s="1">
+        <v>45169</v>
+      </c>
+      <c r="B195">
+        <v>128.56</v>
+      </c>
+      <c r="C195">
+        <v>3997.94</v>
+      </c>
+      <c r="D195">
+        <v>159.50399999999999</v>
+      </c>
+      <c r="E195">
+        <v>4507.66</v>
+      </c>
+      <c r="F195">
+        <v>686.15</v>
+      </c>
+      <c r="G195">
+        <v>1899.6759999999999</v>
+      </c>
+      <c r="H195">
+        <v>2109.16</v>
+      </c>
+      <c r="I195">
+        <v>980.33</v>
+      </c>
+      <c r="J195">
+        <v>539.38930000000005</v>
+      </c>
+      <c r="K195">
+        <v>1502.896</v>
+      </c>
+      <c r="L195">
+        <v>1256.23</v>
+      </c>
+      <c r="M195">
+        <v>18774.57</v>
+      </c>
+      <c r="N195">
+        <v>3779.1060000000002</v>
+      </c>
+      <c r="O195">
+        <v>1718.69</v>
+      </c>
+      <c r="P195">
+        <v>366.99</v>
+      </c>
+      <c r="Q195">
+        <v>162.4709</v>
+      </c>
+      <c r="R195">
+        <v>5.3294600000000001</v>
+      </c>
+      <c r="S195">
+        <v>5.413067388</v>
+      </c>
+      <c r="T195">
+        <v>5362.12</v>
+      </c>
+      <c r="U195">
+        <v>1732.63</v>
+      </c>
+      <c r="V195">
+        <v>2588.1060000000002</v>
+      </c>
+      <c r="W195">
+        <v>127.96875</v>
+      </c>
+      <c r="X195">
+        <v>364.19</v>
+      </c>
+    </row>
+    <row r="196" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A196" s="1">
+        <v>45198</v>
+      </c>
+      <c r="B196">
+        <v>114.43</v>
+      </c>
+      <c r="C196">
+        <v>3787.56</v>
+      </c>
+      <c r="D196">
+        <v>146.2216</v>
+      </c>
+      <c r="E196">
+        <v>4288.05</v>
+      </c>
+      <c r="F196">
+        <v>656.82</v>
+      </c>
+      <c r="G196">
+        <v>1785.1020000000001</v>
+      </c>
+      <c r="H196">
+        <v>2031.26</v>
+      </c>
+      <c r="I196">
+        <v>952.78</v>
+      </c>
+      <c r="J196">
+        <v>544.12260000000003</v>
+      </c>
+      <c r="K196">
+        <v>1485.4169999999999</v>
+      </c>
+      <c r="L196">
+        <v>1264.0029999999999</v>
+      </c>
+      <c r="M196">
+        <v>19002.797999999999</v>
+      </c>
+      <c r="N196">
+        <v>3907.5459999999998</v>
+      </c>
+      <c r="O196">
+        <v>1718.69</v>
+      </c>
+      <c r="P196">
+        <v>360.28</v>
+      </c>
+      <c r="Q196">
+        <v>162.4709</v>
+      </c>
+      <c r="R196">
+        <v>5.3626800000000001</v>
+      </c>
+      <c r="S196">
+        <v>5.4027921179999998</v>
+      </c>
+      <c r="T196">
+        <v>5362.12</v>
+      </c>
+      <c r="U196">
+        <v>1657.17</v>
+      </c>
+      <c r="V196">
+        <v>2462.06</v>
+      </c>
+      <c r="W196">
+        <v>118.6875</v>
+      </c>
+      <c r="X196">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="197" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A197" s="1">
+        <v>45230</v>
+      </c>
+      <c r="B197">
+        <v>105.26</v>
+      </c>
+      <c r="C197">
+        <v>3628.5</v>
+      </c>
+      <c r="D197">
+        <v>138.67570000000001</v>
+      </c>
+      <c r="E197">
+        <v>4193.8</v>
+      </c>
+      <c r="F197">
+        <v>636.65</v>
+      </c>
+      <c r="G197">
+        <v>1662.2819999999999</v>
+      </c>
+      <c r="H197">
+        <v>1947.91</v>
+      </c>
+      <c r="I197">
+        <v>915.2</v>
+      </c>
+      <c r="J197">
+        <v>544.2876</v>
+      </c>
+      <c r="K197">
+        <v>1467.0319999999999</v>
+      </c>
+      <c r="L197">
+        <v>1267.6389999999999</v>
+      </c>
+      <c r="M197">
+        <v>18864.809000000001</v>
+      </c>
+      <c r="N197">
+        <v>3912.1610000000001</v>
+      </c>
+      <c r="O197">
+        <v>1718.69</v>
+      </c>
+      <c r="P197">
+        <v>360.28</v>
+      </c>
+      <c r="Q197">
+        <v>162.4709</v>
+      </c>
+      <c r="R197">
+        <v>5.3648400000000001</v>
+      </c>
+      <c r="S197">
+        <v>5.3976546809999997</v>
+      </c>
+      <c r="T197">
+        <v>5362.12</v>
+      </c>
+      <c r="U197">
+        <v>1600.93</v>
+      </c>
+      <c r="V197">
+        <v>2394.585</v>
+      </c>
+      <c r="W197">
+        <v>112.5625</v>
+      </c>
+      <c r="X197">
+        <v>330.52</v>
+      </c>
+    </row>
+    <row r="198" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A198" s="1">
+        <v>45260</v>
+      </c>
+      <c r="B198">
+        <v>120.27</v>
+      </c>
+      <c r="C198">
+        <v>4022.31</v>
+      </c>
+      <c r="D198">
+        <v>150.5694</v>
+      </c>
+      <c r="E198">
+        <v>4567.8</v>
+      </c>
+      <c r="F198">
+        <v>694.38</v>
+      </c>
+      <c r="G198">
+        <v>1809.02</v>
+      </c>
+      <c r="H198">
+        <v>2124.91</v>
+      </c>
+      <c r="I198">
+        <v>987.1</v>
+      </c>
+      <c r="J198">
+        <v>550.78459999999995</v>
+      </c>
+      <c r="K198">
+        <v>1533.7560000000001</v>
+      </c>
+      <c r="L198">
+        <v>1245.559</v>
+      </c>
+      <c r="M198">
+        <v>18864.809000000001</v>
+      </c>
+      <c r="N198">
+        <v>3721.7759999999998</v>
+      </c>
+      <c r="O198">
+        <v>1718.69</v>
+      </c>
+      <c r="P198">
+        <v>360.28</v>
+      </c>
+      <c r="Q198">
+        <v>162.4709</v>
+      </c>
+      <c r="R198">
+        <v>5.2951499999999996</v>
+      </c>
+      <c r="S198">
+        <v>5.3514236679999998</v>
+      </c>
+      <c r="T198">
+        <v>5362.12</v>
+      </c>
+      <c r="U198">
+        <v>1746.35</v>
+      </c>
+      <c r="V198">
+        <v>2612.866</v>
+      </c>
+      <c r="W198">
+        <v>122.3125</v>
+      </c>
+      <c r="X198">
+        <v>353.03</v>
       </c>
     </row>
   </sheetData>
@@ -14540,15 +15348,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X182"/>
+  <dimension ref="A1:X193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A153" workbookViewId="0">
-      <selection activeCell="A182" sqref="A182"/>
+    <sheetView tabSelected="1" topLeftCell="A147" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G166" sqref="G166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
@@ -26880,7 +27688,7 @@
         <v>496.8091</v>
       </c>
       <c r="K167">
-        <v>1568.47</v>
+        <v>1568.471</v>
       </c>
       <c r="L167">
         <v>1231.8599999999999</v>
@@ -26954,7 +27762,7 @@
         <v>497.9812</v>
       </c>
       <c r="K168">
-        <v>1565.68</v>
+        <v>1565.681</v>
       </c>
       <c r="L168">
         <v>1244.81</v>
@@ -27028,7 +27836,7 @@
         <v>497.22050000000002</v>
       </c>
       <c r="K169">
-        <v>1549.64</v>
+        <v>1549.636</v>
       </c>
       <c r="L169">
         <v>1210.92</v>
@@ -27185,7 +27993,7 @@
         <v>17491.125</v>
       </c>
       <c r="N171">
-        <v>3145.723</v>
+        <v>3145.6610000000001</v>
       </c>
       <c r="O171">
         <v>1759.42</v>
@@ -27250,7 +28058,7 @@
         <v>499.65269999999998</v>
       </c>
       <c r="K172">
-        <v>1521.6</v>
+        <v>1521.604</v>
       </c>
       <c r="L172">
         <v>1194.8599999999999</v>
@@ -27259,7 +28067,7 @@
         <v>17708.370999999999</v>
       </c>
       <c r="N172">
-        <v>3261.558</v>
+        <v>3261.4670000000001</v>
       </c>
       <c r="O172">
         <v>1779.61</v>
@@ -27324,7 +28132,7 @@
         <v>499.84949999999998</v>
       </c>
       <c r="K173">
-        <v>1507.53</v>
+        <v>1507.5250000000001</v>
       </c>
       <c r="L173">
         <v>1231.8699999999999</v>
@@ -27333,7 +28141,7 @@
         <v>18513.787</v>
       </c>
       <c r="N173">
-        <v>3576.8649999999998</v>
+        <v>3576.799</v>
       </c>
       <c r="O173">
         <v>1708.65</v>
@@ -27351,7 +28159,7 @@
         <v>0.60592664699999998</v>
       </c>
       <c r="T173">
-        <v>4778.1000000000004</v>
+        <v>4862.16</v>
       </c>
       <c r="U173">
         <v>1805.11</v>
@@ -27398,7 +28206,7 @@
         <v>500.70659999999998</v>
       </c>
       <c r="K174">
-        <v>1452.69</v>
+        <v>1452.6869999999999</v>
       </c>
       <c r="L174">
         <v>1255.32</v>
@@ -27407,7 +28215,7 @@
         <v>19027.263999999999</v>
       </c>
       <c r="N174">
-        <v>3829.3380000000002</v>
+        <v>3829.2640000000001</v>
       </c>
       <c r="O174">
         <v>1718.69</v>
@@ -27472,7 +28280,7 @@
         <v>488.13490000000002</v>
       </c>
       <c r="K175">
-        <v>1456.32</v>
+        <v>1456.3240000000001</v>
       </c>
       <c r="L175">
         <v>1243.99</v>
@@ -27481,7 +28289,7 @@
         <v>18991.223000000002</v>
       </c>
       <c r="N175">
-        <v>3821.6329999999998</v>
+        <v>3821.616</v>
       </c>
       <c r="O175">
         <v>1718.69</v>
@@ -27546,16 +28354,16 @@
         <v>478.0942</v>
       </c>
       <c r="K176">
-        <v>1357.2</v>
+        <v>1357.1969999999999</v>
       </c>
       <c r="L176">
         <v>1261.07</v>
       </c>
       <c r="M176">
-        <v>18910.812000000002</v>
+        <v>18830.867999999999</v>
       </c>
       <c r="N176">
-        <v>3919.7820000000002</v>
+        <v>3919.8330000000001</v>
       </c>
       <c r="O176">
         <v>1718.69</v>
@@ -27573,7 +28381,7 @@
         <v>1.7577757199999999</v>
       </c>
       <c r="T176">
-        <v>4862.16</v>
+        <v>4887.8999999999996</v>
       </c>
       <c r="U176">
         <v>1510.77</v>
@@ -27626,10 +28434,10 @@
         <v>1242.3499999999999</v>
       </c>
       <c r="M177">
-        <v>18830.867999999999</v>
+        <v>18679.645</v>
       </c>
       <c r="N177">
-        <v>3747.0189999999998</v>
+        <v>3747.049</v>
       </c>
       <c r="O177">
         <v>1718.69</v>
@@ -27647,7 +28455,7 @@
         <v>2.5361553099999998</v>
       </c>
       <c r="T177">
-        <v>4862.16</v>
+        <v>4887.8999999999996</v>
       </c>
       <c r="U177">
         <v>1616.84</v>
@@ -27694,16 +28502,16 @@
         <v>494.48860000000002</v>
       </c>
       <c r="K178">
-        <v>1404.48</v>
+        <v>1404.481</v>
       </c>
       <c r="L178">
         <v>1257.82</v>
       </c>
       <c r="M178">
-        <v>18679.645</v>
+        <v>18922.542000000001</v>
       </c>
       <c r="N178">
-        <v>3896.5830000000001</v>
+        <v>3896.4749999999999</v>
       </c>
       <c r="O178">
         <v>1718.69</v>
@@ -27768,16 +28576,16 @@
         <v>483.77879999999999</v>
       </c>
       <c r="K179">
-        <v>1348</v>
+        <v>1347.9949999999999</v>
       </c>
       <c r="L179">
         <v>1295.3699999999999</v>
       </c>
       <c r="M179">
-        <v>19245.985000000001</v>
+        <v>19166.885999999999</v>
       </c>
       <c r="N179">
-        <v>4120.9750000000004</v>
+        <v>4121.0169999999998</v>
       </c>
       <c r="O179">
         <v>1718.69</v>
@@ -27795,7 +28603,7 @@
         <v>3.2972545599999998</v>
       </c>
       <c r="T179">
-        <v>4887.8999999999996</v>
+        <v>4976.87</v>
       </c>
       <c r="U179">
         <v>1403.68</v>
@@ -27842,16 +28650,16 @@
         <v>487.8895</v>
       </c>
       <c r="K180">
-        <v>1386.37</v>
+        <v>1386.3679999999999</v>
       </c>
       <c r="L180">
         <v>1297.27</v>
       </c>
       <c r="M180">
-        <v>19349.467000000001</v>
+        <v>19286.981</v>
       </c>
       <c r="N180">
-        <v>4128.7719999999999</v>
+        <v>4128.8620000000001</v>
       </c>
       <c r="O180">
         <v>1718.69</v>
@@ -27869,7 +28677,7 @@
         <v>4.11230765</v>
       </c>
       <c r="T180">
-        <v>4887.8999999999996</v>
+        <v>4976.87</v>
       </c>
       <c r="U180">
         <v>1489.05</v>
@@ -27922,10 +28730,10 @@
         <v>1266.26</v>
       </c>
       <c r="M181">
-        <v>18959.576000000001</v>
+        <v>18880.728999999999</v>
       </c>
       <c r="N181">
-        <v>3879.6979999999999</v>
+        <v>3879.7849999999999</v>
       </c>
       <c r="O181">
         <v>1718.69</v>
@@ -27990,16 +28798,16 @@
         <v>495.06270000000001</v>
       </c>
       <c r="K182">
-        <v>1401.68</v>
+        <v>1401.683</v>
       </c>
       <c r="L182">
         <v>1266.8900000000001</v>
       </c>
       <c r="M182">
-        <v>18968.453000000001</v>
+        <v>18910.451000000001</v>
       </c>
       <c r="N182">
-        <v>3870.6570000000002</v>
+        <v>3870.7959999999998</v>
       </c>
       <c r="O182">
         <v>1718.69</v>
@@ -28017,7 +28825,7 @@
         <v>4.3983636739999996</v>
       </c>
       <c r="T182">
-        <v>4976.87</v>
+        <v>5079.05</v>
       </c>
       <c r="U182">
         <v>1536.73</v>
@@ -28030,6 +28838,820 @@
       </c>
       <c r="X182">
         <v>367.56</v>
+      </c>
+    </row>
+    <row r="183" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A183" s="1">
+        <v>44957</v>
+      </c>
+      <c r="B183">
+        <v>145.46</v>
+      </c>
+      <c r="C183">
+        <v>4161.7</v>
+      </c>
+      <c r="D183">
+        <v>178.0941</v>
+      </c>
+      <c r="E183">
+        <v>4076.6</v>
+      </c>
+      <c r="F183">
+        <v>648.37</v>
+      </c>
+      <c r="G183">
+        <v>1931.9449999999999</v>
+      </c>
+      <c r="H183">
+        <v>2100.44</v>
+      </c>
+      <c r="I183">
+        <v>1031.5</v>
+      </c>
+      <c r="J183">
+        <v>507.7645</v>
+      </c>
+      <c r="K183">
+        <v>1456.4829999999999</v>
+      </c>
+      <c r="L183">
+        <v>1267.28</v>
+      </c>
+      <c r="M183">
+        <v>18975.955000000002</v>
+      </c>
+      <c r="N183">
+        <v>3817.5610000000001</v>
+      </c>
+      <c r="O183">
+        <v>1718.69</v>
+      </c>
+      <c r="P183">
+        <v>407.11</v>
+      </c>
+      <c r="Q183">
+        <v>162.4709</v>
+      </c>
+      <c r="R183">
+        <v>4.5090300000000001</v>
+      </c>
+      <c r="S183">
+        <v>4.6489987660000001</v>
+      </c>
+      <c r="T183">
+        <v>5079.05</v>
+      </c>
+      <c r="U183">
+        <v>1648.91</v>
+      </c>
+      <c r="V183">
+        <v>2367.614</v>
+      </c>
+      <c r="W183">
+        <v>141.75</v>
+      </c>
+      <c r="X183">
+        <v>382.39</v>
+      </c>
+    </row>
+    <row r="184" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A184" s="1">
+        <v>44985</v>
+      </c>
+      <c r="B184">
+        <v>136.36000000000001</v>
+      </c>
+      <c r="C184">
+        <v>3934.93</v>
+      </c>
+      <c r="D184">
+        <v>168.9444</v>
+      </c>
+      <c r="E184">
+        <v>3970.15</v>
+      </c>
+      <c r="F184">
+        <v>629.02</v>
+      </c>
+      <c r="G184">
+        <v>1896.991</v>
+      </c>
+      <c r="H184">
+        <v>2053.69</v>
+      </c>
+      <c r="I184">
+        <v>964.01</v>
+      </c>
+      <c r="J184">
+        <v>510.96210000000002</v>
+      </c>
+      <c r="K184">
+        <v>1437.635</v>
+      </c>
+      <c r="L184">
+        <v>1273.56</v>
+      </c>
+      <c r="M184">
+        <v>18958.985000000001</v>
+      </c>
+      <c r="N184">
+        <v>3888.4479999999999</v>
+      </c>
+      <c r="O184">
+        <v>1718.69</v>
+      </c>
+      <c r="P184">
+        <v>382.53</v>
+      </c>
+      <c r="Q184">
+        <v>162.4709</v>
+      </c>
+      <c r="R184">
+        <v>4.67272</v>
+      </c>
+      <c r="S184">
+        <v>4.8077261</v>
+      </c>
+      <c r="T184">
+        <v>5079.05</v>
+      </c>
+      <c r="U184">
+        <v>1601.19</v>
+      </c>
+      <c r="V184">
+        <v>2308.3960000000002</v>
+      </c>
+      <c r="W184">
+        <v>134.5625</v>
+      </c>
+      <c r="X184">
+        <v>366.54</v>
+      </c>
+    </row>
+    <row r="185" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A185" s="1">
+        <v>45016</v>
+      </c>
+      <c r="B185">
+        <v>143.85</v>
+      </c>
+      <c r="C185">
+        <v>4104.91</v>
+      </c>
+      <c r="D185">
+        <v>176.52780000000001</v>
+      </c>
+      <c r="E185">
+        <v>4109.3100000000004</v>
+      </c>
+      <c r="F185">
+        <v>646.76</v>
+      </c>
+      <c r="G185">
+        <v>1802.4839999999999</v>
+      </c>
+      <c r="H185">
+        <v>2092.6</v>
+      </c>
+      <c r="I185">
+        <v>990.28</v>
+      </c>
+      <c r="J185">
+        <v>510.464</v>
+      </c>
+      <c r="K185">
+        <v>1453.818</v>
+      </c>
+      <c r="L185">
+        <v>1235.1600000000001</v>
+      </c>
+      <c r="M185">
+        <v>18448.667000000001</v>
+      </c>
+      <c r="N185">
+        <v>3588.0039999999999</v>
+      </c>
+      <c r="O185">
+        <v>1718.69</v>
+      </c>
+      <c r="P185">
+        <v>373.22</v>
+      </c>
+      <c r="Q185">
+        <v>162.4709</v>
+      </c>
+      <c r="R185">
+        <v>4.6408199999999997</v>
+      </c>
+      <c r="S185">
+        <v>4.7309068339999998</v>
+      </c>
+      <c r="T185">
+        <v>5215.8100000000004</v>
+      </c>
+      <c r="U185">
+        <v>1636.36</v>
+      </c>
+      <c r="V185">
+        <v>2366.27</v>
+      </c>
+      <c r="W185">
+        <v>141.125</v>
+      </c>
+      <c r="X185">
+        <v>385.5</v>
+      </c>
+    </row>
+    <row r="186" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A186" s="1">
+        <v>45044</v>
+      </c>
+      <c r="B186">
+        <v>144.24</v>
+      </c>
+      <c r="C186">
+        <v>4135.75</v>
+      </c>
+      <c r="D186">
+        <v>176.87960000000001</v>
+      </c>
+      <c r="E186">
+        <v>4169.4799999999996</v>
+      </c>
+      <c r="F186">
+        <v>655</v>
+      </c>
+      <c r="G186">
+        <v>1768.9870000000001</v>
+      </c>
+      <c r="H186">
+        <v>2143.85</v>
+      </c>
+      <c r="I186">
+        <v>977.05</v>
+      </c>
+      <c r="J186">
+        <v>515.30060000000003</v>
+      </c>
+      <c r="K186">
+        <v>1467.85</v>
+      </c>
+      <c r="L186">
+        <v>1252.01</v>
+      </c>
+      <c r="M186">
+        <v>18601.562999999998</v>
+      </c>
+      <c r="N186">
+        <v>3691.3</v>
+      </c>
+      <c r="O186">
+        <v>1718.69</v>
+      </c>
+      <c r="P186">
+        <v>373.66</v>
+      </c>
+      <c r="Q186">
+        <v>162.4709</v>
+      </c>
+      <c r="R186">
+        <v>4.9508999999999999</v>
+      </c>
+      <c r="S186">
+        <v>5.1306892120000001</v>
+      </c>
+      <c r="T186">
+        <v>5215.8100000000004</v>
+      </c>
+      <c r="U186">
+        <v>1654.5</v>
+      </c>
+      <c r="V186">
+        <v>2389.3040000000001</v>
+      </c>
+      <c r="W186">
+        <v>141.40625</v>
+      </c>
+      <c r="X186">
+        <v>388.47</v>
+      </c>
+    </row>
+    <row r="187" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A187" s="1">
+        <v>45077</v>
+      </c>
+      <c r="B187">
+        <v>138.65</v>
+      </c>
+      <c r="C187">
+        <v>4020.88</v>
+      </c>
+      <c r="D187">
+        <v>170.57380000000001</v>
+      </c>
+      <c r="E187">
+        <v>4179.83</v>
+      </c>
+      <c r="F187">
+        <v>646.37</v>
+      </c>
+      <c r="G187">
+        <v>1749.65</v>
+      </c>
+      <c r="H187">
+        <v>2041.81</v>
+      </c>
+      <c r="I187">
+        <v>958.53</v>
+      </c>
+      <c r="J187">
+        <v>514.86080000000004</v>
+      </c>
+      <c r="K187">
+        <v>1453.913</v>
+      </c>
+      <c r="L187">
+        <v>1263.18</v>
+      </c>
+      <c r="M187">
+        <v>18548.652999999998</v>
+      </c>
+      <c r="N187">
+        <v>3798.7719999999999</v>
+      </c>
+      <c r="O187">
+        <v>1718.69</v>
+      </c>
+      <c r="P187">
+        <v>357.38</v>
+      </c>
+      <c r="Q187">
+        <v>162.4709</v>
+      </c>
+      <c r="R187">
+        <v>5.1535799999999998</v>
+      </c>
+      <c r="S187">
+        <v>5.3719694689999997</v>
+      </c>
+      <c r="T187">
+        <v>5215.8100000000004</v>
+      </c>
+      <c r="U187">
+        <v>1630.51</v>
+      </c>
+      <c r="V187">
+        <v>2394.2890000000002</v>
+      </c>
+      <c r="W187">
+        <v>136.375</v>
+      </c>
+      <c r="X187">
+        <v>379.55</v>
+      </c>
+    </row>
+    <row r="188" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A188" s="1">
+        <v>45107</v>
+      </c>
+      <c r="B188">
+        <v>139.72999999999999</v>
+      </c>
+      <c r="C188">
+        <v>4082.76</v>
+      </c>
+      <c r="D188">
+        <v>169.756</v>
+      </c>
+      <c r="E188">
+        <v>4450.38</v>
+      </c>
+      <c r="F188">
+        <v>682.84</v>
+      </c>
+      <c r="G188">
+        <v>1888.7339999999999</v>
+      </c>
+      <c r="H188">
+        <v>2131.7199999999998</v>
+      </c>
+      <c r="I188">
+        <v>989.48</v>
+      </c>
+      <c r="J188">
+        <v>526.38220000000001</v>
+      </c>
+      <c r="K188">
+        <v>1477.579</v>
+      </c>
+      <c r="L188">
+        <v>1270.1099999999999</v>
+      </c>
+      <c r="M188">
+        <v>18754.213</v>
+      </c>
+      <c r="N188">
+        <v>3876.107</v>
+      </c>
+      <c r="O188">
+        <v>1718.69</v>
+      </c>
+      <c r="P188">
+        <v>373.51</v>
+      </c>
+      <c r="Q188">
+        <v>162.4709</v>
+      </c>
+      <c r="R188">
+        <v>5.2157900000000001</v>
+      </c>
+      <c r="S188">
+        <v>5.2487262379999997</v>
+      </c>
+      <c r="T188">
+        <v>5362.12</v>
+      </c>
+      <c r="U188">
+        <v>1722.87</v>
+      </c>
+      <c r="V188">
+        <v>2554.4879999999998</v>
+      </c>
+      <c r="W188">
+        <v>136.21875</v>
+      </c>
+      <c r="X188">
+        <v>376.94</v>
+      </c>
+    </row>
+    <row r="189" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A189" s="1">
+        <v>45138</v>
+      </c>
+      <c r="B189">
+        <v>134.74</v>
+      </c>
+      <c r="C189">
+        <v>4077.42</v>
+      </c>
+      <c r="D189">
+        <v>164.77119999999999</v>
+      </c>
+      <c r="E189">
+        <v>4588.96</v>
+      </c>
+      <c r="F189">
+        <v>707.11</v>
+      </c>
+      <c r="G189">
+        <v>2003.1769999999999</v>
+      </c>
+      <c r="H189">
+        <v>2199.36</v>
+      </c>
+      <c r="I189">
+        <v>1046.9100000000001</v>
+      </c>
+      <c r="J189">
+        <v>533.23329999999999</v>
+      </c>
+      <c r="K189">
+        <v>1498.62</v>
+      </c>
+      <c r="L189">
+        <v>1256.76</v>
+      </c>
+      <c r="M189">
+        <v>18878.060000000001</v>
+      </c>
+      <c r="N189">
+        <v>3815.27</v>
+      </c>
+      <c r="O189">
+        <v>1718.69</v>
+      </c>
+      <c r="P189">
+        <v>380.33</v>
+      </c>
+      <c r="Q189">
+        <v>162.4709</v>
+      </c>
+      <c r="R189">
+        <v>5.2787199999999999</v>
+      </c>
+      <c r="S189">
+        <v>5.3514236679999998</v>
+      </c>
+      <c r="T189">
+        <v>5362.12</v>
+      </c>
+      <c r="U189">
+        <v>1786.91</v>
+      </c>
+      <c r="V189">
+        <v>2643.6860000000001</v>
+      </c>
+      <c r="W189">
+        <v>132.21875</v>
+      </c>
+      <c r="X189">
+        <v>371.29</v>
+      </c>
+    </row>
+    <row r="190" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A190" s="1">
+        <v>45169</v>
+      </c>
+      <c r="B190">
+        <v>128.56</v>
+      </c>
+      <c r="C190">
+        <v>3997.94</v>
+      </c>
+      <c r="D190">
+        <v>159.50399999999999</v>
+      </c>
+      <c r="E190">
+        <v>4507.66</v>
+      </c>
+      <c r="F190">
+        <v>686.15</v>
+      </c>
+      <c r="G190">
+        <v>1899.6759999999999</v>
+      </c>
+      <c r="H190">
+        <v>2109.16</v>
+      </c>
+      <c r="I190">
+        <v>980.33</v>
+      </c>
+      <c r="J190">
+        <v>539.38930000000005</v>
+      </c>
+      <c r="K190">
+        <v>1502.896</v>
+      </c>
+      <c r="L190">
+        <v>1256.23</v>
+      </c>
+      <c r="M190">
+        <v>18774.57</v>
+      </c>
+      <c r="N190">
+        <v>3779.1060000000002</v>
+      </c>
+      <c r="O190">
+        <v>1718.69</v>
+      </c>
+      <c r="P190">
+        <v>366.99</v>
+      </c>
+      <c r="Q190">
+        <v>162.4709</v>
+      </c>
+      <c r="R190">
+        <v>5.3294600000000001</v>
+      </c>
+      <c r="S190">
+        <v>5.413067388</v>
+      </c>
+      <c r="T190">
+        <v>5362.12</v>
+      </c>
+      <c r="U190">
+        <v>1732.63</v>
+      </c>
+      <c r="V190">
+        <v>2588.1060000000002</v>
+      </c>
+      <c r="W190">
+        <v>127.96875</v>
+      </c>
+      <c r="X190">
+        <v>364.19</v>
+      </c>
+    </row>
+    <row r="191" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A191" s="1">
+        <v>45198</v>
+      </c>
+      <c r="B191">
+        <v>114.43</v>
+      </c>
+      <c r="C191">
+        <v>3787.56</v>
+      </c>
+      <c r="D191">
+        <v>146.2216</v>
+      </c>
+      <c r="E191">
+        <v>4288.05</v>
+      </c>
+      <c r="F191">
+        <v>656.82</v>
+      </c>
+      <c r="G191">
+        <v>1785.1020000000001</v>
+      </c>
+      <c r="H191">
+        <v>2031.26</v>
+      </c>
+      <c r="I191">
+        <v>952.78</v>
+      </c>
+      <c r="J191">
+        <v>544.12260000000003</v>
+      </c>
+      <c r="K191">
+        <v>1485.4169999999999</v>
+      </c>
+      <c r="L191">
+        <v>1264.0029999999999</v>
+      </c>
+      <c r="M191">
+        <v>19002.797999999999</v>
+      </c>
+      <c r="N191">
+        <v>3907.5459999999998</v>
+      </c>
+      <c r="O191">
+        <v>1718.69</v>
+      </c>
+      <c r="P191">
+        <v>360.28</v>
+      </c>
+      <c r="Q191">
+        <v>162.4709</v>
+      </c>
+      <c r="R191">
+        <v>5.3626800000000001</v>
+      </c>
+      <c r="S191">
+        <v>5.4027921179999998</v>
+      </c>
+      <c r="T191">
+        <v>5362.12</v>
+      </c>
+      <c r="U191">
+        <v>1657.17</v>
+      </c>
+      <c r="V191">
+        <v>2462.06</v>
+      </c>
+      <c r="W191">
+        <v>118.6875</v>
+      </c>
+      <c r="X191">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="192" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A192" s="1">
+        <v>45230</v>
+      </c>
+      <c r="B192">
+        <v>105.26</v>
+      </c>
+      <c r="C192">
+        <v>3628.5</v>
+      </c>
+      <c r="D192">
+        <v>138.67570000000001</v>
+      </c>
+      <c r="E192">
+        <v>4193.8</v>
+      </c>
+      <c r="F192">
+        <v>636.65</v>
+      </c>
+      <c r="G192">
+        <v>1662.2819999999999</v>
+      </c>
+      <c r="H192">
+        <v>1947.91</v>
+      </c>
+      <c r="I192">
+        <v>915.2</v>
+      </c>
+      <c r="J192">
+        <v>544.2876</v>
+      </c>
+      <c r="K192">
+        <v>1467.0319999999999</v>
+      </c>
+      <c r="L192">
+        <v>1267.6389999999999</v>
+      </c>
+      <c r="M192">
+        <v>18864.809000000001</v>
+      </c>
+      <c r="N192">
+        <v>3912.1610000000001</v>
+      </c>
+      <c r="O192">
+        <v>1718.69</v>
+      </c>
+      <c r="P192">
+        <v>360.28</v>
+      </c>
+      <c r="Q192">
+        <v>162.4709</v>
+      </c>
+      <c r="R192">
+        <v>5.3648400000000001</v>
+      </c>
+      <c r="S192">
+        <v>5.3976546809999997</v>
+      </c>
+      <c r="T192">
+        <v>5362.12</v>
+      </c>
+      <c r="U192">
+        <v>1600.93</v>
+      </c>
+      <c r="V192">
+        <v>2394.585</v>
+      </c>
+      <c r="W192">
+        <v>112.5625</v>
+      </c>
+      <c r="X192">
+        <v>330.52</v>
+      </c>
+    </row>
+    <row r="193" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A193" s="1">
+        <v>45260</v>
+      </c>
+      <c r="B193">
+        <v>120.27</v>
+      </c>
+      <c r="C193">
+        <v>4022.31</v>
+      </c>
+      <c r="D193">
+        <v>150.5694</v>
+      </c>
+      <c r="E193">
+        <v>4567.8</v>
+      </c>
+      <c r="F193">
+        <v>694.38</v>
+      </c>
+      <c r="G193">
+        <v>1809.02</v>
+      </c>
+      <c r="H193">
+        <v>2124.91</v>
+      </c>
+      <c r="I193">
+        <v>987.1</v>
+      </c>
+      <c r="J193">
+        <v>550.78459999999995</v>
+      </c>
+      <c r="K193">
+        <v>1533.7560000000001</v>
+      </c>
+      <c r="L193">
+        <v>1245.559</v>
+      </c>
+      <c r="M193">
+        <v>18864.809000000001</v>
+      </c>
+      <c r="N193">
+        <v>3721.7759999999998</v>
+      </c>
+      <c r="O193">
+        <v>1718.69</v>
+      </c>
+      <c r="P193">
+        <v>360.28</v>
+      </c>
+      <c r="Q193">
+        <v>162.4709</v>
+      </c>
+      <c r="R193">
+        <v>5.2951499999999996</v>
+      </c>
+      <c r="S193">
+        <v>5.3514236679999998</v>
+      </c>
+      <c r="T193">
+        <v>5362.12</v>
+      </c>
+      <c r="U193">
+        <v>1746.35</v>
+      </c>
+      <c r="V193">
+        <v>2612.866</v>
+      </c>
+      <c r="W193">
+        <v>122.3125</v>
+      </c>
+      <c r="X193">
+        <v>353.03</v>
       </c>
     </row>
   </sheetData>
@@ -44116,7 +45738,7 @@
       </c>
       <c r="K167" s="6">
         <f>data!K167/data!K166-1</f>
-        <v>3.3483317335747387E-4</v>
+        <v>3.354709508305298E-4</v>
       </c>
       <c r="L167" s="6">
         <f>data!L167/data!L166-1</f>
@@ -44213,7 +45835,7 @@
       </c>
       <c r="K168" s="6">
         <f>data!K168/data!K167-1</f>
-        <v>-1.7788035474060049E-3</v>
+        <v>-1.7788024133056357E-3</v>
       </c>
       <c r="L168" s="6">
         <f>data!L168/data!L167-1</f>
@@ -44310,7 +45932,7 @@
       </c>
       <c r="K169" s="6">
         <f>data!K169/data!K168-1</f>
-        <v>-1.0244749885033988E-2</v>
+        <v>-1.024793684026315E-2</v>
       </c>
       <c r="L169" s="6">
         <f>data!L169/data!L168-1</f>
@@ -44407,7 +46029,7 @@
       </c>
       <c r="K170" s="6">
         <f>data!K170/data!K169-1</f>
-        <v>1.8810820577682463E-2</v>
+        <v>1.8813450384477459E-2</v>
       </c>
       <c r="L170" s="6">
         <f>data!L170/data!L169-1</f>
@@ -44516,7 +46138,7 @@
       </c>
       <c r="N171" s="6">
         <f>data!N171/data!N170-1</f>
-        <v>3.4986342636308843E-2</v>
+        <v>3.4965943779434516E-2</v>
       </c>
       <c r="O171" s="6">
         <f>data!O171/data!O170-1</f>
@@ -44601,7 +46223,7 @@
       </c>
       <c r="K172" s="6">
         <f>data!K172/data!K171-1</f>
-        <v>-8.9814314278457985E-3</v>
+        <v>-8.9788262265613206E-3</v>
       </c>
       <c r="L172" s="6">
         <f>data!L172/data!L171-1</f>
@@ -44613,7 +46235,7 @@
       </c>
       <c r="N172" s="6">
         <f>data!N172/data!N171-1</f>
-        <v>3.6823013342242694E-2</v>
+        <v>3.6814520064304412E-2</v>
       </c>
       <c r="O172" s="6">
         <f>data!O172/data!O171-1</f>
@@ -44698,7 +46320,7 @@
       </c>
       <c r="K173" s="6">
         <f>data!K173/data!K172-1</f>
-        <v>-9.2468454258675115E-3</v>
+        <v>-9.2527359286647126E-3</v>
       </c>
       <c r="L173" s="6">
         <f>data!L173/data!L172-1</f>
@@ -44710,7 +46332,7 @@
       </c>
       <c r="N173" s="6">
         <f>data!N173/data!N172-1</f>
-        <v>9.6673736907330721E-2</v>
+        <v>9.6684099517180488E-2</v>
       </c>
       <c r="O173" s="6">
         <f>data!O173/data!O172-1</f>
@@ -44734,7 +46356,7 @@
       </c>
       <c r="T173" s="6">
         <f>data!T173/data!T172-1</f>
-        <v>0</v>
+        <v>1.7592766999434906E-2</v>
       </c>
       <c r="U173" s="6">
         <f>data!U173/data!U172-1</f>
@@ -44795,7 +46417,7 @@
       </c>
       <c r="K174" s="6">
         <f>data!K174/data!K173-1</f>
-        <v>-3.6377385524666073E-2</v>
+        <v>-3.6376179499510886E-2</v>
       </c>
       <c r="L174" s="6">
         <f>data!L174/data!L173-1</f>
@@ -44807,7 +46429,7 @@
       </c>
       <c r="N174" s="6">
         <f>data!N174/data!N173-1</f>
-        <v>7.0584995519819893E-2</v>
+        <v>7.058406133528905E-2</v>
       </c>
       <c r="O174" s="6">
         <f>data!O174/data!O173-1</f>
@@ -44831,7 +46453,7 @@
       </c>
       <c r="T174" s="6">
         <f>data!T174/data!T173-1</f>
-        <v>1.7592766999434906E-2</v>
+        <v>0</v>
       </c>
       <c r="U174" s="6">
         <f>data!U174/data!U173-1</f>
@@ -44892,7 +46514,7 @@
       </c>
       <c r="K175" s="6">
         <f>data!K175/data!K174-1</f>
-        <v>2.4988125477560796E-3</v>
+        <v>2.50363636488804E-3</v>
       </c>
       <c r="L175" s="6">
         <f>data!L175/data!L174-1</f>
@@ -44904,7 +46526,7 @@
       </c>
       <c r="N175" s="6">
         <f>data!N175/data!N174-1</f>
-        <v>-2.0120971301045287E-3</v>
+        <v>-1.9972506465995021E-3</v>
       </c>
       <c r="O175" s="6">
         <f>data!O175/data!O174-1</f>
@@ -44981,7 +46603,7 @@
       </c>
       <c r="I176" s="6">
         <f>data!I176/data!I175-1</f>
-        <v>-7.1450444013473557E-2</v>
+        <v>-7.1450444013473668E-2</v>
       </c>
       <c r="J176" s="6">
         <f>data!J176/data!J175-1</f>
@@ -44989,7 +46611,7 @@
       </c>
       <c r="K176" s="6">
         <f>data!K176/data!K175-1</f>
-        <v>-6.806196440342771E-2</v>
+        <v>-6.8066584084310988E-2</v>
       </c>
       <c r="L176" s="6">
         <f>data!L176/data!L175-1</f>
@@ -44997,11 +46619,11 @@
       </c>
       <c r="M176" s="6">
         <f>data!M176/data!M175-1</f>
-        <v>-4.2341138324794025E-3</v>
+        <v>-8.4436373581628921E-3</v>
       </c>
       <c r="N176" s="6">
         <f>data!N176/data!N175-1</f>
-        <v>2.5682476574804713E-2</v>
+        <v>2.570038434002786E-2</v>
       </c>
       <c r="O176" s="6">
         <f>data!O176/data!O175-1</f>
@@ -45025,7 +46647,7 @@
       </c>
       <c r="T176" s="6">
         <f>data!T176/data!T175-1</f>
-        <v>0</v>
+        <v>5.2939434325485202E-3</v>
       </c>
       <c r="U176" s="6">
         <f>data!U176/data!U175-1</f>
@@ -45086,7 +46708,7 @@
       </c>
       <c r="K177" s="6">
         <f>data!K177/data!K176-1</f>
-        <v>6.022693781314481E-2</v>
+        <v>6.0229281379195587E-2</v>
       </c>
       <c r="L177" s="6">
         <f>data!L177/data!L176-1</f>
@@ -45094,11 +46716,11 @@
       </c>
       <c r="M177" s="6">
         <f>data!M177/data!M176-1</f>
-        <v>-4.2274229155259135E-3</v>
+        <v>-8.0305910486971888E-3</v>
       </c>
       <c r="N177" s="6">
         <f>data!N177/data!N176-1</f>
-        <v>-4.4074644967500798E-2</v>
+        <v>-4.4079428894037043E-2</v>
       </c>
       <c r="O177" s="6">
         <f>data!O177/data!O176-1</f>
@@ -45183,7 +46805,7 @@
       </c>
       <c r="K178" s="6">
         <f>data!K178/data!K177-1</f>
-        <v>-2.394818407994781E-2</v>
+        <v>-2.3947489123938515E-2</v>
       </c>
       <c r="L178" s="6">
         <f>data!L178/data!L177-1</f>
@@ -45191,11 +46813,11 @@
       </c>
       <c r="M178" s="6">
         <f>data!M178/data!M177-1</f>
-        <v>-8.0305910486971888E-3</v>
+        <v>1.3003298510223305E-2</v>
       </c>
       <c r="N178" s="6">
         <f>data!N178/data!N177-1</f>
-        <v>3.9915463465757695E-2</v>
+        <v>3.9878314908612156E-2</v>
       </c>
       <c r="O178" s="6">
         <f>data!O178/data!O177-1</f>
@@ -45219,7 +46841,7 @@
       </c>
       <c r="T178" s="6">
         <f>data!T178/data!T177-1</f>
-        <v>5.2939434325485202E-3</v>
+        <v>0</v>
       </c>
       <c r="U178" s="6">
         <f>data!U178/data!U177-1</f>
@@ -45280,7 +46902,7 @@
       </c>
       <c r="K179" s="6">
         <f>data!K179/data!K178-1</f>
-        <v>-4.0214171793119147E-2</v>
+        <v>-4.0218415201060065E-2</v>
       </c>
       <c r="L179" s="6">
         <f>data!L179/data!L178-1</f>
@@ -45288,11 +46910,11 @@
       </c>
       <c r="M179" s="6">
         <f>data!M179/data!M178-1</f>
-        <v>3.0318563334581494E-2</v>
+        <v>1.2912852829181087E-2</v>
       </c>
       <c r="N179" s="6">
         <f>data!N179/data!N178-1</f>
-        <v>5.7586865209851901E-2</v>
+        <v>5.762695769894588E-2</v>
       </c>
       <c r="O179" s="6">
         <f>data!O179/data!O178-1</f>
@@ -45316,7 +46938,7 @@
       </c>
       <c r="T179" s="6">
         <f>data!T179/data!T178-1</f>
-        <v>0</v>
+        <v>1.8202090877472932E-2</v>
       </c>
       <c r="U179" s="6">
         <f>data!U179/data!U178-1</f>

</xml_diff>